<commit_message>
Added formatting of data - testing phase
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7F7E15-CB01-47B8-B5AE-0304F38A30BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5B6EB-2B4F-4FD0-9F14-DF6E2D75CCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="83640" yWindow="19140" windowWidth="2820" windowHeight="1230" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="132">
   <si>
     <t>Variable group</t>
   </si>
@@ -333,9 +333,6 @@
     <t>drinker12,13</t>
   </si>
   <si>
-    <t>prevRetStat</t>
-  </si>
-  <si>
     <t>race</t>
   </si>
   <si>
@@ -381,9 +378,6 @@
     <t>Several doubles</t>
   </si>
   <si>
-    <t xml:space="preserve">1 factor </t>
-  </si>
-  <si>
     <t>factor</t>
   </si>
   <si>
@@ -409,13 +403,40 @@
   </si>
   <si>
     <t>Need to check how missings are filled - imputation from pervious period? Make bins - especially for movement between wealth bins. We need to use imputed wealth for missings in 2016</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>1.married, 2.married,spouse absent, 3.partnered, 4. seperated, 5.divorced, 6.seperated/divorced, 7.widowed, 8.never married</t>
+  </si>
+  <si>
+    <t>1.white/caucasian, 2.black/african american, 3.other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 factors </t>
+  </si>
+  <si>
+    <t>1.working now, 2.unemployed and looking for work, 3. temprorarily laid off,  4.disabled, 5. retired, 6. homemaker, 7.other, 8.on sick or leave, 98.DK, 99.RF</t>
+  </si>
+  <si>
+    <t>7.everyday&lt;1.more than once a week&lt;2.once a week,&lt;3.one to three times a month&lt;4.hardly ever or never&lt;8.DK&lt;9.RF</t>
+  </si>
+  <si>
+    <t>1.lt high-school, 2.ged, 3.high-school graduate, 4.some college, 5.college and above</t>
+  </si>
+  <si>
+    <t>prevRetStat, jobStat.A1-5</t>
+  </si>
+  <si>
+    <t>1.fully retired &lt; 3.partially retired &lt;5. not retired</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +461,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -511,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -524,6 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
-  <dimension ref="B2:L32"/>
+  <dimension ref="B2:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -851,14 +880,15 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.40625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1328125" customWidth="1"/>
+    <col min="9" max="9" width="30.40625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="2:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -869,37 +899,40 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>80</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="J3" s="1" t="s">
+    <row r="3" spans="2:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="K3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -910,17 +943,17 @@
       <c r="F4" t="s">
         <v>81</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
       <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
@@ -929,17 +962,17 @@
       <c r="F5" t="s">
         <v>82</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
       <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
         <v>15</v>
       </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -948,109 +981,109 @@
         <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
         <v>16</v>
       </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
       <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
         <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
         <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
         <v>50</v>
       </c>
-      <c r="K7" t="s">
-        <v>24</v>
-      </c>
       <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" t="s">
         <v>85</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
         <v>49</v>
       </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
       <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" t="s">
         <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" t="s">
         <v>86</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
         <v>18</v>
       </c>
-      <c r="K9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1061,225 +1094,237 @@
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F10" t="s">
         <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
         <v>38</v>
       </c>
-      <c r="K10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" t="s">
         <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" t="s">
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" t="s">
         <v>26</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>41</v>
       </c>
-      <c r="K11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" t="s">
         <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F12" t="s">
         <v>89</v>
       </c>
       <c r="G12" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>43</v>
       </c>
-      <c r="K12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" t="s">
         <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
         <v>90</v>
       </c>
       <c r="G13" t="s">
-        <v>112</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" t="s">
         <v>45</v>
       </c>
-      <c r="K13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" t="s">
         <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14" t="s">
         <v>91</v>
       </c>
       <c r="G14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" t="s">
         <v>26</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>47</v>
       </c>
-      <c r="K14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" t="s">
         <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="H15" t="s">
-        <v>23</v>
+      <c r="G15" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" t="s">
         <v>68</v>
       </c>
-      <c r="K15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="G16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" t="s">
         <v>26</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>33</v>
       </c>
-      <c r="K16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" t="s">
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="G17" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" t="s">
         <v>26</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>35</v>
       </c>
-      <c r="K17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" t="s">
         <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="G18" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" t="s">
         <v>26</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>37</v>
       </c>
-      <c r="K18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
         <v>55</v>
@@ -1288,131 +1333,142 @@
         <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" t="s">
-        <v>24</v>
+      <c r="G19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="I19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" t="s">
         <v>56</v>
       </c>
-      <c r="K19" t="s">
-        <v>24</v>
-      </c>
       <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" t="s">
         <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
+      <c r="G20" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
         <v>74</v>
       </c>
-      <c r="K20" t="s">
-        <v>24</v>
-      </c>
       <c r="L20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" t="s">
         <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
         <v>97</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="H21" s="11"/>
       <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" t="s">
         <v>64</v>
       </c>
-      <c r="K21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" t="s">
         <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
+      <c r="G22" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="10"/>
       <c r="I22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" t="s">
         <v>65</v>
       </c>
-      <c r="K22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" t="s">
         <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I23" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="J23" t="s">
         <v>69</v>
       </c>
-      <c r="K23" t="s">
-        <v>24</v>
-      </c>
       <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.75">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
@@ -1421,178 +1477,189 @@
         <v>58</v>
       </c>
       <c r="E24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H24" t="s">
-        <v>23</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="10"/>
       <c r="I24" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
         <v>57</v>
       </c>
-      <c r="K24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" t="s">
         <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" t="s">
-        <v>23</v>
+        <v>99</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>125</v>
       </c>
       <c r="I25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" t="s">
         <v>19</v>
       </c>
-      <c r="K25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" t="s">
         <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H26" t="s">
-        <v>23</v>
+        <v>100</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" t="s">
         <v>20</v>
       </c>
-      <c r="K26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" t="s">
         <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="H27" t="s">
-        <v>23</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="H27" s="11"/>
       <c r="I27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" t="s">
         <v>21</v>
       </c>
-      <c r="K27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" t="s">
         <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H28" t="s">
-        <v>23</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H28" s="11"/>
       <c r="I28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" t="s">
         <v>25</v>
       </c>
-      <c r="K28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" t="s">
         <v>54</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="H29" t="s">
-        <v>23</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="H29" s="11"/>
       <c r="I29" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" t="s">
         <v>53</v>
       </c>
-      <c r="K29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" t="s">
         <v>106</v>
       </c>
-      <c r="E30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" t="s">
-        <v>107</v>
-      </c>
       <c r="G30" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H30" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" t="s">
         <v>26</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>79</v>
       </c>
-      <c r="K30" t="s">
-        <v>24</v>
-      </c>
       <c r="L30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.75">
+        <v>24</v>
+      </c>
+      <c r="M30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B31" s="7" t="s">
         <v>10</v>
       </c>
@@ -1600,14 +1667,14 @@
       <c r="D31" t="s">
         <v>78</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>28</v>
       </c>
-      <c r="K31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.75">
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B32" s="8" t="s">
         <v>11</v>
       </c>
@@ -1615,7 +1682,7 @@
       <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made racial discrimination function complete
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC5B6EB-2B4F-4FD0-9F14-DF6E2D75CCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA631681-83B9-4400-AF1B-EBF882949524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="83640" yWindow="19140" windowWidth="2820" windowHeight="1230" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
   <dimension ref="B2:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Define variables af en bugfix in outliers outcomes - still to add some variables
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA631681-83B9-4400-AF1B-EBF882949524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04AD38B-5C59-4845-8417-1946FF7BC300}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="83640" yWindow="19140" windowWidth="2820" windowHeight="1230" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="82935" yWindow="8970" windowWidth="5760" windowHeight="1230" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable_sheet_thesis" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="137">
   <si>
     <t>Variable group</t>
   </si>
@@ -264,9 +264,6 @@
     <t>r12mstat, r13mstat</t>
   </si>
   <si>
-    <t>Martital status difference (r12 = 1.married, r13 = 7.widowed)</t>
-  </si>
-  <si>
     <t>Marital status difference (r12 = 1.married, r13 = 5.divorced)</t>
   </si>
   <si>
@@ -402,9 +399,6 @@
     <t>double (is in years)</t>
   </si>
   <si>
-    <t>Need to check how missings are filled - imputation from pervious period? Make bins - especially for movement between wealth bins. We need to use imputed wealth for missings in 2016</t>
-  </si>
-  <si>
     <t>Levels</t>
   </si>
   <si>
@@ -430,13 +424,48 @@
   </si>
   <si>
     <t>1.fully retired &lt; 3.partially retired &lt;5. not retired</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>workingNow</t>
+  </si>
+  <si>
+    <t>1 = working now, 0=  not working now</t>
+  </si>
+  <si>
+    <t>Working now or not, from job status</t>
+  </si>
+  <si>
+    <t>Martital status difference (r12 = 1.married, r13 = 7.widowed) Simplification of marital status not done because married already included for w13</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do we want to include a variable where there is a jump from wealth bin to wealth bin? If so -&gt; probably best to make bins 2x so it is about overall position wrt rest. ALSO: Do we want to base wealth buckets on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>our subset or full set</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +498,15 @@
     <font>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -539,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -553,6 +591,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
-  <dimension ref="B2:M32"/>
+  <dimension ref="A2:M33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -888,7 +927,7 @@
     <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -899,16 +938,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>22</v>
@@ -924,7 +963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="3" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="K3" s="1" t="s">
         <v>4</v>
       </c>
@@ -932,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -941,7 +980,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -953,14 +992,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -972,7 +1011,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -981,13 +1020,13 @@
         <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
@@ -1002,20 +1041,20 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
         <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" t="s">
         <v>24</v>
@@ -1030,20 +1069,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
         <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
@@ -1058,20 +1097,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" t="s">
         <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
@@ -1083,7 +1122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1094,13 +1133,13 @@
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I10" t="s">
         <v>23</v>
@@ -1112,20 +1151,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" t="s">
         <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I11" t="s">
         <v>26</v>
@@ -1137,20 +1176,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" t="s">
         <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I12" t="s">
         <v>26</v>
@@ -1162,20 +1201,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" t="s">
         <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" t="s">
         <v>23</v>
@@ -1187,20 +1226,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" t="s">
         <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I14" t="s">
         <v>26</v>
@@ -1212,23 +1251,26 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" t="s">
         <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I15" t="s">
         <v>23</v>
@@ -1240,57 +1282,51 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="I16" t="s">
-        <v>26</v>
+        <v>132</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
+        <v>133</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I17" t="s">
         <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L17" t="s">
         <v>24</v>
@@ -1300,25 +1336,25 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I18" t="s">
         <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L18" t="s">
         <v>24</v>
@@ -1326,60 +1362,57 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="C19" s="6"/>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>114</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="L19" t="s">
         <v>24</v>
-      </c>
-      <c r="M19" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I20" t="s">
         <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
@@ -1392,49 +1425,54 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H21" s="11"/>
+        <v>113</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="I21" t="s">
         <v>24</v>
       </c>
       <c r="J21" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="L21" t="s">
         <v>24</v>
+      </c>
+      <c r="M21" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.75">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="10"/>
+        <v>109</v>
+      </c>
+      <c r="H22" s="11"/>
       <c r="I22" t="s">
         <v>24</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L22" t="s">
         <v>24</v>
@@ -1444,81 +1482,79 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>131</v>
+      <c r="H23" s="10"/>
+      <c r="I23" t="s">
+        <v>24</v>
       </c>
       <c r="J23" t="s">
+        <v>65</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.75">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="J24" t="s">
         <v>69</v>
       </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="L24" t="s">
+        <v>24</v>
+      </c>
+      <c r="M24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B24" s="9" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.75">
+      <c r="B25" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" t="s">
-        <v>57</v>
-      </c>
-      <c r="L24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
         <v>118</v>
       </c>
       <c r="F25" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>125</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="H25" s="10"/>
       <c r="I25" t="s">
         <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
@@ -1528,25 +1564,25 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I26" t="s">
         <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L26" t="s">
         <v>23</v>
@@ -1556,23 +1592,25 @@
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H27" s="11"/>
+        <v>114</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="I27" t="s">
         <v>23</v>
       </c>
       <c r="J27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L27" t="s">
         <v>23</v>
@@ -1582,23 +1620,23 @@
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" t="s">
         <v>23</v>
       </c>
       <c r="J28" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L28" t="s">
         <v>23</v>
@@ -1608,23 +1646,23 @@
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" t="s">
         <v>23</v>
       </c>
       <c r="J29" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="L29" t="s">
         <v>23</v>
@@ -1634,55 +1672,81 @@
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="L30" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="11"/>
+      <c r="I31" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.75">
+      <c r="B32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="C32" s="7"/>
+      <c r="D32" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32" t="s">
         <v>28</v>
       </c>
-      <c r="L31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B32" s="8" t="s">
+      <c r="L32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.75">
+      <c r="B33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added variables previous waves, need to fix drinking and Nas health outcomes
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04AD38B-5C59-4845-8417-1946FF7BC300}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260715B9-BB6B-40CC-84DA-6C164C539286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="82935" yWindow="8970" windowWidth="5760" windowHeight="1230" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="57480" yWindow="5880" windowWidth="29040" windowHeight="15840" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable_sheet_thesis" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="138">
   <si>
     <t>Variable group</t>
   </si>
@@ -459,6 +459,9 @@
       </rPr>
       <t>our subset or full set</t>
     </r>
+  </si>
+  <si>
+    <t>Need to combine this together with drinking days!</t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
   <dimension ref="A2:M33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1250,6 +1253,9 @@
       <c r="L14" t="s">
         <v>24</v>
       </c>
+      <c r="M14" s="13" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Added drinking variable and changed prev wave to11 - needed for multiple blood pressure measurements
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260715B9-BB6B-40CC-84DA-6C164C539286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC9E839-6D64-4629-BA4C-D77AFD757A98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="5880" windowWidth="29040" windowHeight="15840" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable_sheet_thesis" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="161">
   <si>
     <t>Variable group</t>
   </si>
@@ -177,9 +177,6 @@
     <t>pc129</t>
   </si>
   <si>
-    <t>number days per week drink alcohol</t>
-  </si>
-  <si>
     <t>pi859 pi864 pi869</t>
   </si>
   <si>
@@ -249,21 +246,9 @@
     <t>Option 5 of pj005m is retired, 1 working now (note that stuff as disabled will just not count as being reitred but will come back in the job status variable)</t>
   </si>
   <si>
-    <t>s12drink, s13drink</t>
-  </si>
-  <si>
-    <t>r12smoken, r13smoken</t>
-  </si>
-  <si>
-    <t>r12mstat, r13 mstat</t>
-  </si>
-  <si>
     <t>Widowed between previous and current period</t>
   </si>
   <si>
-    <t>r12mstat, r13mstat</t>
-  </si>
-  <si>
     <t>Marital status difference (r12 = 1.married, r13 = 5.divorced)</t>
   </si>
   <si>
@@ -282,9 +267,6 @@
     <t>rDisc1-10</t>
   </si>
   <si>
-    <t>sysBPM1-3</t>
-  </si>
-  <si>
     <t>wLbs</t>
   </si>
   <si>
@@ -306,9 +288,6 @@
     <t>nSmokemos</t>
   </si>
   <si>
-    <t>rnDrink</t>
-  </si>
-  <si>
     <t>jobStat.A1-5</t>
   </si>
   <si>
@@ -319,15 +298,6 @@
   </si>
   <si>
     <t>milAct</t>
-  </si>
-  <si>
-    <t>mStat12,13</t>
-  </si>
-  <si>
-    <t>smoker12,13</t>
-  </si>
-  <si>
-    <t>drinker12,13</t>
   </si>
   <si>
     <t>race</t>
@@ -461,7 +431,106 @@
     </r>
   </si>
   <si>
-    <t>Need to combine this together with drinking days!</t>
+    <t>nSmokepw</t>
+  </si>
+  <si>
+    <t>Smoke cigarettes previous wave</t>
+  </si>
+  <si>
+    <t>wLbs_pw</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>weight (for BMI) prevoius wave</t>
+  </si>
+  <si>
+    <t>syBPM1-3</t>
+  </si>
+  <si>
+    <t>pw_syBPM1-3</t>
+  </si>
+  <si>
+    <t>Systolic blood pressure previous wave</t>
+  </si>
+  <si>
+    <t>hInc_pw</t>
+  </si>
+  <si>
+    <t>height (for BMI) previous wave</t>
+  </si>
+  <si>
+    <t>Waist circumference - prevoius wave</t>
+  </si>
+  <si>
+    <t>number days per week drink alcohol previous wave (last 3 months)</t>
+  </si>
+  <si>
+    <t>number days per week drink alcohol (last 3 months)</t>
+  </si>
+  <si>
+    <t>pc130</t>
+  </si>
+  <si>
+    <t>nDDrink_pw</t>
+  </si>
+  <si>
+    <t>nDDrink</t>
+  </si>
+  <si>
+    <t>number glasses on days that drink</t>
+  </si>
+  <si>
+    <t>nGDrink_pw</t>
+  </si>
+  <si>
+    <t>nGDrink</t>
+  </si>
+  <si>
+    <t>nc118</t>
+  </si>
+  <si>
+    <t>ni907</t>
+  </si>
+  <si>
+    <t>ni834</t>
+  </si>
+  <si>
+    <t>ni841</t>
+  </si>
+  <si>
+    <t>ni859 ni864 ni869</t>
+  </si>
+  <si>
+    <t>nc129</t>
+  </si>
+  <si>
+    <t>nc130</t>
+  </si>
+  <si>
+    <t>Previous wave = wave 11 -- 2012, Current wave = wave 13 -- 2016</t>
+  </si>
+  <si>
+    <t>r11mstat, r13 mstat</t>
+  </si>
+  <si>
+    <t>r11mstat, r13mstat</t>
+  </si>
+  <si>
+    <t>r11smnken, r13smnken</t>
+  </si>
+  <si>
+    <t>s11drink, s13drink</t>
+  </si>
+  <si>
+    <t>mStat11,13</t>
+  </si>
+  <si>
+    <t>smoker11,13</t>
+  </si>
+  <si>
+    <t>drinker11,13</t>
   </si>
 </sst>
 </file>
@@ -909,48 +978,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
-  <dimension ref="A2:M33"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28:F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1328125" customWidth="1"/>
-    <col min="9" max="9" width="30.40625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E1" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>22</v>
@@ -966,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K3" s="1" t="s">
         <v>4</v>
       </c>
@@ -974,7 +1048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -983,7 +1057,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -995,14 +1069,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -1014,22 +1088,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
@@ -1041,51 +1115,42 @@
         <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
@@ -1097,662 +1162,826 @@
         <v>24</v>
       </c>
       <c r="M8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>129</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="J9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
         <v>18</v>
       </c>
-      <c r="L9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="B10" s="6" t="s">
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="E14" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" t="s">
         <v>38</v>
       </c>
-      <c r="L10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" t="s">
-        <v>109</v>
-      </c>
-      <c r="I11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" t="s">
-        <v>110</v>
-      </c>
-      <c r="I14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" t="s">
-        <v>47</v>
-      </c>
       <c r="L14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
-        <v>130</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>125</v>
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
+        <v>99</v>
       </c>
       <c r="I15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="L15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="F16" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G16" t="s">
-        <v>109</v>
-      </c>
-      <c r="H16" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="J16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.75">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>126</v>
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
       </c>
       <c r="I17" t="s">
         <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="L17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>126</v>
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
+        <v>100</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="I19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" t="s">
+        <v>100</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" t="s">
+        <v>142</v>
+      </c>
+      <c r="G20" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" t="s">
         <v>26</v>
       </c>
-      <c r="J19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="I20" t="s">
-        <v>24</v>
-      </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>139</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
       </c>
-      <c r="M20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.75">
+      <c r="M20" s="13"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="I21" t="s">
-        <v>24</v>
+        <v>144</v>
+      </c>
+      <c r="G21" t="s">
+        <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>74</v>
-      </c>
-      <c r="L21" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.75">
+        <v>143</v>
+      </c>
+      <c r="M21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="E22" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="F22" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" t="s">
-        <v>24</v>
+        <v>145</v>
+      </c>
+      <c r="G22" t="s">
+        <v>96</v>
       </c>
       <c r="J22" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.75">
+        <v>143</v>
+      </c>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" s="10"/>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.75">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="J24" t="s">
-        <v>69</v>
-      </c>
-      <c r="L24" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24" t="s">
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E28" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" t="s">
+        <v>158</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B25" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="10"/>
-      <c r="I25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" t="s">
-        <v>57</v>
-      </c>
-      <c r="L25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F26" t="s">
-        <v>98</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="I26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" t="s">
-        <v>19</v>
-      </c>
-      <c r="L26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="L29" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>159</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I27" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="H28" s="11"/>
-      <c r="I28" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" t="s">
-        <v>106</v>
-      </c>
-      <c r="F29" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H29" s="11"/>
-      <c r="I29" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" t="s">
-        <v>25</v>
-      </c>
-      <c r="L29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J30" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J32" t="s">
+        <v>68</v>
+      </c>
+      <c r="L32" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" t="s">
+        <v>56</v>
+      </c>
+      <c r="L33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+      <c r="L34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" t="s">
+        <v>90</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" t="s">
         <v>53</v>
       </c>
-      <c r="L30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="E38" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G31" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H31" s="11"/>
-      <c r="I31" t="s">
-        <v>23</v>
-      </c>
-      <c r="J31" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.75">
-      <c r="B32" s="7" t="s">
+      <c r="H38" s="11"/>
+      <c r="I38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J38" t="s">
+        <v>52</v>
+      </c>
+      <c r="L38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" t="s">
+        <v>23</v>
+      </c>
+      <c r="J39" t="s">
+        <v>73</v>
+      </c>
+      <c r="L39" t="s">
+        <v>24</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" t="s">
-        <v>77</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="C40" s="7"/>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+      <c r="J40" t="s">
         <v>28</v>
       </c>
-      <c r="L32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.75">
-      <c r="B33" s="8" t="s">
+      <c r="L40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="C41" s="8"/>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="J41" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixes and first version prelim data analysis
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC9E839-6D64-4629-BA4C-D77AFD757A98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1935E33-8C37-4C18-AEE1-871CBB3F194D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="57480" yWindow="5880" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Variable_sheet_thesis" sheetId="1" r:id="rId1"/>
+    <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
+    <sheet name="Model_data_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Model_data_2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="203">
   <si>
     <t>Variable group</t>
   </si>
@@ -532,12 +534,138 @@
   <si>
     <t>drinker11,13</t>
   </si>
+  <si>
+    <t>Outcomes</t>
+  </si>
+  <si>
+    <t>Moderators</t>
+  </si>
+  <si>
+    <t>Control variables</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Numerical (1 = male, 2 = female)</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>mStat13</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>syBP_mean</t>
+  </si>
+  <si>
+    <t>expRDAll</t>
+  </si>
+  <si>
+    <t>d_syBP_mean</t>
+  </si>
+  <si>
+    <t>d_BMI</t>
+  </si>
+  <si>
+    <t>d_waist</t>
+  </si>
+  <si>
+    <t>wealth_bin</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Health behavior</t>
+  </si>
+  <si>
+    <t>Recent major life events</t>
+  </si>
+  <si>
+    <t>mStat11</t>
+  </si>
+  <si>
+    <t>drinker13</t>
+  </si>
+  <si>
+    <t>drinker11</t>
+  </si>
+  <si>
+    <t>smoker13</t>
+  </si>
+  <si>
+    <t>smoker11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nDDrink  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nGDrink  </t>
+  </si>
+  <si>
+    <t>prevRetStat</t>
+  </si>
+  <si>
+    <t>nDrinkPerWeek</t>
+  </si>
+  <si>
+    <t>nDrinkPerWeek_pw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerical  </t>
+  </si>
+  <si>
+    <t>quit_smoking</t>
+  </si>
+  <si>
+    <t>started_smoking</t>
+  </si>
+  <si>
+    <t>quit_drinking</t>
+  </si>
+  <si>
+    <t>started_drinking</t>
+  </si>
+  <si>
+    <t>divorced_or seperated</t>
+  </si>
+  <si>
+    <t>widowed</t>
+  </si>
+  <si>
+    <t>recently_married_or_partnered</t>
+  </si>
+  <si>
+    <t>quit_working</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>1) Inclusion previous waves may be for "consistency" of behavior or proximity to lifechanging event in case necessary</t>
+  </si>
+  <si>
+    <t>2) Life events not especially included because those are expected to explain changes but not so much levels (levels can be explained by level of variable that changes as a result of the life-chainging event)</t>
+  </si>
+  <si>
+    <t>2) Life events included as they may explain changes in health outcomes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,8 +711,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,6 +762,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -646,10 +786,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -664,8 +805,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -980,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F31"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,4 +2137,884 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37E278C-1DAC-4F67-8E1E-CC1E987D4B76}">
+  <dimension ref="C2:I49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
+      <c r="D22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="18"/>
+      <c r="D40" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2B95C5-E717-4ABB-BAF8-DAA816951EFA}">
+  <dimension ref="C2:I49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
+      <c r="D22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="9"/>
+      <c r="D40" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on data cleaning proper
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1935E33-8C37-4C18-AEE1-871CBB3F194D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F9CE7-E44D-4039-A0F4-3CB16A974196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="5880" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
     <sheet name="Model_data_1" sheetId="2" r:id="rId2"/>
-    <sheet name="Model_data_2" sheetId="4" r:id="rId3"/>
+    <sheet name="Dataset_1" sheetId="5" r:id="rId3"/>
+    <sheet name="Dataset_2" sheetId="6" r:id="rId4"/>
+    <sheet name="Model_data_2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="214">
   <si>
     <t>Variable group</t>
   </si>
@@ -659,6 +661,39 @@
   </si>
   <si>
     <t>2) Life events included as they may explain changes in health outcomes</t>
+  </si>
+  <si>
+    <t>Number of observations</t>
+  </si>
+  <si>
+    <t>Description step</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>HRS dataset 2016</t>
+  </si>
+  <si>
+    <t>Filled in question about discrimination and measured health outcomes</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Remove unrealistic health outcome measurements</t>
+  </si>
+  <si>
+    <t>SYSBPM's &lt;30, &gt;500, wLBS of &lt;30, &gt;500, hIn of &lt;40, &gt;95, waist of &lt;15, &gt;95</t>
+  </si>
+  <si>
+    <t>Remove unrealistic health outcome measurements and not available differences</t>
+  </si>
+  <si>
+    <t>Remove observations with missing values of moderators</t>
+  </si>
+  <si>
+    <t>Sex, wealth bin, race and age</t>
   </si>
 </sst>
 </file>
@@ -768,7 +803,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -785,12 +820,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -811,6 +855,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2143,7 +2188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37E278C-1DAC-4F67-8E1E-CC1E987D4B76}">
   <dimension ref="C2:I49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
@@ -2580,6 +2625,176 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
+  <dimension ref="C2:F6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>20912</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>5551</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <f>C4-C3</f>
+        <v>-15361</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>C4+E5</f>
+        <v>5512</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5">
+        <v>-39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>C5+E6</f>
+        <v>4581</v>
+      </c>
+      <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6">
+        <v>-931</v>
+      </c>
+      <c r="F6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
+  <dimension ref="C2:F6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>20912</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>5551</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <f>C4-C3</f>
+        <v>-15361</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>C4+E5</f>
+        <v>4197</v>
+      </c>
+      <c r="D5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5">
+        <v>-1354</v>
+      </c>
+      <c r="F5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6">
+        <f>C6-C5</f>
+        <v>-94</v>
+      </c>
+      <c r="F6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2B95C5-E717-4ABB-BAF8-DAA816951EFA}">
   <dimension ref="C2:I49"/>
   <sheetViews>

</xml_diff>

<commit_message>
Built first complete sample and bugfix
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F9CE7-E44D-4039-A0F4-3CB16A974196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911899B4-4181-4E3C-BFA2-44F353C3F978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="241">
   <si>
     <t>Variable group</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>Num cigarettes smoked per day when smoked most</t>
-  </si>
-  <si>
-    <t>pc129</t>
   </si>
   <si>
     <t>pi859 pi864 pi869</t>
@@ -474,9 +471,6 @@
     <t>number days per week drink alcohol (last 3 months)</t>
   </si>
   <si>
-    <t>pc130</t>
-  </si>
-  <si>
     <t>nDDrink_pw</t>
   </si>
   <si>
@@ -507,12 +501,6 @@
     <t>ni859 ni864 ni869</t>
   </si>
   <si>
-    <t>nc129</t>
-  </si>
-  <si>
-    <t>nc130</t>
-  </si>
-  <si>
     <t>Previous wave = wave 11 -- 2012, Current wave = wave 13 -- 2016</t>
   </si>
   <si>
@@ -525,9 +513,6 @@
     <t>r11smnken, r13smnken</t>
   </si>
   <si>
-    <t>s11drink, s13drink</t>
-  </si>
-  <si>
     <t>mStat11,13</t>
   </si>
   <si>
@@ -687,20 +672,119 @@
     <t>SYSBPM's &lt;30, &gt;500, wLBS of &lt;30, &gt;500, hIn of &lt;40, &gt;95, waist of &lt;15, &gt;95</t>
   </si>
   <si>
-    <t>Remove unrealistic health outcome measurements and not available differences</t>
-  </si>
-  <si>
     <t>Remove observations with missing values of moderators</t>
   </si>
   <si>
     <t>Sex, wealth bin, race and age</t>
+  </si>
+  <si>
+    <t>Representative of households</t>
+  </si>
+  <si>
+    <t>Filled in question about discrimination and measured health outcomes 2016</t>
+  </si>
+  <si>
+    <t>Remove unrealistic health outcome measurements and not available differences (no 2012  measurement)</t>
+  </si>
+  <si>
+    <t>Representativenes (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dropped nSmoke_mos, everSmoke, nSmoke_pw </t>
+  </si>
+  <si>
+    <t>r11drink, r13drink</t>
+  </si>
+  <si>
+    <t>r13drinkd</t>
+  </si>
+  <si>
+    <t>r11drinkd</t>
+  </si>
+  <si>
+    <t>r11drinkn</t>
+  </si>
+  <si>
+    <t>double (set 99 to 7)</t>
+  </si>
+  <si>
+    <t>double (set 99 to maxvalue after 99)</t>
+  </si>
+  <si>
+    <t>Drop variables with very large amounts of missing values</t>
+  </si>
+  <si>
+    <t>Drop variablers that have low amounts of extra information and large amounts of missing values</t>
+  </si>
+  <si>
+    <t>Dropped Maried, smokeNow</t>
+  </si>
+  <si>
+    <t>Remove observations with missing activity answers</t>
+  </si>
+  <si>
+    <t>Remove observations with missing information on being a smoker/drinker in w13</t>
+  </si>
+  <si>
+    <t>Smoker/Drinker13</t>
+  </si>
+  <si>
+    <t>Impute values from other wave for variables where that is a feasible approach</t>
+  </si>
+  <si>
+    <t>mStat11 &amp; 13, prevRetStat, smoker13, smoker11, etc</t>
+  </si>
+  <si>
+    <t>Possible impact</t>
+  </si>
+  <si>
+    <t>Representativeness</t>
+  </si>
+  <si>
+    <t>Measurement errors</t>
+  </si>
+  <si>
+    <t>Representativeness, but probably MAR</t>
+  </si>
+  <si>
+    <t>Bias if informative</t>
+  </si>
+  <si>
+    <t>Probably not MAR but, small no obs</t>
+  </si>
+  <si>
+    <t>Bias, but probably reliable estimates</t>
+  </si>
+  <si>
+    <t>Representativeness but small no obs</t>
+  </si>
+  <si>
+    <t>Impute missing values left in moEducation with KNN</t>
+  </si>
+  <si>
+    <t>Impute missing values left in education with mode impute</t>
+  </si>
+  <si>
+    <t>Educ(1)</t>
+  </si>
+  <si>
+    <t>MoEc(353)</t>
+  </si>
+  <si>
+    <t>Bias but assumed to be estimate-able</t>
+  </si>
+  <si>
+    <t>Bias but only one value that is assumed to be less relevant than all other information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,8 +837,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -802,6 +907,16 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -830,11 +945,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -855,11 +973,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="4"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1174,7 +1300,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E1" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1202,22 +1328,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>22</v>
@@ -1250,7 +1376,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
         <v>23</v>
@@ -1269,7 +1395,7 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" t="s">
         <v>23</v>
@@ -1287,16 +1413,16 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
@@ -1308,139 +1434,139 @@
         <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" t="s">
         <v>133</v>
-      </c>
-      <c r="G7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L8" t="s">
         <v>24</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" t="s">
         <v>129</v>
       </c>
-      <c r="G9" t="s">
-        <v>96</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>130</v>
-      </c>
-      <c r="J9" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I10" t="s">
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L10" t="s">
         <v>24</v>
       </c>
       <c r="M10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" t="s">
         <v>135</v>
-      </c>
-      <c r="G11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J11" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I12" t="s">
         <v>24</v>
@@ -1456,19 +1582,19 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -1476,19 +1602,19 @@
         <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I14" t="s">
         <v>23</v>
@@ -1507,13 +1633,13 @@
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
         <v>26</v>
@@ -1529,19 +1655,19 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" t="s">
         <v>127</v>
-      </c>
-      <c r="G16" t="s">
-        <v>105</v>
-      </c>
-      <c r="J16" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1551,13 +1677,13 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I17" t="s">
         <v>26</v>
@@ -1576,13 +1702,13 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I18" t="s">
         <v>23</v>
@@ -1598,41 +1724,41 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>215</v>
       </c>
       <c r="E19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G19" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="J19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>214</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="I20" t="s">
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
@@ -1643,19 +1769,19 @@
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>216</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>218</v>
       </c>
       <c r="J21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M21" s="13"/>
     </row>
@@ -1663,48 +1789,48 @@
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G22" t="s">
-        <v>96</v>
+        <v>218</v>
       </c>
       <c r="J22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M22" s="13"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G23" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="I23" t="s">
         <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
@@ -1714,41 +1840,41 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" t="s">
         <v>121</v>
       </c>
-      <c r="E24" t="s">
-        <v>121</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
+        <v>98</v>
+      </c>
+      <c r="H24" t="s">
         <v>122</v>
       </c>
-      <c r="G24" t="s">
-        <v>99</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>123</v>
-      </c>
-      <c r="J24" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I25" t="s">
         <v>26</v>
@@ -1767,16 +1893,16 @@
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s">
         <v>26</v>
@@ -1795,16 +1921,16 @@
         <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I27" t="s">
         <v>26</v>
@@ -1819,88 +1945,88 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I28" t="s">
         <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L28" t="s">
         <v>24</v>
       </c>
       <c r="M28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I29" t="s">
         <v>24</v>
       </c>
       <c r="J29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L29" t="s">
         <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F30" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" t="s">
         <v>24</v>
       </c>
       <c r="J30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L30" t="s">
         <v>24</v>
@@ -1910,23 +2036,23 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" t="s">
         <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L31" t="s">
         <v>24</v>
@@ -1936,28 +2062,28 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="J32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L32" t="s">
         <v>24</v>
       </c>
       <c r="M32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
@@ -1966,23 +2092,23 @@
       </c>
       <c r="C33" s="9"/>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H33" s="10"/>
       <c r="I33" t="s">
         <v>23</v>
       </c>
       <c r="J33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L33" t="s">
         <v>23</v>
@@ -1995,16 +2121,16 @@
         <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I34" t="s">
         <v>23</v>
@@ -2023,16 +2149,16 @@
         <v>29</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I35" t="s">
         <v>23</v>
@@ -2051,13 +2177,13 @@
         <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H36" s="11"/>
       <c r="I36" t="s">
@@ -2077,13 +2203,13 @@
         <v>32</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" t="s">
@@ -2100,23 +2226,23 @@
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H38" s="11"/>
       <c r="I38" t="s">
         <v>23</v>
       </c>
       <c r="J38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L38" t="s">
         <v>23</v>
@@ -2126,29 +2252,29 @@
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
         <v>94</v>
       </c>
-      <c r="E39" t="s">
-        <v>96</v>
-      </c>
-      <c r="F39" t="s">
-        <v>95</v>
-      </c>
       <c r="G39" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" t="s">
         <v>23</v>
       </c>
       <c r="J39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L39" t="s">
         <v>24</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
@@ -2157,7 +2283,7 @@
       </c>
       <c r="C40" s="7"/>
       <c r="D40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J40" t="s">
         <v>28</v>
@@ -2172,7 +2298,7 @@
       </c>
       <c r="C41" s="8"/>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J41" t="s">
         <v>27</v>
@@ -2202,59 +2328,59 @@
   <sheetData>
     <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
@@ -2263,351 +2389,351 @@
       </c>
       <c r="D7" s="15"/>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="16" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F17" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
       <c r="D22" s="17" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E22" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F38" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F39" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="18"/>
       <c r="D40" s="18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="18" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="18" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
@@ -2626,81 +2752,303 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
-  <dimension ref="C2:F6"/>
+  <dimension ref="C2:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="73.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="I2" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>20912</v>
       </c>
-      <c r="D3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>110313247</v>
+      </c>
+      <c r="E3" s="23">
+        <f>D3/$D$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>5551</v>
       </c>
-      <c r="D4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
+        <v>30222610</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="F4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4">
         <f>C4-C3</f>
         <v>-15361</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5">
-        <f>C4+E5</f>
+        <f>C4+G5</f>
         <v>5512</v>
       </c>
-      <c r="D5" t="s">
-        <v>209</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
+        <v>30009584</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.27203971251068332</v>
+      </c>
+      <c r="F5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5">
         <v>-39</v>
       </c>
-      <c r="F5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6">
-        <f>C5+E6</f>
+        <f>C5+G6</f>
         <v>4581</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>25667783</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6">
+        <v>-931</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4581</v>
+      </c>
+      <c r="D7">
+        <v>25667783</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7">
+        <f>C7-C6</f>
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
         <v>212</v>
       </c>
-      <c r="E6">
-        <v>-931</v>
-      </c>
-      <c r="F6" t="s">
-        <v>213</v>
+      <c r="I7" s="22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4581</v>
+      </c>
+      <c r="D8">
+        <v>25667783</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G13" si="1">C8-C7</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4548</v>
+      </c>
+      <c r="D9">
+        <v>25489283</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>-33</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4548</v>
+      </c>
+      <c r="D10">
+        <v>25489283</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4529</v>
+      </c>
+      <c r="D11">
+        <v>25394917</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="F11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4529</v>
+      </c>
+      <c r="D12">
+        <v>25394917</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4529</v>
+      </c>
+      <c r="D13">
+        <v>25394917</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2711,81 +3059,222 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
-  <dimension ref="C2:F6"/>
+  <dimension ref="C2:H13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="97.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>20912</v>
       </c>
-      <c r="D3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>110313247</v>
+      </c>
+      <c r="E3" s="23">
+        <f>D3/$D$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>5551</v>
       </c>
-      <c r="D4" t="s">
-        <v>207</v>
-      </c>
-      <c r="E4">
+      <c r="D4">
+        <v>30222610</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="F4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4">
         <f>C4-C3</f>
         <v>-15361</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5">
-        <f>C4+E5</f>
+        <f>C4+G5</f>
         <v>4197</v>
       </c>
-      <c r="D5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E5">
-        <v>-1354</v>
+      <c r="D5">
+        <v>23381704</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21195735449614678</v>
       </c>
       <c r="F5" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>-1354</v>
+      </c>
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>4103</v>
       </c>
-      <c r="D6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E6">
+      <c r="D6">
+        <v>23182405</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6">
         <f>C6-C5</f>
         <v>-94</v>
       </c>
-      <c r="F6" t="s">
-        <v>213</v>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4103</v>
+      </c>
+      <c r="D7">
+        <v>23182405</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4103</v>
+      </c>
+      <c r="D8">
+        <v>23182405</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4073</v>
+      </c>
+      <c r="D9">
+        <v>23012867</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20861381226499479</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4073</v>
+      </c>
+      <c r="D10">
+        <v>22945346</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4059</v>
+      </c>
+      <c r="D11">
+        <v>22945346</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4059</v>
+      </c>
+      <c r="D12">
+        <v>22945346</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4059</v>
+      </c>
+      <c r="D13">
+        <v>22945346</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2812,59 +3301,59 @@
   <sheetData>
     <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
@@ -2873,351 +3362,351 @@
       </c>
       <c r="D7" s="15"/>
       <c r="E7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="16" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F17" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
       <c r="D22" s="17" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E22" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F31" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C40" s="9"/>
       <c r="D40" s="17" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E40" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made extra evaluation and k-fold ps  estimation possible
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,16 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911899B4-4181-4E3C-BFA2-44F353C3F978}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7CA4EE-6DD9-460A-83E8-194BB025BA3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="17685" yWindow="675" windowWidth="21600" windowHeight="10890" firstSheet="3" activeTab="6" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
     <sheet name="Model_data_1" sheetId="2" r:id="rId2"/>
     <sheet name="Dataset_1" sheetId="5" r:id="rId3"/>
-    <sheet name="Dataset_2" sheetId="6" r:id="rId4"/>
-    <sheet name="Model_data_2" sheetId="4" r:id="rId5"/>
+    <sheet name="Text_table_sample_cons" sheetId="7" r:id="rId4"/>
+    <sheet name="Table_summary_stats" sheetId="8" r:id="rId5"/>
+    <sheet name="Text_table_AUCs" sheetId="10" r:id="rId6"/>
+    <sheet name="Unweighted results table" sheetId="11" r:id="rId7"/>
+    <sheet name="Text_table_sumstats" sheetId="9" r:id="rId8"/>
+    <sheet name="Dataset_2" sheetId="6" r:id="rId9"/>
+    <sheet name="Model_data_2" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="342">
   <si>
     <t>Variable group</t>
   </si>
@@ -776,15 +781,321 @@
   <si>
     <t>Bias but only one value that is assumed to be less relevant than all other information</t>
   </si>
+  <si>
+    <t>Respondents</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>Longitudinal sample</t>
+  </si>
+  <si>
+    <t>Cross-sectional sample</t>
+  </si>
+  <si>
+    <t>Population represented</t>
+  </si>
+  <si>
+    <t>Share total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAND HRS 2016 </t>
+  </si>
+  <si>
+    <t>No measure health or discrimination</t>
+  </si>
+  <si>
+    <t>Missing moderator variables</t>
+  </si>
+  <si>
+    <t>Missing smoking and drinking \tnote{\dag}</t>
+  </si>
+  <si>
+    <t>Missing activity answers</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Unweighted sample</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Sd.</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Cardio-metabolic risk markers</t>
+  </si>
+  <si>
+    <t>Weighted sample</t>
+  </si>
+  <si>
+    <t>Unweighted sample (z = 1)</t>
+  </si>
+  <si>
+    <t>Unweighted sample (z = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n = </t>
+  </si>
+  <si>
+    <t>n = 25,394,917</t>
+  </si>
+  <si>
+    <t>n = 4,259</t>
+  </si>
+  <si>
+    <t>Systolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>Experienced racial discrimination</t>
+  </si>
+  <si>
+    <t>Control an moderator variables</t>
+  </si>
+  <si>
+    <t>Demographics (control only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demographics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race </t>
+  </si>
+  <si>
+    <t>White or caucasian</t>
+  </si>
+  <si>
+    <t>Black or African American</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Wealth bin</t>
+  </si>
+  <si>
+    <t>Marital status 2012</t>
+  </si>
+  <si>
+    <t>Marital status 2016</t>
+  </si>
+  <si>
+    <t>Education level</t>
+  </si>
+  <si>
+    <t>lt high-school</t>
+  </si>
+  <si>
+    <t>ged</t>
+  </si>
+  <si>
+    <t>high-school graduate</t>
+  </si>
+  <si>
+    <t>some college</t>
+  </si>
+  <si>
+    <t>college and above</t>
+  </si>
+  <si>
+    <t>Education mother (years)</t>
+  </si>
+  <si>
+    <t>Working status 2012</t>
+  </si>
+  <si>
+    <t>Working status 2016</t>
+  </si>
+  <si>
+    <t>Drinker 2012</t>
+  </si>
+  <si>
+    <t>Drinker 2016</t>
+  </si>
+  <si>
+    <t>Drinking days per week 2016</t>
+  </si>
+  <si>
+    <t>Drinking days per week 2012</t>
+  </si>
+  <si>
+    <t>Drinks per drinking day 2012</t>
+  </si>
+  <si>
+    <t>Drinks per drinking day 2016</t>
+  </si>
+  <si>
+    <t>Drinks per week 2016</t>
+  </si>
+  <si>
+    <t>Drinks per week  2012</t>
+  </si>
+  <si>
+    <t>Smoker 2012</t>
+  </si>
+  <si>
+    <t>Smoker 2016</t>
+  </si>
+  <si>
+    <t>Activity - vigorous</t>
+  </si>
+  <si>
+    <t>Every day</t>
+  </si>
+  <si>
+    <t>More than once a week</t>
+  </si>
+  <si>
+    <t>One to three times a month</t>
+  </si>
+  <si>
+    <t>Hardly ever or never</t>
+  </si>
+  <si>
+    <t>Activity - moderate</t>
+  </si>
+  <si>
+    <t>Activity - mild</t>
+  </si>
+  <si>
+    <t>Quit smoking</t>
+  </si>
+  <si>
+    <t>Started smoking</t>
+  </si>
+  <si>
+    <t>Quit drinking</t>
+  </si>
+  <si>
+    <t>Started drinking</t>
+  </si>
+  <si>
+    <t>Divorced or seperated</t>
+  </si>
+  <si>
+    <t>Widowed</t>
+  </si>
+  <si>
+    <t>Recenlty married</t>
+  </si>
+  <si>
+    <t>Quit working</t>
+  </si>
+  <si>
+    <t>z = 1</t>
+  </si>
+  <si>
+    <t>z = 0</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Share cum.</t>
+  </si>
+  <si>
+    <t>Moderator variables - ratios</t>
+  </si>
+  <si>
+    <t>Moderator variables - characteristics</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>n =</t>
+  </si>
+  <si>
+    <t>Mean Systolic Blood Pressure</t>
+  </si>
+  <si>
+    <t>k = 2</t>
+  </si>
+  <si>
+    <t>k = 3</t>
+  </si>
+  <si>
+    <t>k = 4</t>
+  </si>
+  <si>
+    <t>m = 50</t>
+  </si>
+  <si>
+    <t>m = 100</t>
+  </si>
+  <si>
+    <t>m = 200</t>
+  </si>
+  <si>
+    <t>m =200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unbalanced </t>
+  </si>
+  <si>
+    <t>SMOTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
+  <si>
+    <t>$hat{(C)ATE}$</t>
+  </si>
+  <si>
+    <t>$P(CATE)&gt;0$</t>
+  </si>
+  <si>
+    <t>ATE</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Femal</t>
+  </si>
+  <si>
+    <t>Age group</t>
+  </si>
+  <si>
+    <t>Wealth Bin</t>
+  </si>
+  <si>
+    <t>&lt;60</t>
+  </si>
+  <si>
+    <t>60-80</t>
+  </si>
+  <si>
+    <t>&gt;80</t>
+  </si>
+  <si>
+    <t>HDPI 89% (u)</t>
+  </si>
+  <si>
+    <t>HDPI 89% (l)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="171" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -858,6 +1169,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -918,7 +1237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -944,6 +1263,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -952,7 +1280,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -978,7 +1306,38 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="4"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2310,980 +2669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37E278C-1DAC-4F67-8E1E-CC1E987D4B76}">
-  <dimension ref="C2:I49"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" t="s">
-        <v>92</v>
-      </c>
-      <c r="F12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" t="s">
-        <v>175</v>
-      </c>
-      <c r="F16" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" t="s">
-        <v>163</v>
-      </c>
-      <c r="F17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" t="s">
-        <v>182</v>
-      </c>
-      <c r="F19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="9"/>
-      <c r="D22" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="E22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="18"/>
-      <c r="D40" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
-  <dimension ref="C2:I13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="73.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>20912</v>
-      </c>
-      <c r="D3">
-        <v>110313247</v>
-      </c>
-      <c r="E3" s="23">
-        <f>D3/$D$3</f>
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>5551</v>
-      </c>
-      <c r="D4">
-        <v>30222610</v>
-      </c>
-      <c r="E4" s="23">
-        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
-        <v>0.27397081331492307</v>
-      </c>
-      <c r="F4" t="s">
-        <v>202</v>
-      </c>
-      <c r="G4">
-        <f>C4-C3</f>
-        <v>-15361</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <f>C4+G5</f>
-        <v>5512</v>
-      </c>
-      <c r="D5">
-        <v>30009584</v>
-      </c>
-      <c r="E5" s="23">
-        <f t="shared" si="0"/>
-        <v>0.27203971251068332</v>
-      </c>
-      <c r="F5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G5">
-        <v>-39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>205</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <f>C5+G6</f>
-        <v>4581</v>
-      </c>
-      <c r="D6">
-        <v>25667783</v>
-      </c>
-      <c r="E6" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23268087648621202</v>
-      </c>
-      <c r="F6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G6">
-        <v>-931</v>
-      </c>
-      <c r="H6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>4581</v>
-      </c>
-      <c r="D7">
-        <v>25667783</v>
-      </c>
-      <c r="E7" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23268087648621202</v>
-      </c>
-      <c r="F7" t="s">
-        <v>219</v>
-      </c>
-      <c r="G7">
-        <f>C7-C6</f>
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>212</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>4581</v>
-      </c>
-      <c r="D8">
-        <v>25667783</v>
-      </c>
-      <c r="E8" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23268087648621202</v>
-      </c>
-      <c r="F8" t="s">
-        <v>220</v>
-      </c>
-      <c r="G8">
-        <f t="shared" ref="G8:G13" si="1">C8-C7</f>
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>221</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>4548</v>
-      </c>
-      <c r="D9">
-        <v>25489283</v>
-      </c>
-      <c r="E9" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23106275713196983</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>-33</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>4548</v>
-      </c>
-      <c r="D10">
-        <v>25489283</v>
-      </c>
-      <c r="E10" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23106275713196983</v>
-      </c>
-      <c r="F10" t="s">
-        <v>225</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>226</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>4529</v>
-      </c>
-      <c r="D11">
-        <v>25394917</v>
-      </c>
-      <c r="E11" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="F11" t="s">
-        <v>223</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="1"/>
-        <v>-19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>224</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>4529</v>
-      </c>
-      <c r="D12">
-        <v>25394917</v>
-      </c>
-      <c r="E12" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="F12" t="s">
-        <v>235</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>238</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>4529</v>
-      </c>
-      <c r="D13">
-        <v>25394917</v>
-      </c>
-      <c r="E13" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="F13" t="s">
-        <v>236</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>237</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
-  <dimension ref="C2:H13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="97.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>20912</v>
-      </c>
-      <c r="D3">
-        <v>110313247</v>
-      </c>
-      <c r="E3" s="23">
-        <f>D3/$D$3</f>
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>5551</v>
-      </c>
-      <c r="D4">
-        <v>30222610</v>
-      </c>
-      <c r="E4" s="23">
-        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
-        <v>0.27397081331492307</v>
-      </c>
-      <c r="F4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G4">
-        <f>C4-C3</f>
-        <v>-15361</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <f>C4+G5</f>
-        <v>4197</v>
-      </c>
-      <c r="D5">
-        <v>23381704</v>
-      </c>
-      <c r="E5" s="23">
-        <f t="shared" si="0"/>
-        <v>0.21195735449614678</v>
-      </c>
-      <c r="F5" t="s">
-        <v>210</v>
-      </c>
-      <c r="G5">
-        <v>-1354</v>
-      </c>
-      <c r="H5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>4103</v>
-      </c>
-      <c r="D6">
-        <v>23182405</v>
-      </c>
-      <c r="E6" s="23">
-        <f t="shared" si="0"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="F6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G6">
-        <f>C6-C5</f>
-        <v>-94</v>
-      </c>
-      <c r="H6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>4103</v>
-      </c>
-      <c r="D7">
-        <v>23182405</v>
-      </c>
-      <c r="E7" s="23">
-        <f t="shared" si="0"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>4103</v>
-      </c>
-      <c r="D8">
-        <v>23182405</v>
-      </c>
-      <c r="E8" s="23">
-        <f t="shared" si="0"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="F8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>4073</v>
-      </c>
-      <c r="D9">
-        <v>23012867</v>
-      </c>
-      <c r="E9" s="23">
-        <f t="shared" si="0"/>
-        <v>0.20861381226499479</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>4073</v>
-      </c>
-      <c r="D10">
-        <v>22945346</v>
-      </c>
-      <c r="E10" s="23">
-        <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>4059</v>
-      </c>
-      <c r="D11">
-        <v>22945346</v>
-      </c>
-      <c r="E11" s="23">
-        <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>4059</v>
-      </c>
-      <c r="D12">
-        <v>22945346</v>
-      </c>
-      <c r="E12" s="23">
-        <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>4059</v>
-      </c>
-      <c r="D13">
-        <v>22945346</v>
-      </c>
-      <c r="E13" s="23">
-        <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F13" t="s">
-        <v>236</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2B95C5-E717-4ABB-BAF8-DAA816951EFA}">
   <dimension ref="C2:I49"/>
   <sheetViews>
@@ -3721,4 +3107,3200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37E278C-1DAC-4F67-8E1E-CC1E987D4B76}">
+  <dimension ref="C2:I49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="9"/>
+      <c r="D22" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="18"/>
+      <c r="D40" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
+  <dimension ref="C2:J20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="73.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>20912</v>
+      </c>
+      <c r="D3">
+        <v>110313247</v>
+      </c>
+      <c r="E3" s="23">
+        <f>D3/$D$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>5551</v>
+      </c>
+      <c r="D4">
+        <v>30222610</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="F4" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4">
+        <f>C4-C3</f>
+        <v>-15361</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>C4+G5</f>
+        <v>5512</v>
+      </c>
+      <c r="D5">
+        <v>30009584</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.27203971251068332</v>
+      </c>
+      <c r="F5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5">
+        <v>-39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>C5+G6</f>
+        <v>4581</v>
+      </c>
+      <c r="D6">
+        <v>25667783</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6">
+        <v>-931</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4581</v>
+      </c>
+      <c r="D7">
+        <v>25667783</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7">
+        <f>C7-C6</f>
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4581</v>
+      </c>
+      <c r="D8">
+        <v>25667783</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G13" si="1">C8-C7</f>
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>221</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4548</v>
+      </c>
+      <c r="D9">
+        <v>25489283</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>-33</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4548</v>
+      </c>
+      <c r="D10">
+        <v>25489283</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4529</v>
+      </c>
+      <c r="D11">
+        <v>25394917</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="F11" t="s">
+        <v>223</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>224</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4529</v>
+      </c>
+      <c r="D12">
+        <v>25394917</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4529</v>
+      </c>
+      <c r="D13">
+        <v>25394917</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="13"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60364F5B-DCE9-46C6-A586-3092036B5563}">
+  <dimension ref="D4:O12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+    </row>
+    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F5" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="I5" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="J5" s="45"/>
+    </row>
+    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" t="s">
+        <v>242</v>
+      </c>
+      <c r="G6" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I6" t="s">
+        <v>242</v>
+      </c>
+      <c r="J6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7">
+        <f>Dataset_1!C3</f>
+        <v>20912</v>
+      </c>
+      <c r="F7">
+        <f>Dataset_1!D3</f>
+        <v>110313247</v>
+      </c>
+      <c r="G7" s="23">
+        <f>F7/$F$7</f>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f>Dataset_2!C3</f>
+        <v>20912</v>
+      </c>
+      <c r="I7">
+        <f>Dataset_2!D3</f>
+        <v>110313247</v>
+      </c>
+      <c r="J7" s="23">
+        <f>I7/$I$7</f>
+        <v>1</v>
+      </c>
+      <c r="K7" s="23"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8">
+        <f>Dataset_1!C5-Dataset_1!C3</f>
+        <v>-15400</v>
+      </c>
+      <c r="F8">
+        <f>Dataset_1!D5-Dataset_1!D3</f>
+        <v>-80303663</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" ref="G8:G12" si="0">F8/$F$7</f>
+        <v>-0.72796028748931663</v>
+      </c>
+      <c r="H8">
+        <f>Dataset_2!C5-Dataset_2!C3</f>
+        <v>-16715</v>
+      </c>
+      <c r="I8">
+        <f>Dataset_2!D5-Dataset_2!D3</f>
+        <v>-86931543</v>
+      </c>
+      <c r="J8" s="23">
+        <f t="shared" ref="J8:J12" si="1">I8/$I$7</f>
+        <v>-0.78804264550385317</v>
+      </c>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9">
+        <f>Dataset_1!C6-Dataset_1!C5</f>
+        <v>-931</v>
+      </c>
+      <c r="F9">
+        <f>Dataset_1!D6-Dataset_1!D5</f>
+        <v>-4341801</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="0"/>
+        <v>-3.9358836024471294E-2</v>
+      </c>
+      <c r="H9">
+        <f>Dataset_2!C6-Dataset_2!C5</f>
+        <v>-94</v>
+      </c>
+      <c r="I9">
+        <f>Dataset_2!D6-Dataset_2!D5</f>
+        <v>-199299</v>
+      </c>
+      <c r="J9" s="23">
+        <f t="shared" si="1"/>
+        <v>-1.806664253115494E-3</v>
+      </c>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10">
+        <f>Dataset_1!C9-Dataset_1!C6</f>
+        <v>-33</v>
+      </c>
+      <c r="F10">
+        <f>Dataset_1!D9-Dataset_1!D6</f>
+        <v>-178500</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="0"/>
+        <v>-1.6181193542421973E-3</v>
+      </c>
+      <c r="H10">
+        <f>Dataset_2!C9-Dataset_2!C6</f>
+        <v>-30</v>
+      </c>
+      <c r="I10">
+        <f>Dataset_2!D9-Dataset_2!D6</f>
+        <v>-169538</v>
+      </c>
+      <c r="J10" s="23">
+        <f t="shared" si="1"/>
+        <v>-1.5368779780364908E-3</v>
+      </c>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11">
+        <f>Dataset_1!C11-Dataset_1!C9</f>
+        <v>-19</v>
+      </c>
+      <c r="F11">
+        <f>Dataset_1!D11-Dataset_1!D9</f>
+        <v>-94366</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="0"/>
+        <v>-8.5543670018162004E-4</v>
+      </c>
+      <c r="H11">
+        <f>Dataset_2!C11-Dataset_2!C9</f>
+        <v>-14</v>
+      </c>
+      <c r="I11">
+        <f>Dataset_2!D11-Dataset_2!D9</f>
+        <v>-67521</v>
+      </c>
+      <c r="J11" s="23">
+        <f t="shared" si="1"/>
+        <v>-6.1208424043578374E-4</v>
+      </c>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>252</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E7:E11)</f>
+        <v>4529</v>
+      </c>
+      <c r="F12">
+        <f>SUM(F7:F11)</f>
+        <v>25394917</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H12">
+        <f>SUM(H7:H11)</f>
+        <v>4059</v>
+      </c>
+      <c r="I12">
+        <f>SUM(I7:I11)</f>
+        <v>22945346</v>
+      </c>
+      <c r="J12" s="23">
+        <f t="shared" si="1"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="K12" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G12" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FBAE27-4D7B-4D03-B5B4-DAD9C59D9C9D}">
+  <dimension ref="B1:Z60"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:Z2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+    </row>
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="O2" s="24"/>
+      <c r="P2" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="R2" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="S2" s="24"/>
+      <c r="T2" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="U2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="V2" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="W2" s="24"/>
+      <c r="X2" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="C8" s="27"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="27"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C11" s="27"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="27"/>
+      <c r="C14" s="24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B15" s="27"/>
+      <c r="C15" s="24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="24" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="24" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="24" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="C40" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="24"/>
+      <c r="C41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="24"/>
+      <c r="C42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="24"/>
+      <c r="C43" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C44" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="24"/>
+      <c r="C45" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="24"/>
+      <c r="C46" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="24"/>
+      <c r="C47" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="C48" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="24"/>
+      <c r="C49" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="24"/>
+      <c r="C50" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="24"/>
+      <c r="C51" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B6F673-63EF-4D30-A5E9-76FC267124A8}">
+  <dimension ref="C2:L10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="13"/>
+      <c r="E3" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="I3" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="43">
+        <v>0.82180149999999996</v>
+      </c>
+      <c r="F5" s="43">
+        <v>0.82152579999999997</v>
+      </c>
+      <c r="G5" s="43">
+        <v>0.82372889999999999</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43">
+        <v>0.76921150000000005</v>
+      </c>
+      <c r="J5" s="43">
+        <v>0.76580139999999997</v>
+      </c>
+      <c r="K5" s="43">
+        <v>0.76115809999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E6" s="43">
+        <v>0.8236696</v>
+      </c>
+      <c r="F6" s="43">
+        <v>0.82412779999999997</v>
+      </c>
+      <c r="G6" s="43">
+        <v>0.8228801</v>
+      </c>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43">
+        <v>0.76211340000000005</v>
+      </c>
+      <c r="J6" s="43">
+        <v>0.76399660000000003</v>
+      </c>
+      <c r="K6" s="43">
+        <v>0.77052699999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>322</v>
+      </c>
+      <c r="E7" s="43">
+        <v>0.82320090000000001</v>
+      </c>
+      <c r="F7" s="43">
+        <v>0.8227911</v>
+      </c>
+      <c r="G7" s="43">
+        <v>0.82299659999999997</v>
+      </c>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43">
+        <v>0.76773159999999996</v>
+      </c>
+      <c r="J7" s="43">
+        <v>0.76721479999999997</v>
+      </c>
+      <c r="K7" s="43">
+        <v>0.76413359999999997</v>
+      </c>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J8" s="43"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6589B6-0C3E-46EB-9A34-8AB789243ADA}">
+  <dimension ref="C1:W15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>335</v>
+      </c>
+      <c r="N2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I3" t="s">
+        <v>333</v>
+      </c>
+      <c r="J3" t="s">
+        <v>334</v>
+      </c>
+      <c r="K3" t="s">
+        <v>337</v>
+      </c>
+      <c r="L3" t="s">
+        <v>338</v>
+      </c>
+      <c r="M3" t="s">
+        <v>339</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="T3">
+        <v>7</v>
+      </c>
+      <c r="U3">
+        <v>8</v>
+      </c>
+      <c r="V3">
+        <v>9</v>
+      </c>
+      <c r="W3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" s="36">
+        <v>-0.18870000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E5" s="36">
+        <v>0.57339390000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="E6" s="36">
+        <v>-1.032214</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="E7" s="36">
+        <v>0.36380000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E8" s="36">
+        <v>4.1099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D9" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="36">
+        <v>0.49000709999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="36">
+        <v>-0.440552</v>
+      </c>
+    </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D11" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="E11" s="36">
+        <v>0.57040000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E12" s="36">
+        <v>-1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D13" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="E13" s="36">
+        <v>0.29692429999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="41" t="s">
+        <v>341</v>
+      </c>
+      <c r="E14" s="36">
+        <v>-0.3664499</v>
+      </c>
+    </row>
+    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D15" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="E15" s="36">
+        <v>0.47920000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C71D8DF-2DF6-476F-91B9-DD47201B35C2}">
+  <dimension ref="D3:AB30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="G3" s="46" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="35"/>
+      <c r="S3" s="46" t="s">
+        <v>258</v>
+      </c>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+    </row>
+    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F4" s="13"/>
+      <c r="G4" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" t="s">
+        <v>261</v>
+      </c>
+      <c r="I4" s="24">
+        <v>3918</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="O4" s="24">
+        <v>611</v>
+      </c>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="T4" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="U4" s="24">
+        <v>23047018</v>
+      </c>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA4" s="24">
+        <v>2359143</v>
+      </c>
+      <c r="AB4" s="23">
+        <f>AA4/SUM(U4,AA4)</f>
+        <v>9.2857122333437153E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F5" s="24"/>
+      <c r="G5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="K5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="L5" s="24"/>
+      <c r="M5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="O5" s="31"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="U5" s="40"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="41"/>
+    </row>
+    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D6" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" s="47"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+    </row>
+    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D7" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="48"/>
+      <c r="G7">
+        <v>127.98</v>
+      </c>
+      <c r="H7" s="36">
+        <v>18.384840000000001</v>
+      </c>
+      <c r="M7">
+        <v>128.34</v>
+      </c>
+      <c r="N7" s="36">
+        <v>19.25619</v>
+      </c>
+      <c r="S7" s="41">
+        <v>126.923238</v>
+      </c>
+      <c r="T7" s="36">
+        <v>18.110648999999999</v>
+      </c>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41">
+        <v>126.06586059999999</v>
+      </c>
+      <c r="Z7" s="37">
+        <v>18.439636100000001</v>
+      </c>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+    </row>
+    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8">
+        <v>29.6</v>
+      </c>
+      <c r="H8" s="36">
+        <v>5.9282329999999996</v>
+      </c>
+      <c r="M8">
+        <v>30.76</v>
+      </c>
+      <c r="N8" s="36">
+        <v>6.3475760000000001</v>
+      </c>
+      <c r="S8" s="36">
+        <v>29.662302499999999</v>
+      </c>
+      <c r="T8" s="36">
+        <v>5.9267823000000002</v>
+      </c>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41">
+        <v>29.959577500000002</v>
+      </c>
+      <c r="Z8" s="37">
+        <v>6.2308531</v>
+      </c>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+    </row>
+    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D9" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="48"/>
+      <c r="G9">
+        <v>40.1</v>
+      </c>
+      <c r="H9" s="36">
+        <v>5.7592100000000004</v>
+      </c>
+      <c r="M9">
+        <v>40.619999999999997</v>
+      </c>
+      <c r="N9" s="36">
+        <v>5.5369099999999998</v>
+      </c>
+      <c r="S9" s="36">
+        <v>40.103714400000001</v>
+      </c>
+      <c r="T9" s="36">
+        <v>5.8665503000000001</v>
+      </c>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="36">
+        <v>40.107512399999997</v>
+      </c>
+      <c r="Z9" s="37">
+        <v>5.6566346999999997</v>
+      </c>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+    </row>
+    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="S10" s="41"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+    </row>
+    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D11" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="S11" s="41"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+    </row>
+    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="37">
+        <v>70.12</v>
+      </c>
+      <c r="H12" s="37">
+        <v>9.8203709999999997</v>
+      </c>
+      <c r="M12" s="37">
+        <v>65.349999999999994</v>
+      </c>
+      <c r="N12" s="37">
+        <v>8.5174970000000005</v>
+      </c>
+      <c r="S12" s="37">
+        <v>67.901583500000001</v>
+      </c>
+      <c r="T12" s="36">
+        <v>9.2750620000000001</v>
+      </c>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="37">
+        <v>64.861546799999999</v>
+      </c>
+      <c r="Z12" s="37">
+        <v>8.3972078000000003</v>
+      </c>
+      <c r="AA12" s="41"/>
+      <c r="AB12" s="41"/>
+    </row>
+    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D13" s="24"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="37"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
+    </row>
+    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D14" s="24"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+    </row>
+    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D15" s="24"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="41"/>
+      <c r="AB15" s="41"/>
+    </row>
+    <row r="16" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D16" s="47" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" s="47"/>
+      <c r="G16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="M16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="O16" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="S16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="U16" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA16" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB16" s="41"/>
+    </row>
+    <row r="17" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="G17">
+        <f>H17*I4</f>
+        <v>1578.9540000000002</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="M17" s="39">
+        <f>N17*O4</f>
+        <v>267.00700000000001</v>
+      </c>
+      <c r="N17" s="23">
+        <v>0.437</v>
+      </c>
+      <c r="S17" s="50">
+        <f>T17*U4</f>
+        <v>9945516.5527688004</v>
+      </c>
+      <c r="T17" s="26">
+        <v>0.43153160000000002</v>
+      </c>
+      <c r="U17" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="39">
+        <f>Z17*AA4</f>
+        <v>1143629.0127377999</v>
+      </c>
+      <c r="Z17" s="23">
+        <v>0.48476459999999999</v>
+      </c>
+      <c r="AA17" s="41"/>
+      <c r="AB17" s="41"/>
+    </row>
+    <row r="18" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D18" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="G18">
+        <v>3246</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" ref="H18:H30" si="0">G18/$I$4</f>
+        <v>0.82848392036753449</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="M18">
+        <v>187</v>
+      </c>
+      <c r="N18" s="23">
+        <f>M18/$O$4</f>
+        <v>0.30605564648117839</v>
+      </c>
+      <c r="S18" s="50">
+        <v>20959837</v>
+      </c>
+      <c r="T18" s="23">
+        <f>S18/$U$4</f>
+        <v>0.90943813208285773</v>
+      </c>
+      <c r="U18" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41">
+        <v>1054148</v>
+      </c>
+      <c r="Z18" s="49">
+        <f>Y18/$AA$4</f>
+        <v>0.44683514310069378</v>
+      </c>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="41"/>
+    </row>
+    <row r="19" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D19" s="27"/>
+      <c r="E19" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="G19">
+        <v>445</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11357835630423685</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="M19">
+        <v>323</v>
+      </c>
+      <c r="N19" s="23">
+        <f t="shared" ref="N19:N20" si="1">M19/$O$4</f>
+        <v>0.52864157119476274</v>
+      </c>
+      <c r="S19" s="50">
+        <v>1137593</v>
+      </c>
+      <c r="T19" s="23">
+        <f>S19/$U$4</f>
+        <v>4.9359661193478482E-2</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41">
+        <v>877192</v>
+      </c>
+      <c r="Z19" s="23">
+        <f>Y19/$AA$4</f>
+        <v>0.37182654887813077</v>
+      </c>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="41"/>
+    </row>
+    <row r="20" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D20" s="27"/>
+      <c r="E20" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="G20">
+        <v>227</v>
+      </c>
+      <c r="H20" s="23">
+        <f t="shared" si="0"/>
+        <v>5.7937723328228691E-2</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="M20">
+        <v>101</v>
+      </c>
+      <c r="N20" s="23">
+        <f t="shared" si="1"/>
+        <v>0.16530278232405893</v>
+      </c>
+      <c r="S20" s="50">
+        <v>949588</v>
+      </c>
+      <c r="T20" s="23">
+        <f>S20/$U$4</f>
+        <v>4.1202206723663773E-2</v>
+      </c>
+      <c r="U20" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41">
+        <v>427803</v>
+      </c>
+      <c r="Z20" s="23">
+        <f>Y20/$AA$4</f>
+        <v>0.18133830802117548</v>
+      </c>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="41"/>
+    </row>
+    <row r="21" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D21" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>339</v>
+      </c>
+      <c r="H21" s="23">
+        <f t="shared" si="0"/>
+        <v>8.6523736600306281E-2</v>
+      </c>
+      <c r="I21" s="26">
+        <f>SUM($H$21)</f>
+        <v>8.6523736600306281E-2</v>
+      </c>
+      <c r="M21">
+        <v>110</v>
+      </c>
+      <c r="N21" s="23">
+        <f t="shared" ref="N21:N30" si="2">M21/$O$4</f>
+        <v>0.18003273322422259</v>
+      </c>
+      <c r="O21" s="26">
+        <f>N21</f>
+        <v>0.18003273322422259</v>
+      </c>
+      <c r="S21" s="50">
+        <v>1559571</v>
+      </c>
+      <c r="T21" s="23">
+        <f>S21/$U$4</f>
+        <v>6.7669101486361488E-2</v>
+      </c>
+      <c r="U21" s="26">
+        <f>SUM($T$21)</f>
+        <v>6.7669101486361488E-2</v>
+      </c>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41">
+        <v>404485</v>
+      </c>
+      <c r="Z21" s="23">
+        <f>Y21/$AA$4</f>
+        <v>0.17145421027890212</v>
+      </c>
+      <c r="AA21" s="23">
+        <f>Z21</f>
+        <v>0.17145421027890212</v>
+      </c>
+      <c r="AB21" s="41"/>
+    </row>
+    <row r="22" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D22" s="24"/>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>342</v>
+      </c>
+      <c r="H22" s="23">
+        <f t="shared" si="0"/>
+        <v>8.7289433384379791E-2</v>
+      </c>
+      <c r="I22" s="26">
+        <f>SUM($H$21:$H22)</f>
+        <v>0.17381316998468607</v>
+      </c>
+      <c r="M22">
+        <v>92</v>
+      </c>
+      <c r="N22" s="23">
+        <f t="shared" si="2"/>
+        <v>0.15057283142389524</v>
+      </c>
+      <c r="O22" s="26">
+        <f>SUM($N$21:N22)</f>
+        <v>0.33060556464811786</v>
+      </c>
+      <c r="S22" s="50">
+        <v>1461268</v>
+      </c>
+      <c r="T22" s="23">
+        <f>S22/$U$4</f>
+        <v>6.3403777443138201E-2</v>
+      </c>
+      <c r="U22" s="26">
+        <f>SUM($T$21:$T22)</f>
+        <v>0.1310728789294997</v>
+      </c>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41">
+        <v>240757</v>
+      </c>
+      <c r="Z22" s="23">
+        <f>Y22/$AA$4</f>
+        <v>0.10205273694727281</v>
+      </c>
+      <c r="AA22" s="23">
+        <f>SUM($Z$21:Z22)</f>
+        <v>0.27350694722617491</v>
+      </c>
+      <c r="AB22" s="41"/>
+    </row>
+    <row r="23" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D23" s="24"/>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>365</v>
+      </c>
+      <c r="H23" s="23">
+        <f t="shared" si="0"/>
+        <v>9.3159775395610003E-2</v>
+      </c>
+      <c r="I23" s="26">
+        <f>SUM($H$21:$H23)</f>
+        <v>0.26697294538029609</v>
+      </c>
+      <c r="M23">
+        <v>87</v>
+      </c>
+      <c r="N23" s="23">
+        <f t="shared" si="2"/>
+        <v>0.14238952536824878</v>
+      </c>
+      <c r="O23" s="26">
+        <f>SUM($N$21:N23)</f>
+        <v>0.47299509001636664</v>
+      </c>
+      <c r="S23" s="50">
+        <v>2051140</v>
+      </c>
+      <c r="T23" s="23">
+        <f>S23/$U$4</f>
+        <v>8.8998064738787463E-2</v>
+      </c>
+      <c r="U23" s="26">
+        <f>SUM($T$21:$T23)</f>
+        <v>0.22007094366828717</v>
+      </c>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41">
+        <v>339098</v>
+      </c>
+      <c r="Z23" s="23">
+        <f>Y23/$AA$4</f>
+        <v>0.14373778952780733</v>
+      </c>
+      <c r="AA23" s="23">
+        <f>SUM($Z$21:Z23)</f>
+        <v>0.41724473675398221</v>
+      </c>
+      <c r="AB23" s="41"/>
+    </row>
+    <row r="24" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D24" s="24"/>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>368</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" si="0"/>
+        <v>9.3925472179683514E-2</v>
+      </c>
+      <c r="I24" s="26">
+        <f>SUM($H$21:$H24)</f>
+        <v>0.36089841755997959</v>
+      </c>
+      <c r="M24">
+        <v>83</v>
+      </c>
+      <c r="N24" s="23">
+        <f t="shared" si="2"/>
+        <v>0.13584288052373159</v>
+      </c>
+      <c r="O24" s="26">
+        <f>SUM($N$21:N24)</f>
+        <v>0.60883797054009825</v>
+      </c>
+      <c r="S24" s="50">
+        <v>2002854</v>
+      </c>
+      <c r="T24" s="23">
+        <f>S24/$U$4</f>
+        <v>8.6902956382469962E-2</v>
+      </c>
+      <c r="U24" s="26">
+        <f>SUM($T$21:$T24)</f>
+        <v>0.30697390005075714</v>
+      </c>
+      <c r="V24" s="41"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="41">
+        <v>311698</v>
+      </c>
+      <c r="Z24" s="23">
+        <f>Y24/$AA$4</f>
+        <v>0.1321234024389365</v>
+      </c>
+      <c r="AA24" s="23">
+        <f>SUM($Z$21:Z24)</f>
+        <v>0.54936813919291871</v>
+      </c>
+      <c r="AB24" s="41"/>
+    </row>
+    <row r="25" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D25" s="24"/>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>397</v>
+      </c>
+      <c r="H25" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10132720775906075</v>
+      </c>
+      <c r="I25" s="26">
+        <f>SUM($H$21:$H25)</f>
+        <v>0.46222562531904032</v>
+      </c>
+      <c r="M25">
+        <v>61</v>
+      </c>
+      <c r="N25" s="23">
+        <f t="shared" si="2"/>
+        <v>9.9836333878887074E-2</v>
+      </c>
+      <c r="O25" s="26">
+        <f>SUM($N$21:N25)</f>
+        <v>0.70867430441898538</v>
+      </c>
+      <c r="S25" s="50">
+        <v>2308963</v>
+      </c>
+      <c r="T25" s="23">
+        <f>S25/$U$4</f>
+        <v>0.10018489159855735</v>
+      </c>
+      <c r="U25" s="26">
+        <f>SUM($T$21:$T25)</f>
+        <v>0.40715879164931451</v>
+      </c>
+      <c r="V25" s="41"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41">
+        <v>183943</v>
+      </c>
+      <c r="Z25" s="23">
+        <f>Y25/$AA$4</f>
+        <v>7.797026293022509E-2</v>
+      </c>
+      <c r="AA25" s="23">
+        <f>SUM($Z$21:Z25)</f>
+        <v>0.62733840212314385</v>
+      </c>
+      <c r="AB25" s="41"/>
+    </row>
+    <row r="26" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D26" s="24"/>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>412</v>
+      </c>
+      <c r="H26" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10515569167942827</v>
+      </c>
+      <c r="I26" s="26">
+        <f>SUM($H$21:$H26)</f>
+        <v>0.56738131699846861</v>
+      </c>
+      <c r="M26">
+        <v>42</v>
+      </c>
+      <c r="N26" s="23">
+        <f t="shared" si="2"/>
+        <v>6.8739770867430439E-2</v>
+      </c>
+      <c r="O26" s="26">
+        <f>SUM($N$21:N26)</f>
+        <v>0.77741407528641582</v>
+      </c>
+      <c r="S26" s="50">
+        <v>2389812</v>
+      </c>
+      <c r="T26" s="23">
+        <f>S26/$U$4</f>
+        <v>0.10369289423907249</v>
+      </c>
+      <c r="U26" s="26">
+        <f>SUM($T$21:$T26)</f>
+        <v>0.51085168588838703</v>
+      </c>
+      <c r="V26" s="41"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41">
+        <v>153145</v>
+      </c>
+      <c r="Z26" s="23">
+        <f>Y26/$AA$4</f>
+        <v>6.4915522289238081E-2</v>
+      </c>
+      <c r="AA26" s="23">
+        <f>SUM($Z$21:Z26)</f>
+        <v>0.69225392441238198</v>
+      </c>
+      <c r="AB26" s="41"/>
+    </row>
+    <row r="27" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D27" s="24"/>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>414</v>
+      </c>
+      <c r="H27" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10566615620214395</v>
+      </c>
+      <c r="I27" s="26">
+        <f>SUM($H$21:$H27)</f>
+        <v>0.67304747320061253</v>
+      </c>
+      <c r="M27">
+        <v>43</v>
+      </c>
+      <c r="N27" s="23">
+        <f t="shared" si="2"/>
+        <v>7.0376432078559745E-2</v>
+      </c>
+      <c r="O27" s="26">
+        <f>SUM($N$21:N27)</f>
+        <v>0.84779050736497552</v>
+      </c>
+      <c r="S27" s="50">
+        <v>2556546</v>
+      </c>
+      <c r="T27" s="23">
+        <f>S27/$U$4</f>
+        <v>0.11092740935074551</v>
+      </c>
+      <c r="U27" s="26">
+        <f>SUM($T$21:$T27)</f>
+        <v>0.62177909523913255</v>
+      </c>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41">
+        <v>171274</v>
+      </c>
+      <c r="Z27" s="23">
+        <f>Y27/$AA$4</f>
+        <v>7.2600092491213977E-2</v>
+      </c>
+      <c r="AA27" s="23">
+        <f>SUM($Z$21:Z27)</f>
+        <v>0.764854016903596</v>
+      </c>
+      <c r="AB27" s="41"/>
+    </row>
+    <row r="28" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D28" s="24"/>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>426</v>
+      </c>
+      <c r="H28" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10872894333843798</v>
+      </c>
+      <c r="I28" s="26">
+        <f>SUM($H$21:$H28)</f>
+        <v>0.7817764165390505</v>
+      </c>
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="N28" s="23">
+        <f t="shared" si="2"/>
+        <v>4.9099836333878884E-2</v>
+      </c>
+      <c r="O28" s="26">
+        <f>SUM($N$21:N28)</f>
+        <v>0.89689034369885445</v>
+      </c>
+      <c r="S28" s="50">
+        <v>2805331</v>
+      </c>
+      <c r="T28" s="23">
+        <f>S28/$U$4</f>
+        <v>0.12172208135560098</v>
+      </c>
+      <c r="U28" s="26">
+        <f>SUM($T$21:$T28)</f>
+        <v>0.74350117659473347</v>
+      </c>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41">
+        <v>127970</v>
+      </c>
+      <c r="Z28" s="23">
+        <f>Y28/$AA$4</f>
+        <v>5.4244274297912419E-2</v>
+      </c>
+      <c r="AA28" s="23">
+        <f>SUM($Z$21:Z28)</f>
+        <v>0.81909829120150845</v>
+      </c>
+      <c r="AB28" s="41"/>
+    </row>
+    <row r="29" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D29" s="24"/>
+      <c r="E29">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>421</v>
+      </c>
+      <c r="H29" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10745278203164881</v>
+      </c>
+      <c r="I29" s="26">
+        <f>SUM($H$21:$H29)</f>
+        <v>0.88922919857069926</v>
+      </c>
+      <c r="M29">
+        <v>38</v>
+      </c>
+      <c r="N29" s="23">
+        <f t="shared" si="2"/>
+        <v>6.2193126022913256E-2</v>
+      </c>
+      <c r="O29" s="26">
+        <f>SUM($N$21:N29)</f>
+        <v>0.95908346972176772</v>
+      </c>
+      <c r="S29" s="50">
+        <v>2756844</v>
+      </c>
+      <c r="T29" s="23">
+        <f>S29/$U$4</f>
+        <v>0.11961825169746472</v>
+      </c>
+      <c r="U29" s="26">
+        <f>SUM($T$21:$T29)</f>
+        <v>0.86311942829219823</v>
+      </c>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41">
+        <v>274731</v>
+      </c>
+      <c r="Z29" s="23">
+        <f>Y29/$AA$4</f>
+        <v>0.11645372917199169</v>
+      </c>
+      <c r="AA29" s="23">
+        <f>SUM($Z$21:Z29)</f>
+        <v>0.93555202037350016</v>
+      </c>
+      <c r="AB29" s="41"/>
+    </row>
+    <row r="30" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D30" s="24"/>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>434</v>
+      </c>
+      <c r="H30" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11077080142930067</v>
+      </c>
+      <c r="I30" s="26">
+        <f>SUM($H$21:$H30)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="M30">
+        <v>25</v>
+      </c>
+      <c r="N30" s="23">
+        <f t="shared" si="2"/>
+        <v>4.0916530278232409E-2</v>
+      </c>
+      <c r="O30" s="26">
+        <f>SUM($N$21:N30)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="S30" s="50">
+        <v>3154689</v>
+      </c>
+      <c r="T30" s="23">
+        <f>S30/$U$4</f>
+        <v>0.13688057170780185</v>
+      </c>
+      <c r="U30" s="26">
+        <f>SUM($T$21:$T30)</f>
+        <v>1</v>
+      </c>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41">
+        <v>152042</v>
+      </c>
+      <c r="Z30" s="23">
+        <f>Y30/$AA$4</f>
+        <v>6.4447979626499965E-2</v>
+      </c>
+      <c r="AA30" s="23">
+        <f>SUM($Z$21:Z30)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="AB30" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G3:P3"/>
+    <mergeCell ref="S3:AB3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
+  <dimension ref="C2:H13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="97.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>20912</v>
+      </c>
+      <c r="D3">
+        <v>110313247</v>
+      </c>
+      <c r="E3" s="23">
+        <f>D3/$D$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>5551</v>
+      </c>
+      <c r="D4">
+        <v>30222610</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="F4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4">
+        <f>C4-C3</f>
+        <v>-15361</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>C4+G5</f>
+        <v>4197</v>
+      </c>
+      <c r="D5">
+        <v>23381704</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21195735449614678</v>
+      </c>
+      <c r="F5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5">
+        <v>-1354</v>
+      </c>
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4103</v>
+      </c>
+      <c r="D6">
+        <v>23182405</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6">
+        <f>C6-C5</f>
+        <v>-94</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4103</v>
+      </c>
+      <c r="D7">
+        <v>23182405</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4103</v>
+      </c>
+      <c r="D8">
+        <v>23182405</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4073</v>
+      </c>
+      <c r="D9">
+        <v>23012867</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20861381226499479</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4073</v>
+      </c>
+      <c r="D10">
+        <v>22945346</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4059</v>
+      </c>
+      <c r="D11">
+        <v>22945346</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4059</v>
+      </c>
+      <c r="D12">
+        <v>22945346</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4059</v>
+      </c>
+      <c r="D13">
+        <v>22945346</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated some of the tables
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7CA4EE-6DD9-460A-83E8-194BB025BA3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F600BB-C520-4B93-8EA8-03249A0CECB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17685" yWindow="675" windowWidth="21600" windowHeight="10890" firstSheet="3" activeTab="6" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="346">
   <si>
     <t>Variable group</t>
   </si>
@@ -1046,9 +1046,6 @@
     <t>SMOTE</t>
   </si>
   <si>
-    <t xml:space="preserve">N </t>
-  </si>
-  <si>
     <t>$hat{(C)ATE}$</t>
   </si>
   <si>
@@ -1083,6 +1080,21 @@
   </si>
   <si>
     <t>HDPI 89% (l)</t>
+  </si>
+  <si>
+    <t>Cardio-metabolic risk marker</t>
+  </si>
+  <si>
+    <t>Estimatand</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Model 1</t>
+  </si>
+  <si>
+    <t>Model 2</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1105,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="0.0E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1280,7 +1292,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1329,6 +1341,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1336,8 +1352,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -3889,26 +3903,26 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44" t="s">
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="45"/>
-      <c r="I5" s="45" t="s">
+      <c r="G5" s="49"/>
+      <c r="I5" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="J5" s="45"/>
+      <c r="J5" s="49"/>
     </row>
     <row r="6" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
@@ -4595,31 +4609,52 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B6F673-63EF-4D30-A5E9-76FC267124A8}">
-  <dimension ref="C2:L10"/>
+  <dimension ref="C1:V10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>344</v>
+      </c>
+      <c r="N1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="I3" s="46" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="I3" s="50" t="s">
         <v>328</v>
       </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="50" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E4" s="31" t="s">
         <v>323</v>
       </c>
@@ -4639,8 +4674,29 @@
       <c r="K4" s="42" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q4" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="R4" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="U4" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="V4" s="42" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>320</v>
       </c>
@@ -4663,8 +4719,31 @@
       <c r="K5" s="43">
         <v>0.76115809999999995</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="45"/>
+      <c r="O5" s="43" t="s">
+        <v>320</v>
+      </c>
+      <c r="P5" s="43">
+        <v>0.82615720000000004</v>
+      </c>
+      <c r="Q5" s="43">
+        <v>0.82540389999999997</v>
+      </c>
+      <c r="R5" s="43">
+        <v>0.82389570000000001</v>
+      </c>
+      <c r="S5" s="43"/>
+      <c r="T5" s="43">
+        <v>0.81987650000000001</v>
+      </c>
+      <c r="U5" s="43">
+        <v>0.8213857</v>
+      </c>
+      <c r="V5" s="43">
+        <v>0.81876749999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>321</v>
       </c>
@@ -4687,8 +4766,31 @@
       <c r="K6" s="43">
         <v>0.77052699999999996</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="45"/>
+      <c r="O6" s="43" t="s">
+        <v>321</v>
+      </c>
+      <c r="P6" s="43">
+        <v>0.82351560000000001</v>
+      </c>
+      <c r="Q6" s="43">
+        <v>0.82562670000000005</v>
+      </c>
+      <c r="R6" s="43">
+        <v>0.82555909999999999</v>
+      </c>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43">
+        <v>0.82084829999999998</v>
+      </c>
+      <c r="U6" s="43">
+        <v>0.81855599999999995</v>
+      </c>
+      <c r="V6" s="43">
+        <v>0.8229921</v>
+      </c>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>322</v>
       </c>
@@ -4712,17 +4814,42 @@
         <v>0.76413359999999997</v>
       </c>
       <c r="L7" s="43"/>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="45"/>
+      <c r="O7" s="43" t="s">
+        <v>322</v>
+      </c>
+      <c r="P7" s="43">
+        <v>0.82559769999999999</v>
+      </c>
+      <c r="Q7" s="43">
+        <v>0.82505079999999997</v>
+      </c>
+      <c r="R7" s="43">
+        <v>0.82451600000000003</v>
+      </c>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43">
+        <v>0.82250040000000002</v>
+      </c>
+      <c r="U7" s="43">
+        <v>0.81933920000000005</v>
+      </c>
+      <c r="V7" s="43">
+        <v>0.82151149999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
       <c r="J8" s="43"/>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E10" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="I3:K3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="T3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4733,8 +4860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6589B6-0C3E-46EB-9A34-8AB789243ADA}">
   <dimension ref="C1:W15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4745,7 +4872,7 @@
   <sheetData>
     <row r="1" spans="3:23" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="3:23" x14ac:dyDescent="0.25">
@@ -4756,15 +4883,21 @@
         <v>55</v>
       </c>
       <c r="K2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N2" t="s">
         <v>335</v>
       </c>
-      <c r="N2" t="s">
-        <v>336</v>
-      </c>
     </row>
     <row r="3" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>341</v>
+      </c>
       <c r="D3" t="s">
-        <v>329</v>
+        <v>342</v>
+      </c>
+      <c r="E3" t="s">
+        <v>343</v>
       </c>
       <c r="F3" t="s">
         <v>270</v>
@@ -4776,19 +4909,19 @@
         <v>272</v>
       </c>
       <c r="I3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J3" t="s">
         <v>333</v>
       </c>
-      <c r="J3" t="s">
-        <v>334</v>
-      </c>
       <c r="K3" t="s">
+        <v>336</v>
+      </c>
+      <c r="L3" t="s">
         <v>337</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>338</v>
-      </c>
-      <c r="M3" t="s">
-        <v>339</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -4826,7 +4959,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E4" s="36">
         <v>-0.18870000000000001</v>
@@ -4834,7 +4967,7 @@
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E5" s="36">
         <v>0.57339390000000001</v>
@@ -4842,7 +4975,7 @@
     </row>
     <row r="6" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E6" s="36">
         <v>-1.032214</v>
@@ -4850,7 +4983,7 @@
     </row>
     <row r="7" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E7" s="36">
         <v>0.36380000000000001</v>
@@ -4861,7 +4994,7 @@
         <v>164</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E8" s="36">
         <v>4.1099999999999998E-2</v>
@@ -4869,7 +5002,7 @@
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D9" s="25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E9" s="36">
         <v>0.49000709999999997</v>
@@ -4877,7 +5010,7 @@
     </row>
     <row r="10" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E10" s="36">
         <v>-0.440552</v>
@@ -4885,7 +5018,7 @@
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D11" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E11" s="36">
         <v>0.57040000000000002</v>
@@ -4896,7 +5029,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E12" s="36">
         <v>-1.9599999999999999E-2</v>
@@ -4904,7 +5037,7 @@
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D13" s="41" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E13" s="36">
         <v>0.29692429999999997</v>
@@ -4912,7 +5045,7 @@
     </row>
     <row r="14" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E14" s="36">
         <v>-0.3664499</v>
@@ -4920,7 +5053,7 @@
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D15" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E15" s="36">
         <v>0.47920000000000001</v>
@@ -4935,7 +5068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C71D8DF-2DF6-476F-91B9-DD47201B35C2}">
   <dimension ref="D3:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -4949,31 +5082,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="46" t="s">
+      <c r="S3" s="50" t="s">
         <v>258</v>
       </c>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="46"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
@@ -5067,10 +5200,10 @@
       <c r="AB5" s="41"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="51" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="47"/>
+      <c r="E6" s="51"/>
       <c r="S6" s="41"/>
       <c r="T6" s="41"/>
       <c r="U6" s="41"/>
@@ -5083,10 +5216,10 @@
       <c r="AB6" s="41"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="52" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="52"/>
       <c r="G7">
         <v>127.98</v>
       </c>
@@ -5154,10 +5287,10 @@
       <c r="AB8" s="41"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="48"/>
+      <c r="E9" s="52"/>
       <c r="G9">
         <v>40.1</v>
       </c>
@@ -5294,10 +5427,10 @@
       <c r="AB15" s="41"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="E16" s="47"/>
+      <c r="E16" s="51"/>
       <c r="G16" s="33" t="s">
         <v>313</v>
       </c>
@@ -5363,7 +5496,7 @@
       <c r="N17" s="23">
         <v>0.437</v>
       </c>
-      <c r="S17" s="50">
+      <c r="S17" s="47">
         <f>T17*U4</f>
         <v>9945516.5527688004</v>
       </c>
@@ -5410,11 +5543,11 @@
         <f>M18/$O$4</f>
         <v>0.30605564648117839</v>
       </c>
-      <c r="S18" s="50">
+      <c r="S18" s="47">
         <v>20959837</v>
       </c>
       <c r="T18" s="23">
-        <f>S18/$U$4</f>
+        <f t="shared" ref="T18:T30" si="1">S18/$U$4</f>
         <v>0.90943813208285773</v>
       </c>
       <c r="U18" s="23" t="s">
@@ -5426,8 +5559,8 @@
       <c r="Y18" s="41">
         <v>1054148</v>
       </c>
-      <c r="Z18" s="49">
-        <f>Y18/$AA$4</f>
+      <c r="Z18" s="46">
+        <f t="shared" ref="Z18:Z30" si="2">Y18/$AA$4</f>
         <v>0.44683514310069378</v>
       </c>
       <c r="AA18" s="23"/>
@@ -5452,14 +5585,14 @@
         <v>323</v>
       </c>
       <c r="N19" s="23">
-        <f t="shared" ref="N19:N20" si="1">M19/$O$4</f>
+        <f t="shared" ref="N19:N20" si="3">M19/$O$4</f>
         <v>0.52864157119476274</v>
       </c>
-      <c r="S19" s="50">
+      <c r="S19" s="47">
         <v>1137593</v>
       </c>
       <c r="T19" s="23">
-        <f>S19/$U$4</f>
+        <f t="shared" si="1"/>
         <v>4.9359661193478482E-2</v>
       </c>
       <c r="U19" s="23" t="s">
@@ -5472,7 +5605,7 @@
         <v>877192</v>
       </c>
       <c r="Z19" s="23">
-        <f>Y19/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.37182654887813077</v>
       </c>
       <c r="AA19" s="23"/>
@@ -5497,14 +5630,14 @@
         <v>101</v>
       </c>
       <c r="N20" s="23">
+        <f t="shared" si="3"/>
+        <v>0.16530278232405893</v>
+      </c>
+      <c r="S20" s="47">
+        <v>949588</v>
+      </c>
+      <c r="T20" s="23">
         <f t="shared" si="1"/>
-        <v>0.16530278232405893</v>
-      </c>
-      <c r="S20" s="50">
-        <v>949588</v>
-      </c>
-      <c r="T20" s="23">
-        <f>S20/$U$4</f>
         <v>4.1202206723663773E-2</v>
       </c>
       <c r="U20" s="23" t="s">
@@ -5517,7 +5650,7 @@
         <v>427803</v>
       </c>
       <c r="Z20" s="23">
-        <f>Y20/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.18133830802117548</v>
       </c>
       <c r="AA20" s="23"/>
@@ -5545,18 +5678,18 @@
         <v>110</v>
       </c>
       <c r="N21" s="23">
-        <f t="shared" ref="N21:N30" si="2">M21/$O$4</f>
+        <f t="shared" ref="N21:N30" si="4">M21/$O$4</f>
         <v>0.18003273322422259</v>
       </c>
       <c r="O21" s="26">
         <f>N21</f>
         <v>0.18003273322422259</v>
       </c>
-      <c r="S21" s="50">
+      <c r="S21" s="47">
         <v>1559571</v>
       </c>
       <c r="T21" s="23">
-        <f>S21/$U$4</f>
+        <f t="shared" si="1"/>
         <v>6.7669101486361488E-2</v>
       </c>
       <c r="U21" s="26">
@@ -5570,7 +5703,7 @@
         <v>404485</v>
       </c>
       <c r="Z21" s="23">
-        <f>Y21/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.17145421027890212</v>
       </c>
       <c r="AA21" s="23">
@@ -5599,18 +5732,18 @@
         <v>92</v>
       </c>
       <c r="N22" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.15057283142389524</v>
       </c>
       <c r="O22" s="26">
         <f>SUM($N$21:N22)</f>
         <v>0.33060556464811786</v>
       </c>
-      <c r="S22" s="50">
+      <c r="S22" s="47">
         <v>1461268</v>
       </c>
       <c r="T22" s="23">
-        <f>S22/$U$4</f>
+        <f t="shared" si="1"/>
         <v>6.3403777443138201E-2</v>
       </c>
       <c r="U22" s="26">
@@ -5624,7 +5757,7 @@
         <v>240757</v>
       </c>
       <c r="Z22" s="23">
-        <f>Y22/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.10205273694727281</v>
       </c>
       <c r="AA22" s="23">
@@ -5653,18 +5786,18 @@
         <v>87</v>
       </c>
       <c r="N23" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.14238952536824878</v>
       </c>
       <c r="O23" s="26">
         <f>SUM($N$21:N23)</f>
         <v>0.47299509001636664</v>
       </c>
-      <c r="S23" s="50">
+      <c r="S23" s="47">
         <v>2051140</v>
       </c>
       <c r="T23" s="23">
-        <f>S23/$U$4</f>
+        <f t="shared" si="1"/>
         <v>8.8998064738787463E-2</v>
       </c>
       <c r="U23" s="26">
@@ -5678,7 +5811,7 @@
         <v>339098</v>
       </c>
       <c r="Z23" s="23">
-        <f>Y23/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.14373778952780733</v>
       </c>
       <c r="AA23" s="23">
@@ -5707,18 +5840,18 @@
         <v>83</v>
       </c>
       <c r="N24" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.13584288052373159</v>
       </c>
       <c r="O24" s="26">
         <f>SUM($N$21:N24)</f>
         <v>0.60883797054009825</v>
       </c>
-      <c r="S24" s="50">
+      <c r="S24" s="47">
         <v>2002854</v>
       </c>
       <c r="T24" s="23">
-        <f>S24/$U$4</f>
+        <f t="shared" si="1"/>
         <v>8.6902956382469962E-2</v>
       </c>
       <c r="U24" s="26">
@@ -5732,7 +5865,7 @@
         <v>311698</v>
       </c>
       <c r="Z24" s="23">
-        <f>Y24/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.1321234024389365</v>
       </c>
       <c r="AA24" s="23">
@@ -5761,18 +5894,18 @@
         <v>61</v>
       </c>
       <c r="N25" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.9836333878887074E-2</v>
       </c>
       <c r="O25" s="26">
         <f>SUM($N$21:N25)</f>
         <v>0.70867430441898538</v>
       </c>
-      <c r="S25" s="50">
+      <c r="S25" s="47">
         <v>2308963</v>
       </c>
       <c r="T25" s="23">
-        <f>S25/$U$4</f>
+        <f t="shared" si="1"/>
         <v>0.10018489159855735</v>
       </c>
       <c r="U25" s="26">
@@ -5786,7 +5919,7 @@
         <v>183943</v>
       </c>
       <c r="Z25" s="23">
-        <f>Y25/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>7.797026293022509E-2</v>
       </c>
       <c r="AA25" s="23">
@@ -5815,18 +5948,18 @@
         <v>42</v>
       </c>
       <c r="N26" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.8739770867430439E-2</v>
       </c>
       <c r="O26" s="26">
         <f>SUM($N$21:N26)</f>
         <v>0.77741407528641582</v>
       </c>
-      <c r="S26" s="50">
+      <c r="S26" s="47">
         <v>2389812</v>
       </c>
       <c r="T26" s="23">
-        <f>S26/$U$4</f>
+        <f t="shared" si="1"/>
         <v>0.10369289423907249</v>
       </c>
       <c r="U26" s="26">
@@ -5840,7 +5973,7 @@
         <v>153145</v>
       </c>
       <c r="Z26" s="23">
-        <f>Y26/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>6.4915522289238081E-2</v>
       </c>
       <c r="AA26" s="23">
@@ -5869,18 +6002,18 @@
         <v>43</v>
       </c>
       <c r="N27" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.0376432078559745E-2</v>
       </c>
       <c r="O27" s="26">
         <f>SUM($N$21:N27)</f>
         <v>0.84779050736497552</v>
       </c>
-      <c r="S27" s="50">
+      <c r="S27" s="47">
         <v>2556546</v>
       </c>
       <c r="T27" s="23">
-        <f>S27/$U$4</f>
+        <f t="shared" si="1"/>
         <v>0.11092740935074551</v>
       </c>
       <c r="U27" s="26">
@@ -5894,7 +6027,7 @@
         <v>171274</v>
       </c>
       <c r="Z27" s="23">
-        <f>Y27/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>7.2600092491213977E-2</v>
       </c>
       <c r="AA27" s="23">
@@ -5923,18 +6056,18 @@
         <v>30</v>
       </c>
       <c r="N28" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.9099836333878884E-2</v>
       </c>
       <c r="O28" s="26">
         <f>SUM($N$21:N28)</f>
         <v>0.89689034369885445</v>
       </c>
-      <c r="S28" s="50">
+      <c r="S28" s="47">
         <v>2805331</v>
       </c>
       <c r="T28" s="23">
-        <f>S28/$U$4</f>
+        <f t="shared" si="1"/>
         <v>0.12172208135560098</v>
       </c>
       <c r="U28" s="26">
@@ -5948,7 +6081,7 @@
         <v>127970</v>
       </c>
       <c r="Z28" s="23">
-        <f>Y28/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>5.4244274297912419E-2</v>
       </c>
       <c r="AA28" s="23">
@@ -5977,18 +6110,18 @@
         <v>38</v>
       </c>
       <c r="N29" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.2193126022913256E-2</v>
       </c>
       <c r="O29" s="26">
         <f>SUM($N$21:N29)</f>
         <v>0.95908346972176772</v>
       </c>
-      <c r="S29" s="50">
+      <c r="S29" s="47">
         <v>2756844</v>
       </c>
       <c r="T29" s="23">
-        <f>S29/$U$4</f>
+        <f t="shared" si="1"/>
         <v>0.11961825169746472</v>
       </c>
       <c r="U29" s="26">
@@ -6002,7 +6135,7 @@
         <v>274731</v>
       </c>
       <c r="Z29" s="23">
-        <f>Y29/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>0.11645372917199169</v>
       </c>
       <c r="AA29" s="23">
@@ -6031,18 +6164,18 @@
         <v>25</v>
       </c>
       <c r="N30" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.0916530278232409E-2</v>
       </c>
       <c r="O30" s="26">
         <f>SUM($N$21:N30)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S30" s="50">
+      <c r="S30" s="47">
         <v>3154689</v>
       </c>
       <c r="T30" s="23">
-        <f>S30/$U$4</f>
+        <f t="shared" si="1"/>
         <v>0.13688057170780185</v>
       </c>
       <c r="U30" s="26">
@@ -6056,7 +6189,7 @@
         <v>152042</v>
       </c>
       <c r="Z30" s="23">
-        <f>Y30/$AA$4</f>
+        <f t="shared" si="2"/>
         <v>6.4447979626499965E-2</v>
       </c>
       <c r="AA30" s="23">
@@ -6067,12 +6200,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="S3:AB3"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="G3:P3"/>
-    <mergeCell ref="S3:AB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Improved CART visuals and updated some tables
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6477EF3A-35F7-446B-A8AA-CB0F00484DF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BE3A48-59FD-4EB3-8379-BB8743A4B62E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="Text_table_AUCs" sheetId="10" r:id="rId6"/>
     <sheet name="Unweighted results table" sheetId="11" r:id="rId7"/>
     <sheet name="Text_table_sumstats" sheetId="9" r:id="rId8"/>
-    <sheet name="Dataset_2" sheetId="6" r:id="rId9"/>
-    <sheet name="Model_data_2" sheetId="4" r:id="rId10"/>
+    <sheet name="Text_table_sumstats_L" sheetId="12" r:id="rId9"/>
+    <sheet name="Dataset_2" sheetId="6" r:id="rId10"/>
+    <sheet name="Model_data_2" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="347">
   <si>
     <t>Variable group</t>
   </si>
@@ -1096,18 +1097,22 @@
   <si>
     <t>With other forms of disc</t>
   </si>
+  <si>
+    <t>Cardio-metabolic risk markers (change)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="195" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1185,6 +1190,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1292,7 +1304,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1347,6 +1359,11 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="8" fillId="9" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="10" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1357,8 +1374,19 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="8" fillId="9" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="9" fillId="10" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2691,6 +2719,232 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
+  <dimension ref="C2:H13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="97.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>20912</v>
+      </c>
+      <c r="D3">
+        <v>110313247</v>
+      </c>
+      <c r="E3" s="23">
+        <f>D3/$D$3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>5551</v>
+      </c>
+      <c r="D4">
+        <v>30222610</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="F4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4">
+        <f>C4-C3</f>
+        <v>-15361</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>C4+G5</f>
+        <v>4197</v>
+      </c>
+      <c r="D5">
+        <v>23381704</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21195735449614678</v>
+      </c>
+      <c r="F5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5">
+        <v>-1354</v>
+      </c>
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4103</v>
+      </c>
+      <c r="D6">
+        <v>23182405</v>
+      </c>
+      <c r="E6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F6" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6">
+        <f>C6-C5</f>
+        <v>-94</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>4103</v>
+      </c>
+      <c r="D7">
+        <v>23182405</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4103</v>
+      </c>
+      <c r="D8">
+        <v>23182405</v>
+      </c>
+      <c r="E8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4073</v>
+      </c>
+      <c r="D9">
+        <v>23012867</v>
+      </c>
+      <c r="E9" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20861381226499479</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>4073</v>
+      </c>
+      <c r="D10">
+        <v>22945346</v>
+      </c>
+      <c r="E10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4059</v>
+      </c>
+      <c r="D11">
+        <v>22945346</v>
+      </c>
+      <c r="E11" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4059</v>
+      </c>
+      <c r="D12">
+        <v>22945346</v>
+      </c>
+      <c r="E12" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>4059</v>
+      </c>
+      <c r="D13">
+        <v>22945346</v>
+      </c>
+      <c r="E13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2B95C5-E717-4ABB-BAF8-DAA816951EFA}">
   <dimension ref="C2:I49"/>
   <sheetViews>
@@ -3910,26 +4164,26 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="55" t="s">
         <v>244</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50" t="s">
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55" t="s">
         <v>243</v>
       </c>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
     </row>
     <row r="5" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="I5" s="51" t="s">
+      <c r="G5" s="56"/>
+      <c r="I5" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="J5" s="51"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
@@ -4618,7 +4872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B6F673-63EF-4D30-A5E9-76FC267124A8}">
   <dimension ref="C2:S16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="W22" sqref="W22:X22"/>
     </sheetView>
   </sheetViews>
@@ -4628,48 +4882,48 @@
       <c r="C2" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="M2" s="53" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="M2" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="I3" s="52" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="I3" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="M3" s="52" t="s">
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="M3" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
       <c r="P3" s="45"/>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E4" s="31" t="s">
@@ -4853,51 +5107,51 @@
       <c r="E10" s="43"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
       <c r="L11" s="49"/>
-      <c r="M11" s="53" t="s">
+      <c r="M11" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D12" s="49"/>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
       <c r="H12" s="49"/>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="52" t="s">
+      <c r="M12" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
       <c r="P12" s="49"/>
-      <c r="Q12" s="52" t="s">
+      <c r="Q12" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D13" s="49"/>
@@ -4989,7 +5243,7 @@
       <c r="D15" s="49" t="s">
         <v>321</v>
       </c>
-      <c r="E15" s="56">
+      <c r="E15" s="53">
         <v>0.84761169999999997</v>
       </c>
       <c r="F15" s="43">
@@ -5009,7 +5263,7 @@
         <v>0.81318610000000002</v>
       </c>
       <c r="L15" s="43"/>
-      <c r="M15" s="57">
+      <c r="M15" s="54">
         <v>0.84852490000000003</v>
       </c>
       <c r="N15" s="43">
@@ -5025,7 +5279,7 @@
       <c r="R15" s="43">
         <v>0.85248389999999996</v>
       </c>
-      <c r="S15" s="56">
+      <c r="S15" s="53">
         <v>0.85503340000000005</v>
       </c>
     </row>
@@ -5075,18 +5329,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="M11:S11"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="E2:K2"/>
     <mergeCell ref="M2:S2"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="M11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5305,7 +5559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C71D8DF-2DF6-476F-91B9-DD47201B35C2}">
   <dimension ref="D3:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -5319,31 +5573,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="57" t="s">
         <v>253</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="52" t="s">
+      <c r="S3" s="57" t="s">
         <v>258</v>
       </c>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
@@ -5437,10 +5691,10 @@
       <c r="AB5" s="41"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="59" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="54"/>
+      <c r="E6" s="59"/>
       <c r="S6" s="41"/>
       <c r="T6" s="41"/>
       <c r="U6" s="41"/>
@@ -5453,10 +5707,10 @@
       <c r="AB6" s="41"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="60" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="60"/>
       <c r="G7">
         <v>127.98</v>
       </c>
@@ -5524,10 +5778,10 @@
       <c r="AB8" s="41"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="55"/>
+      <c r="E9" s="60"/>
       <c r="G9">
         <v>40.1</v>
       </c>
@@ -5664,10 +5918,10 @@
       <c r="AB15" s="41"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="59" t="s">
         <v>315</v>
       </c>
-      <c r="E16" s="54"/>
+      <c r="E16" s="59"/>
       <c r="G16" s="33" t="s">
         <v>313</v>
       </c>
@@ -6450,226 +6704,1254 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
-  <dimension ref="C2:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F52B84-34FD-493D-A4ED-2F71A840B086}">
+  <dimension ref="D3:AB32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21:U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="97.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="52"/>
+    <col min="4" max="4" width="13.42578125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="52"/>
+    <col min="10" max="10" width="12" style="52" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="9.140625" style="52"/>
+    <col min="19" max="19" width="13.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.140625" style="52"/>
+    <col min="26" max="26" width="14.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>20912</v>
-      </c>
-      <c r="D3">
-        <v>110313247</v>
-      </c>
-      <c r="E3" s="23">
-        <f>D3/$D$3</f>
+    <row r="3" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="G3" s="57" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="35"/>
+      <c r="S3" s="57" t="s">
+        <v>258</v>
+      </c>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+    </row>
+    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F4" s="13"/>
+      <c r="G4" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="I4" s="11">
+        <v>3521</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="O4" s="11">
+        <v>536</v>
+      </c>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="T4" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="U4" s="11">
+        <v>20856866</v>
+      </c>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA4" s="11">
+        <v>2088210</v>
+      </c>
+      <c r="AB4" s="23">
+        <f>AA4/SUM(U4,AA4)</f>
+        <v>9.1009068786697414E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F5" s="24"/>
+      <c r="G5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="50"/>
+      <c r="K5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="L5" s="24"/>
+      <c r="M5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="O5" s="50"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="U5" s="50"/>
+      <c r="W5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA5" s="50"/>
+    </row>
+    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D6" s="59" t="s">
+        <v>346</v>
+      </c>
+      <c r="E6" s="59"/>
+    </row>
+    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D7" s="60" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="G7" s="73">
+        <v>-0.13370000000000001</v>
+      </c>
+      <c r="H7" s="68">
+        <v>18.590910000000001</v>
+      </c>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="73">
+        <v>-0.31540000000000001</v>
+      </c>
+      <c r="N7" s="68">
+        <v>19.523710000000001</v>
+      </c>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="73">
+        <v>0.52728123199999999</v>
+      </c>
+      <c r="T7" s="68">
+        <v>17.906265770000001</v>
+      </c>
+      <c r="U7" s="61"/>
+      <c r="V7" s="61"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="73">
+        <v>-9.7058546999999995E-2</v>
+      </c>
+      <c r="Z7" s="68">
+        <v>17.747307200000002</v>
+      </c>
+      <c r="AA7" s="61"/>
+      <c r="AB7" s="61"/>
+    </row>
+    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D8" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="73">
+        <v>-0.10290000000000001</v>
+      </c>
+      <c r="H8" s="68">
+        <v>2.9492189999999998</v>
+      </c>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="73">
+        <v>-1.9890000000000001E-2</v>
+      </c>
+      <c r="N8" s="68">
+        <v>3.2508530000000002</v>
+      </c>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="73">
+        <v>-9.6131410000000004E-3</v>
+      </c>
+      <c r="T8" s="68">
+        <v>2.9238787999999998</v>
+      </c>
+      <c r="U8" s="61"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="61"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="73">
+        <v>-5.0169170999999999E-2</v>
+      </c>
+      <c r="Z8" s="68">
+        <v>2.7173759</v>
+      </c>
+      <c r="AA8" s="61"/>
+      <c r="AB8" s="61"/>
+    </row>
+    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D9" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="60"/>
+      <c r="G9" s="73">
+        <v>0.46750000000000003</v>
+      </c>
+      <c r="H9" s="68">
+        <v>3.121013</v>
+      </c>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="73">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="N9" s="68">
+        <v>2.9945520000000001</v>
+      </c>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="73">
+        <v>0.62268060999999997</v>
+      </c>
+      <c r="T9" s="68">
+        <v>3.1024815000000001</v>
+      </c>
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="73">
+        <v>2.0048094799999999E-2</v>
+      </c>
+      <c r="Z9" s="68">
+        <v>2.7435390000000002</v>
+      </c>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61"/>
+    </row>
+    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="61"/>
+      <c r="S10" s="61"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="61"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="61"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="61"/>
+      <c r="Z10" s="63"/>
+      <c r="AA10" s="61"/>
+      <c r="AB10" s="61"/>
+    </row>
+    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D11" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="61"/>
+      <c r="V11" s="61"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="61"/>
+      <c r="Z11" s="63"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="61"/>
+    </row>
+    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="64">
+        <v>70.23</v>
+      </c>
+      <c r="H12" s="64">
+        <v>9.7927110000000006</v>
+      </c>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="64">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="N12" s="64">
+        <v>8.4884939999999993</v>
+      </c>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="64">
+        <v>67.976400960999996</v>
+      </c>
+      <c r="T12" s="64">
+        <v>9.2971120000000003</v>
+      </c>
+      <c r="U12" s="61"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="64">
+        <v>64.862389569000001</v>
+      </c>
+      <c r="Z12" s="64">
+        <v>8.3990585000000006</v>
+      </c>
+      <c r="AA12" s="61"/>
+      <c r="AB12" s="61"/>
+    </row>
+    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D13" s="24"/>
+      <c r="H13" s="11"/>
+      <c r="T13" s="36"/>
+      <c r="Z13" s="37"/>
+    </row>
+    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D15" s="24"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+    </row>
+    <row r="16" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D16" s="59" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" s="59"/>
+      <c r="G16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="M16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="O16" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="S16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="U16" s="50" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA16" s="38" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="G17" s="67">
+        <f>H17*I4</f>
+        <v>1435.8638000000001</v>
+      </c>
+      <c r="H17" s="65">
+        <v>0.4078</v>
+      </c>
+      <c r="I17" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="67">
+        <f>N17*O4</f>
+        <v>232.14159999999998</v>
+      </c>
+      <c r="N17" s="66">
+        <v>0.43309999999999998</v>
+      </c>
+      <c r="O17" s="61"/>
+      <c r="P17" s="61"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61"/>
+      <c r="S17" s="69">
+        <f>T17*U4</f>
+        <v>9103604.9968211949</v>
+      </c>
+      <c r="T17" s="65">
+        <v>0.43648000599999998</v>
+      </c>
+      <c r="U17" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="V17" s="61"/>
+      <c r="W17" s="61"/>
+      <c r="X17" s="61"/>
+      <c r="Y17" s="67">
+        <f>Z17*AA4</f>
+        <v>1017229.47418554</v>
+      </c>
+      <c r="Z17" s="66">
+        <v>0.48712987400000002</v>
+      </c>
+      <c r="AA17" s="65" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D18" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="G18" s="11">
+        <v>2939</v>
+      </c>
+      <c r="H18" s="66">
+        <f t="shared" ref="H18:H30" si="0">G18/$I$4</f>
+        <v>0.83470604941777904</v>
+      </c>
+      <c r="I18" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="11">
+        <v>173</v>
+      </c>
+      <c r="N18" s="66">
+        <f>M18/$O$4</f>
+        <v>0.32276119402985076</v>
+      </c>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="69">
+        <v>19069752</v>
+      </c>
+      <c r="T18" s="66">
+        <f t="shared" ref="T18:T30" si="1">S18/$U$4</f>
+        <v>0.91431531467862914</v>
+      </c>
+      <c r="U18" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="11">
+        <v>974813</v>
+      </c>
+      <c r="Z18" s="70">
+        <f t="shared" ref="Z18:Z30" si="2">Y18/$AA$4</f>
+        <v>0.46681751356424883</v>
+      </c>
+      <c r="AA18" s="66" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D19" s="51"/>
+      <c r="E19" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="G19" s="11">
+        <v>387</v>
+      </c>
+      <c r="H19" s="66">
+        <f t="shared" si="0"/>
+        <v>0.1099119568304459</v>
+      </c>
+      <c r="I19" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="11">
+        <v>277</v>
+      </c>
+      <c r="N19" s="66">
+        <f t="shared" ref="N19:N30" si="3">M19/$O$4</f>
+        <v>0.51679104477611937</v>
+      </c>
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="69">
+        <v>958019</v>
+      </c>
+      <c r="T19" s="66">
+        <f t="shared" si="1"/>
+        <v>4.5933027521968067E-2</v>
+      </c>
+      <c r="U19" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="V19" s="61"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
+      <c r="Y19" s="11">
+        <v>743978</v>
+      </c>
+      <c r="Z19" s="66">
+        <f t="shared" si="2"/>
+        <v>0.35627547037893698</v>
+      </c>
+      <c r="AA19" s="66" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D20" s="51"/>
+      <c r="E20" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="G20" s="11">
+        <v>195</v>
+      </c>
+      <c r="H20" s="66">
+        <f t="shared" si="0"/>
+        <v>5.5381993751775063E-2</v>
+      </c>
+      <c r="I20" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="11">
+        <v>88</v>
+      </c>
+      <c r="N20" s="66">
+        <f t="shared" si="3"/>
+        <v>0.16417910447761194</v>
+      </c>
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="69">
+        <v>829095</v>
+      </c>
+      <c r="T20" s="66">
+        <f t="shared" si="1"/>
+        <v>3.9751657799402845E-2</v>
+      </c>
+      <c r="U20" s="66" t="s">
+        <v>317</v>
+      </c>
+      <c r="V20" s="61"/>
+      <c r="W20" s="61"/>
+      <c r="X20" s="61"/>
+      <c r="Y20" s="11">
+        <v>369689</v>
+      </c>
+      <c r="Z20" s="66">
+        <f t="shared" si="2"/>
+        <v>0.1770363133975989</v>
+      </c>
+      <c r="AA20" s="66" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D21" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" s="52">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>5551</v>
-      </c>
-      <c r="D4">
-        <v>30222610</v>
-      </c>
-      <c r="E4" s="23">
-        <f t="shared" ref="E4:E13" si="0">D4/$D$3</f>
-        <v>0.27397081331492307</v>
-      </c>
-      <c r="F4" t="s">
-        <v>209</v>
-      </c>
-      <c r="G4">
-        <f>C4-C3</f>
-        <v>-15361</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <f>C4+G5</f>
-        <v>4197</v>
-      </c>
-      <c r="D5">
-        <v>23381704</v>
-      </c>
-      <c r="E5" s="23">
+      <c r="G21" s="11">
+        <v>298</v>
+      </c>
+      <c r="H21" s="66">
         <f t="shared" si="0"/>
-        <v>0.21195735449614678</v>
-      </c>
-      <c r="F5" t="s">
-        <v>210</v>
-      </c>
-      <c r="G5">
-        <v>-1354</v>
-      </c>
-      <c r="H5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>4103</v>
-      </c>
-      <c r="D6">
-        <v>23182405</v>
-      </c>
-      <c r="E6" s="23">
+        <v>8.4635046861687019E-2</v>
+      </c>
+      <c r="I21" s="65">
+        <f>SUM($H$21)</f>
+        <v>8.4635046861687019E-2</v>
+      </c>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="11">
+        <v>91</v>
+      </c>
+      <c r="N21" s="66">
+        <f t="shared" si="3"/>
+        <v>0.16977611940298507</v>
+      </c>
+      <c r="O21" s="65">
+        <f>N21</f>
+        <v>0.16977611940298507</v>
+      </c>
+      <c r="P21" s="61"/>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="61"/>
+      <c r="S21" s="69">
+        <v>1367144</v>
+      </c>
+      <c r="T21" s="66">
+        <f t="shared" si="1"/>
+        <v>6.5548870093905767E-2</v>
+      </c>
+      <c r="U21" s="65">
+        <f>SUM($T$21)</f>
+        <v>6.5548870093905767E-2</v>
+      </c>
+      <c r="V21" s="61"/>
+      <c r="W21" s="61"/>
+      <c r="X21" s="61"/>
+      <c r="Y21" s="11">
+        <v>341824</v>
+      </c>
+      <c r="Z21" s="66">
+        <f t="shared" si="2"/>
+        <v>0.16369234894957882</v>
+      </c>
+      <c r="AA21" s="66">
+        <f>Z21</f>
+        <v>0.16369234894957882</v>
+      </c>
+    </row>
+    <row r="22" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D22" s="24"/>
+      <c r="E22" s="52">
+        <v>2</v>
+      </c>
+      <c r="G22" s="11">
+        <v>284</v>
+      </c>
+      <c r="H22" s="66">
         <f t="shared" si="0"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="F6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G6">
-        <f>C6-C5</f>
-        <v>-94</v>
-      </c>
-      <c r="H6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>4103</v>
-      </c>
-      <c r="D7">
-        <v>23182405</v>
-      </c>
-      <c r="E7" s="23">
+        <v>8.0658903720533942E-2</v>
+      </c>
+      <c r="I22" s="65">
+        <f>SUM($H$21:$H22)</f>
+        <v>0.16529395058222096</v>
+      </c>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="11">
+        <v>81</v>
+      </c>
+      <c r="N22" s="66">
+        <f t="shared" si="3"/>
+        <v>0.15111940298507462</v>
+      </c>
+      <c r="O22" s="65">
+        <f>SUM($N$21:N22)</f>
+        <v>0.32089552238805968</v>
+      </c>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="61"/>
+      <c r="R22" s="61"/>
+      <c r="S22" s="69">
+        <v>1205251</v>
+      </c>
+      <c r="T22" s="66">
+        <f t="shared" si="1"/>
+        <v>5.778677390936874E-2</v>
+      </c>
+      <c r="U22" s="65">
+        <f>SUM($T$21:$T22)</f>
+        <v>0.12333564400327451</v>
+      </c>
+      <c r="V22" s="61"/>
+      <c r="W22" s="61"/>
+      <c r="X22" s="61"/>
+      <c r="Y22" s="11">
+        <v>225332</v>
+      </c>
+      <c r="Z22" s="66">
+        <f t="shared" si="2"/>
+        <v>0.10790677182850383</v>
+      </c>
+      <c r="AA22" s="66">
+        <f>SUM($Z$21:Z22)</f>
+        <v>0.27159912077808268</v>
+      </c>
+    </row>
+    <row r="23" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D23" s="24"/>
+      <c r="E23" s="52">
+        <v>3</v>
+      </c>
+      <c r="G23" s="11">
+        <v>310</v>
+      </c>
+      <c r="H23" s="66">
         <f t="shared" si="0"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="F7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>4103</v>
-      </c>
-      <c r="D8">
-        <v>23182405</v>
-      </c>
-      <c r="E8" s="23">
+        <v>8.8043169554103948E-2</v>
+      </c>
+      <c r="I23" s="65">
+        <f>SUM($H$21:$H23)</f>
+        <v>0.25333712013632492</v>
+      </c>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="11">
+        <v>80</v>
+      </c>
+      <c r="N23" s="66">
+        <f t="shared" si="3"/>
+        <v>0.14925373134328357</v>
+      </c>
+      <c r="O23" s="65">
+        <f>SUM($N$21:N23)</f>
+        <v>0.47014925373134325</v>
+      </c>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="61"/>
+      <c r="S23" s="69">
+        <v>1791053</v>
+      </c>
+      <c r="T23" s="66">
+        <f t="shared" si="1"/>
+        <v>8.5873543992659299E-2</v>
+      </c>
+      <c r="U23" s="65">
+        <f>SUM($T$21:$T23)</f>
+        <v>0.2092091879959338</v>
+      </c>
+      <c r="V23" s="61"/>
+      <c r="W23" s="61"/>
+      <c r="X23" s="61"/>
+      <c r="Y23" s="11">
+        <v>319647</v>
+      </c>
+      <c r="Z23" s="66">
+        <f t="shared" si="2"/>
+        <v>0.15307224848075623</v>
+      </c>
+      <c r="AA23" s="66">
+        <f>SUM($Z$21:Z23)</f>
+        <v>0.42467136925883892</v>
+      </c>
+    </row>
+    <row r="24" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D24" s="24"/>
+      <c r="E24" s="52">
+        <v>4</v>
+      </c>
+      <c r="G24" s="11">
+        <v>335</v>
+      </c>
+      <c r="H24" s="66">
         <f t="shared" si="0"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="F8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>4073</v>
-      </c>
-      <c r="D9">
-        <v>23012867</v>
-      </c>
-      <c r="E9" s="23">
+        <v>9.5143425163305873E-2</v>
+      </c>
+      <c r="I24" s="65">
+        <f>SUM($H$21:$H24)</f>
+        <v>0.3484805452996308</v>
+      </c>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="11">
+        <v>71</v>
+      </c>
+      <c r="N24" s="66">
+        <f t="shared" si="3"/>
+        <v>0.13246268656716417</v>
+      </c>
+      <c r="O24" s="65">
+        <f>SUM($N$21:N24)</f>
+        <v>0.6026119402985074</v>
+      </c>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="69">
+        <v>1799998</v>
+      </c>
+      <c r="T24" s="66">
+        <f t="shared" si="1"/>
+        <v>8.6302419548555373E-2</v>
+      </c>
+      <c r="U24" s="65">
+        <f>SUM($T$21:$T24)</f>
+        <v>0.29551160754448919</v>
+      </c>
+      <c r="V24" s="61"/>
+      <c r="W24" s="61"/>
+      <c r="X24" s="61"/>
+      <c r="Y24" s="11">
+        <v>265664</v>
+      </c>
+      <c r="Z24" s="66">
+        <f t="shared" si="2"/>
+        <v>0.12722092126749704</v>
+      </c>
+      <c r="AA24" s="66">
+        <f>SUM($Z$21:Z24)</f>
+        <v>0.55189229052633593</v>
+      </c>
+    </row>
+    <row r="25" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D25" s="24"/>
+      <c r="E25" s="52">
+        <v>5</v>
+      </c>
+      <c r="G25" s="11">
+        <v>360</v>
+      </c>
+      <c r="H25" s="66">
         <f t="shared" si="0"/>
-        <v>0.20861381226499479</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>4073</v>
-      </c>
-      <c r="D10">
-        <v>22945346</v>
-      </c>
-      <c r="E10" s="23">
+        <v>0.10224368077250781</v>
+      </c>
+      <c r="I25" s="65">
+        <f>SUM($H$21:$H25)</f>
+        <v>0.45072422607213858</v>
+      </c>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="11">
+        <v>56</v>
+      </c>
+      <c r="N25" s="66">
+        <f t="shared" si="3"/>
+        <v>0.1044776119402985</v>
+      </c>
+      <c r="O25" s="65">
+        <f>SUM($N$21:N25)</f>
+        <v>0.70708955223880587</v>
+      </c>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="61"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="69">
+        <v>2093126</v>
+      </c>
+      <c r="T25" s="66">
+        <f t="shared" si="1"/>
+        <v>0.10035668829631451</v>
+      </c>
+      <c r="U25" s="65">
+        <f>SUM($T$21:$T25)</f>
+        <v>0.39586829584080369</v>
+      </c>
+      <c r="V25" s="61"/>
+      <c r="W25" s="61"/>
+      <c r="X25" s="61"/>
+      <c r="Y25" s="11">
+        <v>152178</v>
+      </c>
+      <c r="Z25" s="66">
+        <f t="shared" si="2"/>
+        <v>7.2874854540491613E-2</v>
+      </c>
+      <c r="AA25" s="66">
+        <f>SUM($Z$21:Z25)</f>
+        <v>0.62476714506682751</v>
+      </c>
+    </row>
+    <row r="26" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D26" s="24"/>
+      <c r="E26" s="52">
+        <v>6</v>
+      </c>
+      <c r="G26" s="11">
+        <v>377</v>
+      </c>
+      <c r="H26" s="66">
         <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>4059</v>
-      </c>
-      <c r="D11">
-        <v>22945346</v>
-      </c>
-      <c r="E11" s="23">
+        <v>0.10707185458676512</v>
+      </c>
+      <c r="I26" s="65">
+        <f>SUM($H$21:$H26)</f>
+        <v>0.55779608065890374</v>
+      </c>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="11">
+        <v>38</v>
+      </c>
+      <c r="N26" s="66">
+        <f t="shared" si="3"/>
+        <v>7.0895522388059698E-2</v>
+      </c>
+      <c r="O26" s="65">
+        <f>SUM($N$21:N26)</f>
+        <v>0.77798507462686561</v>
+      </c>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="61"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="69">
+        <v>2227717</v>
+      </c>
+      <c r="T26" s="66">
+        <f t="shared" si="1"/>
+        <v>0.10680976710499075</v>
+      </c>
+      <c r="U26" s="65">
+        <f>SUM($T$21:$T26)</f>
+        <v>0.50267806294579442</v>
+      </c>
+      <c r="V26" s="61"/>
+      <c r="W26" s="61"/>
+      <c r="X26" s="61"/>
+      <c r="Y26" s="11">
+        <v>147308</v>
+      </c>
+      <c r="Z26" s="66">
+        <f t="shared" si="2"/>
+        <v>7.0542713615967742E-2</v>
+      </c>
+      <c r="AA26" s="66">
+        <f>SUM($Z$21:Z26)</f>
+        <v>0.69530985868279527</v>
+      </c>
+    </row>
+    <row r="27" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D27" s="24"/>
+      <c r="E27" s="52">
+        <v>7</v>
+      </c>
+      <c r="G27" s="11">
+        <v>383</v>
+      </c>
+      <c r="H27" s="66">
         <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>4059</v>
-      </c>
-      <c r="D12">
-        <v>22945346</v>
-      </c>
-      <c r="E12" s="23">
+        <v>0.10877591593297359</v>
+      </c>
+      <c r="I27" s="65">
+        <f>SUM($H$21:$H27)</f>
+        <v>0.66657199659187727</v>
+      </c>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="11">
+        <v>36</v>
+      </c>
+      <c r="N27" s="66">
+        <f t="shared" si="3"/>
+        <v>6.7164179104477612E-2</v>
+      </c>
+      <c r="O27" s="65">
+        <f>SUM($N$21:N27)</f>
+        <v>0.8451492537313432</v>
+      </c>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="69">
+        <v>2380952</v>
+      </c>
+      <c r="T27" s="66">
+        <f t="shared" si="1"/>
+        <v>0.11415674819026023</v>
+      </c>
+      <c r="U27" s="65">
+        <f>SUM($T$21:$T27)</f>
+        <v>0.61683481113605465</v>
+      </c>
+      <c r="V27" s="61"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="61"/>
+      <c r="Y27" s="11">
+        <v>145770</v>
+      </c>
+      <c r="Z27" s="66">
+        <f t="shared" si="2"/>
+        <v>6.9806197652534943E-2</v>
+      </c>
+      <c r="AA27" s="66">
+        <f>SUM($Z$21:Z27)</f>
+        <v>0.7651160563353302</v>
+      </c>
+    </row>
+    <row r="28" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D28" s="24"/>
+      <c r="E28" s="52">
+        <v>8</v>
+      </c>
+      <c r="G28" s="11">
+        <v>388</v>
+      </c>
+      <c r="H28" s="66">
         <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>4059</v>
-      </c>
-      <c r="D13">
-        <v>22945346</v>
-      </c>
-      <c r="E13" s="23">
+        <v>0.11019596705481398</v>
+      </c>
+      <c r="I28" s="65">
+        <f>SUM($H$21:$H28)</f>
+        <v>0.77676796364669121</v>
+      </c>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="11">
+        <v>24</v>
+      </c>
+      <c r="N28" s="66">
+        <f t="shared" si="3"/>
+        <v>4.4776119402985072E-2</v>
+      </c>
+      <c r="O28" s="65">
+        <f>SUM($N$21:N28)</f>
+        <v>0.88992537313432829</v>
+      </c>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="61"/>
+      <c r="R28" s="61"/>
+      <c r="S28" s="69">
+        <v>2592761</v>
+      </c>
+      <c r="T28" s="66">
+        <f t="shared" si="1"/>
+        <v>0.12431210901963891</v>
+      </c>
+      <c r="U28" s="65">
+        <f>SUM($T$21:$T28)</f>
+        <v>0.7411469201556935</v>
+      </c>
+      <c r="V28" s="61"/>
+      <c r="W28" s="61"/>
+      <c r="X28" s="61"/>
+      <c r="Y28" s="11">
+        <v>92991</v>
+      </c>
+      <c r="Z28" s="66">
+        <f t="shared" si="2"/>
+        <v>4.4531440803367475E-2</v>
+      </c>
+      <c r="AA28" s="66">
+        <f>SUM($Z$21:Z28)</f>
+        <v>0.80964749713869766</v>
+      </c>
+    </row>
+    <row r="29" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D29" s="24"/>
+      <c r="E29" s="52">
+        <v>9</v>
+      </c>
+      <c r="G29" s="11">
+        <v>388</v>
+      </c>
+      <c r="H29" s="66">
         <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="F13" t="s">
-        <v>236</v>
-      </c>
+        <v>0.11019596705481398</v>
+      </c>
+      <c r="I29" s="65">
+        <f>SUM($H$21:$H29)</f>
+        <v>0.88696393070150514</v>
+      </c>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="11">
+        <v>36</v>
+      </c>
+      <c r="N29" s="66">
+        <f t="shared" si="3"/>
+        <v>6.7164179104477612E-2</v>
+      </c>
+      <c r="O29" s="65">
+        <f>SUM($N$21:N29)</f>
+        <v>0.95708955223880587</v>
+      </c>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="61"/>
+      <c r="S29" s="69">
+        <v>2538282</v>
+      </c>
+      <c r="T29" s="66">
+        <f t="shared" si="1"/>
+        <v>0.12170006749815625</v>
+      </c>
+      <c r="U29" s="65">
+        <f>SUM($T$21:$T29)</f>
+        <v>0.86284698765384971</v>
+      </c>
+      <c r="V29" s="61"/>
+      <c r="W29" s="61"/>
+      <c r="X29" s="61"/>
+      <c r="Y29" s="11">
+        <v>258692</v>
+      </c>
+      <c r="Z29" s="66">
+        <f t="shared" si="2"/>
+        <v>0.12388217660101235</v>
+      </c>
+      <c r="AA29" s="66">
+        <f>SUM($Z$21:Z29)</f>
+        <v>0.93352967373970996</v>
+      </c>
+    </row>
+    <row r="30" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="D30" s="24"/>
+      <c r="E30" s="52">
+        <v>10</v>
+      </c>
+      <c r="G30" s="11">
+        <v>398</v>
+      </c>
+      <c r="H30" s="66">
+        <f t="shared" si="0"/>
+        <v>0.11303606929849475</v>
+      </c>
+      <c r="I30" s="65">
+        <f>SUM($H$21:$H30)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="11">
+        <v>23</v>
+      </c>
+      <c r="N30" s="66">
+        <f t="shared" si="3"/>
+        <v>4.2910447761194029E-2</v>
+      </c>
+      <c r="O30" s="65">
+        <f>SUM($N$21:N30)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="61"/>
+      <c r="S30" s="69">
+        <v>2860582</v>
+      </c>
+      <c r="T30" s="66">
+        <f t="shared" si="1"/>
+        <v>0.13715301234615018</v>
+      </c>
+      <c r="U30" s="65">
+        <f>SUM($T$21:$T30)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="V30" s="61"/>
+      <c r="W30" s="61"/>
+      <c r="X30" s="61"/>
+      <c r="Y30" s="11">
+        <v>138804</v>
+      </c>
+      <c r="Z30" s="66">
+        <f t="shared" si="2"/>
+        <v>6.6470326260289911E-2</v>
+      </c>
+      <c r="AA30" s="66">
+        <f>SUM($Z$21:Z30)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="32" spans="4:27" x14ac:dyDescent="0.25">
+      <c r="S32" s="72"/>
+      <c r="Z32" s="71"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="G3:P3"/>
+    <mergeCell ref="S3:AB3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Discussion tables code gripstrength doctorvisits
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C6F5DC-7628-41F4-AC29-09E9C1C99C8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2090B-1BA1-416B-8EEE-C60D75C64070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="0" yWindow="570" windowWidth="24480" windowHeight="10080" activeTab="4" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
-    <sheet name="Model_data_1" sheetId="2" r:id="rId2"/>
-    <sheet name="Dataset_1" sheetId="5" r:id="rId3"/>
-    <sheet name="Text_table_sample_cons" sheetId="7" r:id="rId4"/>
-    <sheet name="Table_summary_stats" sheetId="8" r:id="rId5"/>
-    <sheet name="Text_table_AUCs" sheetId="10" r:id="rId6"/>
-    <sheet name="Tables_quantiles" sheetId="13" r:id="rId7"/>
-    <sheet name="Unweighted results table" sheetId="11" r:id="rId8"/>
-    <sheet name="Text_table_sumstats" sheetId="9" r:id="rId9"/>
-    <sheet name="Text_table_sumstats_L" sheetId="12" r:id="rId10"/>
-    <sheet name="Dataset_2" sheetId="6" r:id="rId11"/>
-    <sheet name="Model_data_2" sheetId="4" r:id="rId12"/>
+    <sheet name="Random seeds" sheetId="14" r:id="rId2"/>
+    <sheet name="Model_data_1" sheetId="2" r:id="rId3"/>
+    <sheet name="Dataset_1" sheetId="5" r:id="rId4"/>
+    <sheet name="Discussion_table" sheetId="15" r:id="rId5"/>
+    <sheet name="Text_table_sample_cons" sheetId="7" r:id="rId6"/>
+    <sheet name="Table_summary_stats" sheetId="8" r:id="rId7"/>
+    <sheet name="Text_table_AUCs" sheetId="10" r:id="rId8"/>
+    <sheet name="Tables_quantiles" sheetId="13" r:id="rId9"/>
+    <sheet name="Unweighted results table" sheetId="11" r:id="rId10"/>
+    <sheet name="Text_table_sumstats" sheetId="9" r:id="rId11"/>
+    <sheet name="Text_table_sumstats_L" sheetId="12" r:id="rId12"/>
+    <sheet name="Dataset_2" sheetId="6" r:id="rId13"/>
+    <sheet name="Model_data_2" sheetId="4" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="370">
   <si>
     <t>Variable group</t>
   </si>
@@ -1130,6 +1132,45 @@
   </si>
   <si>
     <t>Share (\%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Seeds were manually changed each iterations. Starting with both seeds at 30121997 for the first run, then 13022021 to 31022021 for the other 18. </t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Batch number</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Cross sectional</t>
+  </si>
+  <si>
+    <t>Longitudinal</t>
+  </si>
+  <si>
+    <t>Times seen doctor</t>
+  </si>
+  <si>
+    <t>Dominant hand grip strength</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>S.d.</t>
+  </si>
+  <si>
+    <t>White/caucasian</t>
+  </si>
+  <si>
+    <t>Black/african american</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1387,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1423,6 +1464,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1432,17 +1481,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1764,7 +1807,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H39" sqref="C2:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2775,6 +2818,1362 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6589B6-0C3E-46EB-9A34-8AB789243ADA}">
+  <dimension ref="C1:W15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E3" t="s">
+        <v>343</v>
+      </c>
+      <c r="F3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H3" t="s">
+        <v>272</v>
+      </c>
+      <c r="I3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J3" t="s">
+        <v>333</v>
+      </c>
+      <c r="K3" t="s">
+        <v>336</v>
+      </c>
+      <c r="L3" t="s">
+        <v>337</v>
+      </c>
+      <c r="M3" t="s">
+        <v>338</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="T3">
+        <v>7</v>
+      </c>
+      <c r="U3">
+        <v>8</v>
+      </c>
+      <c r="V3">
+        <v>9</v>
+      </c>
+      <c r="W3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="E4" s="36">
+        <v>-0.18870000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E5" s="36">
+        <v>0.57339390000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="E6" s="36">
+        <v>-1.032214</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E7" s="36">
+        <v>0.36380000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="E8" s="36">
+        <v>4.1099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D9" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="E9" s="36">
+        <v>0.49000709999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="E10" s="36">
+        <v>-0.440552</v>
+      </c>
+    </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D11" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E11" s="36">
+        <v>0.57040000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="E12" s="36">
+        <v>-1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D13" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="E13" s="36">
+        <v>0.29692429999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="E14" s="36">
+        <v>-0.3664499</v>
+      </c>
+    </row>
+    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="D15" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E15" s="36">
+        <v>0.47920000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C71D8DF-2DF6-476F-91B9-DD47201B35C2}">
+  <dimension ref="D3:AB30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O30" sqref="D2:P30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="G3" s="82" t="s">
+        <v>253</v>
+      </c>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="35"/>
+      <c r="S3" s="82" t="s">
+        <v>258</v>
+      </c>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
+    </row>
+    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F4" s="13"/>
+      <c r="G4" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" t="s">
+        <v>261</v>
+      </c>
+      <c r="I4" s="24">
+        <v>3918</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="O4" s="24">
+        <v>611</v>
+      </c>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="T4" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="U4" s="24">
+        <v>23047018</v>
+      </c>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="AA4" s="24">
+        <v>2359143</v>
+      </c>
+      <c r="AB4" s="23">
+        <f>AA4/SUM(U4,AA4)</f>
+        <v>9.2857122333437153E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F5" s="24"/>
+      <c r="G5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="K5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="L5" s="24"/>
+      <c r="M5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="N5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="O5" s="31"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="U5" s="40"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z5" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="41"/>
+    </row>
+    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D6" s="84" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" s="84"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+    </row>
+    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D7" s="86" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="86"/>
+      <c r="G7">
+        <v>127.98</v>
+      </c>
+      <c r="H7" s="36">
+        <v>18.384840000000001</v>
+      </c>
+      <c r="M7">
+        <v>128.34</v>
+      </c>
+      <c r="N7" s="36">
+        <v>19.25619</v>
+      </c>
+      <c r="S7" s="41">
+        <v>126.923238</v>
+      </c>
+      <c r="T7" s="36">
+        <v>18.110648999999999</v>
+      </c>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41">
+        <v>126.06586059999999</v>
+      </c>
+      <c r="Z7" s="37">
+        <v>18.439636100000001</v>
+      </c>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+    </row>
+    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8">
+        <v>29.6</v>
+      </c>
+      <c r="H8" s="36">
+        <v>5.9282329999999996</v>
+      </c>
+      <c r="M8">
+        <v>30.76</v>
+      </c>
+      <c r="N8" s="36">
+        <v>6.3475760000000001</v>
+      </c>
+      <c r="S8" s="36">
+        <v>29.662302499999999</v>
+      </c>
+      <c r="T8" s="36">
+        <v>5.9267823000000002</v>
+      </c>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41">
+        <v>29.959577500000002</v>
+      </c>
+      <c r="Z8" s="37">
+        <v>6.2308531</v>
+      </c>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
+    </row>
+    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D9" s="86" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="86"/>
+      <c r="G9">
+        <v>40.1</v>
+      </c>
+      <c r="H9" s="36">
+        <v>5.7592100000000004</v>
+      </c>
+      <c r="M9">
+        <v>40.619999999999997</v>
+      </c>
+      <c r="N9" s="36">
+        <v>5.5369099999999998</v>
+      </c>
+      <c r="S9" s="36">
+        <v>40.103714400000001</v>
+      </c>
+      <c r="T9" s="36">
+        <v>5.8665503000000001</v>
+      </c>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="36">
+        <v>40.107512399999997</v>
+      </c>
+      <c r="Z9" s="37">
+        <v>5.6566346999999997</v>
+      </c>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
+    </row>
+    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="S10" s="41"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
+    </row>
+    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D11" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="S11" s="41"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+    </row>
+    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D12" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="37">
+        <v>70.12</v>
+      </c>
+      <c r="H12" s="37">
+        <v>9.8203709999999997</v>
+      </c>
+      <c r="M12" s="37">
+        <v>65.349999999999994</v>
+      </c>
+      <c r="N12" s="37">
+        <v>8.5174970000000005</v>
+      </c>
+      <c r="S12" s="37">
+        <v>67.901583500000001</v>
+      </c>
+      <c r="T12" s="36">
+        <v>9.2750620000000001</v>
+      </c>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="37">
+        <v>64.861546799999999</v>
+      </c>
+      <c r="Z12" s="37">
+        <v>8.3972078000000003</v>
+      </c>
+      <c r="AA12" s="41"/>
+      <c r="AB12" s="41"/>
+    </row>
+    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D13" s="24"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="37"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
+    </row>
+    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D14" s="24"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+    </row>
+    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D15" s="24"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="41"/>
+      <c r="AB15" s="41"/>
+    </row>
+    <row r="16" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D16" s="84" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" s="84"/>
+      <c r="G16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="M16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="O16" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="S16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="U16" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z16" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA16" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB16" s="41"/>
+    </row>
+    <row r="17" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="G17">
+        <f>H17*I4</f>
+        <v>1578.9540000000002</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="M17" s="39">
+        <f>N17*O4</f>
+        <v>267.00700000000001</v>
+      </c>
+      <c r="N17" s="23">
+        <v>0.437</v>
+      </c>
+      <c r="S17" s="47">
+        <f>T17*U4</f>
+        <v>9945516.5527688004</v>
+      </c>
+      <c r="T17" s="26">
+        <v>0.43153160000000002</v>
+      </c>
+      <c r="U17" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="39">
+        <f>Z17*AA4</f>
+        <v>1143629.0127377999</v>
+      </c>
+      <c r="Z17" s="23">
+        <v>0.48476459999999999</v>
+      </c>
+      <c r="AA17" s="41"/>
+      <c r="AB17" s="41"/>
+    </row>
+    <row r="18" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D18" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="G18">
+        <v>3246</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" ref="H18:H30" si="0">G18/$I$4</f>
+        <v>0.82848392036753449</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="M18">
+        <v>187</v>
+      </c>
+      <c r="N18" s="23">
+        <f>M18/$O$4</f>
+        <v>0.30605564648117839</v>
+      </c>
+      <c r="S18" s="47">
+        <v>20959837</v>
+      </c>
+      <c r="T18" s="23">
+        <f t="shared" ref="T18:T30" si="1">S18/$U$4</f>
+        <v>0.90943813208285773</v>
+      </c>
+      <c r="U18" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41">
+        <v>1054148</v>
+      </c>
+      <c r="Z18" s="46">
+        <f t="shared" ref="Z18:Z30" si="2">Y18/$AA$4</f>
+        <v>0.44683514310069378</v>
+      </c>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="41"/>
+    </row>
+    <row r="19" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D19" s="27"/>
+      <c r="E19" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="G19">
+        <v>445</v>
+      </c>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11357835630423685</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="M19">
+        <v>323</v>
+      </c>
+      <c r="N19" s="23">
+        <f t="shared" ref="N19:N20" si="3">M19/$O$4</f>
+        <v>0.52864157119476274</v>
+      </c>
+      <c r="S19" s="47">
+        <v>1137593</v>
+      </c>
+      <c r="T19" s="23">
+        <f t="shared" si="1"/>
+        <v>4.9359661193478482E-2</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41">
+        <v>877192</v>
+      </c>
+      <c r="Z19" s="23">
+        <f t="shared" si="2"/>
+        <v>0.37182654887813077</v>
+      </c>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="41"/>
+    </row>
+    <row r="20" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D20" s="27"/>
+      <c r="E20" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="G20">
+        <v>227</v>
+      </c>
+      <c r="H20" s="23">
+        <f t="shared" si="0"/>
+        <v>5.7937723328228691E-2</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="M20">
+        <v>101</v>
+      </c>
+      <c r="N20" s="23">
+        <f t="shared" si="3"/>
+        <v>0.16530278232405893</v>
+      </c>
+      <c r="S20" s="47">
+        <v>949588</v>
+      </c>
+      <c r="T20" s="23">
+        <f t="shared" si="1"/>
+        <v>4.1202206723663773E-2</v>
+      </c>
+      <c r="U20" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41">
+        <v>427803</v>
+      </c>
+      <c r="Z20" s="23">
+        <f t="shared" si="2"/>
+        <v>0.18133830802117548</v>
+      </c>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="41"/>
+    </row>
+    <row r="21" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D21" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>339</v>
+      </c>
+      <c r="H21" s="23">
+        <f t="shared" si="0"/>
+        <v>8.6523736600306281E-2</v>
+      </c>
+      <c r="I21" s="26">
+        <f>SUM($H$21)</f>
+        <v>8.6523736600306281E-2</v>
+      </c>
+      <c r="M21">
+        <v>110</v>
+      </c>
+      <c r="N21" s="23">
+        <f t="shared" ref="N21:N30" si="4">M21/$O$4</f>
+        <v>0.18003273322422259</v>
+      </c>
+      <c r="O21" s="26">
+        <f>N21</f>
+        <v>0.18003273322422259</v>
+      </c>
+      <c r="S21" s="47">
+        <v>1559571</v>
+      </c>
+      <c r="T21" s="23">
+        <f t="shared" si="1"/>
+        <v>6.7669101486361488E-2</v>
+      </c>
+      <c r="U21" s="26">
+        <f>SUM($T$21)</f>
+        <v>6.7669101486361488E-2</v>
+      </c>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41">
+        <v>404485</v>
+      </c>
+      <c r="Z21" s="23">
+        <f t="shared" si="2"/>
+        <v>0.17145421027890212</v>
+      </c>
+      <c r="AA21" s="23">
+        <f>Z21</f>
+        <v>0.17145421027890212</v>
+      </c>
+      <c r="AB21" s="41"/>
+    </row>
+    <row r="22" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D22" s="24"/>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>342</v>
+      </c>
+      <c r="H22" s="23">
+        <f t="shared" si="0"/>
+        <v>8.7289433384379791E-2</v>
+      </c>
+      <c r="I22" s="26">
+        <f>SUM($H$21:$H22)</f>
+        <v>0.17381316998468607</v>
+      </c>
+      <c r="M22">
+        <v>92</v>
+      </c>
+      <c r="N22" s="23">
+        <f t="shared" si="4"/>
+        <v>0.15057283142389524</v>
+      </c>
+      <c r="O22" s="26">
+        <f>SUM($N$21:N22)</f>
+        <v>0.33060556464811786</v>
+      </c>
+      <c r="S22" s="47">
+        <v>1461268</v>
+      </c>
+      <c r="T22" s="23">
+        <f t="shared" si="1"/>
+        <v>6.3403777443138201E-2</v>
+      </c>
+      <c r="U22" s="26">
+        <f>SUM($T$21:$T22)</f>
+        <v>0.1310728789294997</v>
+      </c>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41">
+        <v>240757</v>
+      </c>
+      <c r="Z22" s="23">
+        <f t="shared" si="2"/>
+        <v>0.10205273694727281</v>
+      </c>
+      <c r="AA22" s="23">
+        <f>SUM($Z$21:Z22)</f>
+        <v>0.27350694722617491</v>
+      </c>
+      <c r="AB22" s="41"/>
+    </row>
+    <row r="23" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D23" s="24"/>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>365</v>
+      </c>
+      <c r="H23" s="23">
+        <f t="shared" si="0"/>
+        <v>9.3159775395610003E-2</v>
+      </c>
+      <c r="I23" s="26">
+        <f>SUM($H$21:$H23)</f>
+        <v>0.26697294538029609</v>
+      </c>
+      <c r="M23">
+        <v>87</v>
+      </c>
+      <c r="N23" s="23">
+        <f t="shared" si="4"/>
+        <v>0.14238952536824878</v>
+      </c>
+      <c r="O23" s="26">
+        <f>SUM($N$21:N23)</f>
+        <v>0.47299509001636664</v>
+      </c>
+      <c r="S23" s="47">
+        <v>2051140</v>
+      </c>
+      <c r="T23" s="23">
+        <f t="shared" si="1"/>
+        <v>8.8998064738787463E-2</v>
+      </c>
+      <c r="U23" s="26">
+        <f>SUM($T$21:$T23)</f>
+        <v>0.22007094366828717</v>
+      </c>
+      <c r="V23" s="41"/>
+      <c r="W23" s="41"/>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41">
+        <v>339098</v>
+      </c>
+      <c r="Z23" s="23">
+        <f t="shared" si="2"/>
+        <v>0.14373778952780733</v>
+      </c>
+      <c r="AA23" s="23">
+        <f>SUM($Z$21:Z23)</f>
+        <v>0.41724473675398221</v>
+      </c>
+      <c r="AB23" s="41"/>
+    </row>
+    <row r="24" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D24" s="24"/>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>368</v>
+      </c>
+      <c r="H24" s="23">
+        <f t="shared" si="0"/>
+        <v>9.3925472179683514E-2</v>
+      </c>
+      <c r="I24" s="26">
+        <f>SUM($H$21:$H24)</f>
+        <v>0.36089841755997959</v>
+      </c>
+      <c r="M24">
+        <v>83</v>
+      </c>
+      <c r="N24" s="23">
+        <f t="shared" si="4"/>
+        <v>0.13584288052373159</v>
+      </c>
+      <c r="O24" s="26">
+        <f>SUM($N$21:N24)</f>
+        <v>0.60883797054009825</v>
+      </c>
+      <c r="S24" s="47">
+        <v>2002854</v>
+      </c>
+      <c r="T24" s="23">
+        <f t="shared" si="1"/>
+        <v>8.6902956382469962E-2</v>
+      </c>
+      <c r="U24" s="26">
+        <f>SUM($T$21:$T24)</f>
+        <v>0.30697390005075714</v>
+      </c>
+      <c r="V24" s="41"/>
+      <c r="W24" s="41"/>
+      <c r="X24" s="41"/>
+      <c r="Y24" s="41">
+        <v>311698</v>
+      </c>
+      <c r="Z24" s="23">
+        <f t="shared" si="2"/>
+        <v>0.1321234024389365</v>
+      </c>
+      <c r="AA24" s="23">
+        <f>SUM($Z$21:Z24)</f>
+        <v>0.54936813919291871</v>
+      </c>
+      <c r="AB24" s="41"/>
+    </row>
+    <row r="25" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D25" s="24"/>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>397</v>
+      </c>
+      <c r="H25" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10132720775906075</v>
+      </c>
+      <c r="I25" s="26">
+        <f>SUM($H$21:$H25)</f>
+        <v>0.46222562531904032</v>
+      </c>
+      <c r="M25">
+        <v>61</v>
+      </c>
+      <c r="N25" s="23">
+        <f t="shared" si="4"/>
+        <v>9.9836333878887074E-2</v>
+      </c>
+      <c r="O25" s="26">
+        <f>SUM($N$21:N25)</f>
+        <v>0.70867430441898538</v>
+      </c>
+      <c r="S25" s="47">
+        <v>2308963</v>
+      </c>
+      <c r="T25" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10018489159855735</v>
+      </c>
+      <c r="U25" s="26">
+        <f>SUM($T$21:$T25)</f>
+        <v>0.40715879164931451</v>
+      </c>
+      <c r="V25" s="41"/>
+      <c r="W25" s="41"/>
+      <c r="X25" s="41"/>
+      <c r="Y25" s="41">
+        <v>183943</v>
+      </c>
+      <c r="Z25" s="23">
+        <f t="shared" si="2"/>
+        <v>7.797026293022509E-2</v>
+      </c>
+      <c r="AA25" s="23">
+        <f>SUM($Z$21:Z25)</f>
+        <v>0.62733840212314385</v>
+      </c>
+      <c r="AB25" s="41"/>
+    </row>
+    <row r="26" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D26" s="24"/>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>412</v>
+      </c>
+      <c r="H26" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10515569167942827</v>
+      </c>
+      <c r="I26" s="26">
+        <f>SUM($H$21:$H26)</f>
+        <v>0.56738131699846861</v>
+      </c>
+      <c r="M26">
+        <v>42</v>
+      </c>
+      <c r="N26" s="23">
+        <f t="shared" si="4"/>
+        <v>6.8739770867430439E-2</v>
+      </c>
+      <c r="O26" s="26">
+        <f>SUM($N$21:N26)</f>
+        <v>0.77741407528641582</v>
+      </c>
+      <c r="S26" s="47">
+        <v>2389812</v>
+      </c>
+      <c r="T26" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10369289423907249</v>
+      </c>
+      <c r="U26" s="26">
+        <f>SUM($T$21:$T26)</f>
+        <v>0.51085168588838703</v>
+      </c>
+      <c r="V26" s="41"/>
+      <c r="W26" s="41"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41">
+        <v>153145</v>
+      </c>
+      <c r="Z26" s="23">
+        <f t="shared" si="2"/>
+        <v>6.4915522289238081E-2</v>
+      </c>
+      <c r="AA26" s="23">
+        <f>SUM($Z$21:Z26)</f>
+        <v>0.69225392441238198</v>
+      </c>
+      <c r="AB26" s="41"/>
+    </row>
+    <row r="27" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D27" s="24"/>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>414</v>
+      </c>
+      <c r="H27" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10566615620214395</v>
+      </c>
+      <c r="I27" s="26">
+        <f>SUM($H$21:$H27)</f>
+        <v>0.67304747320061253</v>
+      </c>
+      <c r="M27">
+        <v>43</v>
+      </c>
+      <c r="N27" s="23">
+        <f t="shared" si="4"/>
+        <v>7.0376432078559745E-2</v>
+      </c>
+      <c r="O27" s="26">
+        <f>SUM($N$21:N27)</f>
+        <v>0.84779050736497552</v>
+      </c>
+      <c r="S27" s="47">
+        <v>2556546</v>
+      </c>
+      <c r="T27" s="23">
+        <f t="shared" si="1"/>
+        <v>0.11092740935074551</v>
+      </c>
+      <c r="U27" s="26">
+        <f>SUM($T$21:$T27)</f>
+        <v>0.62177909523913255</v>
+      </c>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41">
+        <v>171274</v>
+      </c>
+      <c r="Z27" s="23">
+        <f t="shared" si="2"/>
+        <v>7.2600092491213977E-2</v>
+      </c>
+      <c r="AA27" s="23">
+        <f>SUM($Z$21:Z27)</f>
+        <v>0.764854016903596</v>
+      </c>
+      <c r="AB27" s="41"/>
+    </row>
+    <row r="28" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D28" s="24"/>
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>426</v>
+      </c>
+      <c r="H28" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10872894333843798</v>
+      </c>
+      <c r="I28" s="26">
+        <f>SUM($H$21:$H28)</f>
+        <v>0.7817764165390505</v>
+      </c>
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="N28" s="23">
+        <f t="shared" si="4"/>
+        <v>4.9099836333878884E-2</v>
+      </c>
+      <c r="O28" s="26">
+        <f>SUM($N$21:N28)</f>
+        <v>0.89689034369885445</v>
+      </c>
+      <c r="S28" s="47">
+        <v>2805331</v>
+      </c>
+      <c r="T28" s="23">
+        <f t="shared" si="1"/>
+        <v>0.12172208135560098</v>
+      </c>
+      <c r="U28" s="26">
+        <f>SUM($T$21:$T28)</f>
+        <v>0.74350117659473347</v>
+      </c>
+      <c r="V28" s="41"/>
+      <c r="W28" s="41"/>
+      <c r="X28" s="41"/>
+      <c r="Y28" s="41">
+        <v>127970</v>
+      </c>
+      <c r="Z28" s="23">
+        <f t="shared" si="2"/>
+        <v>5.4244274297912419E-2</v>
+      </c>
+      <c r="AA28" s="23">
+        <f>SUM($Z$21:Z28)</f>
+        <v>0.81909829120150845</v>
+      </c>
+      <c r="AB28" s="41"/>
+    </row>
+    <row r="29" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D29" s="24"/>
+      <c r="E29">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>421</v>
+      </c>
+      <c r="H29" s="23">
+        <f t="shared" si="0"/>
+        <v>0.10745278203164881</v>
+      </c>
+      <c r="I29" s="26">
+        <f>SUM($H$21:$H29)</f>
+        <v>0.88922919857069926</v>
+      </c>
+      <c r="M29">
+        <v>38</v>
+      </c>
+      <c r="N29" s="23">
+        <f t="shared" si="4"/>
+        <v>6.2193126022913256E-2</v>
+      </c>
+      <c r="O29" s="26">
+        <f>SUM($N$21:N29)</f>
+        <v>0.95908346972176772</v>
+      </c>
+      <c r="S29" s="47">
+        <v>2756844</v>
+      </c>
+      <c r="T29" s="23">
+        <f t="shared" si="1"/>
+        <v>0.11961825169746472</v>
+      </c>
+      <c r="U29" s="26">
+        <f>SUM($T$21:$T29)</f>
+        <v>0.86311942829219823</v>
+      </c>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41">
+        <v>274731</v>
+      </c>
+      <c r="Z29" s="23">
+        <f t="shared" si="2"/>
+        <v>0.11645372917199169</v>
+      </c>
+      <c r="AA29" s="23">
+        <f>SUM($Z$21:Z29)</f>
+        <v>0.93555202037350016</v>
+      </c>
+      <c r="AB29" s="41"/>
+    </row>
+    <row r="30" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="D30" s="24"/>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>434</v>
+      </c>
+      <c r="H30" s="23">
+        <f t="shared" si="0"/>
+        <v>0.11077080142930067</v>
+      </c>
+      <c r="I30" s="26">
+        <f>SUM($H$21:$H30)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="M30">
+        <v>25</v>
+      </c>
+      <c r="N30" s="23">
+        <f t="shared" si="4"/>
+        <v>4.0916530278232409E-2</v>
+      </c>
+      <c r="O30" s="26">
+        <f>SUM($N$21:N30)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="S30" s="47">
+        <v>3154689</v>
+      </c>
+      <c r="T30" s="23">
+        <f t="shared" si="1"/>
+        <v>0.13688057170780185</v>
+      </c>
+      <c r="U30" s="26">
+        <f>SUM($T$21:$T30)</f>
+        <v>1</v>
+      </c>
+      <c r="V30" s="41"/>
+      <c r="W30" s="41"/>
+      <c r="X30" s="41"/>
+      <c r="Y30" s="41">
+        <v>152042</v>
+      </c>
+      <c r="Z30" s="23">
+        <f t="shared" si="2"/>
+        <v>6.4447979626499965E-2</v>
+      </c>
+      <c r="AA30" s="23">
+        <f>SUM($Z$21:Z30)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="AB30" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="S3:AB3"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="G3:P3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F52B84-34FD-493D-A4ED-2F71A840B086}">
   <dimension ref="D3:AB32"/>
   <sheetViews>
@@ -2798,31 +4197,31 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="82" t="s">
         <v>253</v>
       </c>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="74" t="s">
+      <c r="S3" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
@@ -2912,16 +4311,16 @@
       <c r="AA5" s="50"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="E6" s="76"/>
+      <c r="E6" s="84"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="77"/>
+      <c r="E7" s="86"/>
       <c r="G7" s="70">
         <v>-0.13370000000000001</v>
       </c>
@@ -3005,10 +4404,10 @@
       <c r="AB8" s="58"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="77"/>
+      <c r="E9" s="86"/>
       <c r="G9" s="70">
         <v>0.46750000000000003</v>
       </c>
@@ -3161,10 +4560,10 @@
       <c r="U15" s="30"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="84" t="s">
         <v>315</v>
       </c>
-      <c r="E16" s="76"/>
+      <c r="E16" s="84"/>
       <c r="G16" s="33" t="s">
         <v>313</v>
       </c>
@@ -4028,7 +5427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
   <dimension ref="C2:H13"/>
   <sheetViews>
@@ -4254,7 +5653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2B95C5-E717-4ABB-BAF8-DAA816951EFA}">
   <dimension ref="C2:I49"/>
   <sheetViews>
@@ -4695,6 +6094,260 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDC04DF-1D9A-4131-9442-DC1AD08BDDA5}">
+  <dimension ref="C4:E27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D6" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>30121997</v>
+      </c>
+      <c r="E8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>13022021</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>14022021</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>15022021</v>
+      </c>
+      <c r="E11" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="72">
+        <v>16022021</v>
+      </c>
+      <c r="E12" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" s="72">
+        <v>17022021</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="72">
+        <v>18022021</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="72">
+        <v>8</v>
+      </c>
+      <c r="D15" s="72">
+        <v>19022021</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="72">
+        <v>9</v>
+      </c>
+      <c r="D16" s="72">
+        <v>20022021</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="72">
+        <v>10</v>
+      </c>
+      <c r="D17" s="72">
+        <v>21022021</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="72">
+        <v>11</v>
+      </c>
+      <c r="D18" s="72">
+        <v>22022021</v>
+      </c>
+      <c r="E18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="72">
+        <v>12</v>
+      </c>
+      <c r="D19" s="72">
+        <v>23022021</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="72">
+        <v>13</v>
+      </c>
+      <c r="D20" s="72">
+        <v>24022021</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="72">
+        <v>14</v>
+      </c>
+      <c r="D21" s="72">
+        <v>25022021</v>
+      </c>
+      <c r="E21" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="72">
+        <v>15</v>
+      </c>
+      <c r="D22" s="72">
+        <v>26022021</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="72">
+        <v>16</v>
+      </c>
+      <c r="D23" s="72">
+        <v>27022021</v>
+      </c>
+      <c r="E23" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="72">
+        <v>17</v>
+      </c>
+      <c r="D24" s="72">
+        <v>28022021</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="72">
+        <v>18</v>
+      </c>
+      <c r="D25" s="72">
+        <v>29022021</v>
+      </c>
+      <c r="E25" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="72">
+        <v>19</v>
+      </c>
+      <c r="D26" s="72">
+        <v>30022021</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="72">
+        <v>20</v>
+      </c>
+      <c r="D27" s="72">
+        <v>31022021</v>
+      </c>
+      <c r="E27" s="72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37E278C-1DAC-4F67-8E1E-CC1E987D4B76}">
   <dimension ref="C2:I49"/>
   <sheetViews>
@@ -5134,7 +6787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
   <dimension ref="C2:J20"/>
   <sheetViews>
@@ -5457,7 +7110,269 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E776B9-4EC5-46CF-B1E5-E124814149F5}">
+  <dimension ref="A2:K13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" t="s">
+        <v>365</v>
+      </c>
+      <c r="E4" t="s">
+        <v>366</v>
+      </c>
+      <c r="I4" s="79" t="s">
+        <v>254</v>
+      </c>
+      <c r="J4" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="K4" s="79" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5">
+        <v>9.61</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>16.28</v>
+      </c>
+      <c r="G5" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="I5">
+        <v>29.95</v>
+      </c>
+      <c r="J5">
+        <v>28.25</v>
+      </c>
+      <c r="K5">
+        <v>10.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6">
+        <v>8.7469999999999999</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>15.94</v>
+      </c>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79" t="s">
+        <v>311</v>
+      </c>
+      <c r="I6">
+        <v>29.58</v>
+      </c>
+      <c r="J6">
+        <v>27.5</v>
+      </c>
+      <c r="K6">
+        <v>11.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>367</v>
+      </c>
+      <c r="C8">
+        <v>9.6</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="G8" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="79" t="s">
+        <v>367</v>
+      </c>
+      <c r="I8">
+        <v>29.76</v>
+      </c>
+      <c r="J8">
+        <v>27.75</v>
+      </c>
+      <c r="K8">
+        <v>11.14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>368</v>
+      </c>
+      <c r="C9">
+        <v>9.6</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="I9">
+        <v>29.12</v>
+      </c>
+      <c r="J9">
+        <v>27.75</v>
+      </c>
+      <c r="K9">
+        <v>9.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>369</v>
+      </c>
+      <c r="C10">
+        <v>8.4</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>13.49</v>
+      </c>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79" t="s">
+        <v>369</v>
+      </c>
+      <c r="I10">
+        <v>27.84</v>
+      </c>
+      <c r="J10">
+        <v>26</v>
+      </c>
+      <c r="K10">
+        <v>9.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>332</v>
+      </c>
+      <c r="C12">
+        <v>8.83</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>13.34</v>
+      </c>
+      <c r="G12" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="79" t="s">
+        <v>332</v>
+      </c>
+      <c r="I12">
+        <v>37.93</v>
+      </c>
+      <c r="J12">
+        <v>38</v>
+      </c>
+      <c r="K12">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13">
+        <v>10.1</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>18.23</v>
+      </c>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79" t="s">
+        <v>273</v>
+      </c>
+      <c r="I13">
+        <v>23.05</v>
+      </c>
+      <c r="J13">
+        <v>23.25</v>
+      </c>
+      <c r="K13">
+        <v>7.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60364F5B-DCE9-46C6-A586-3092036B5563}">
   <dimension ref="D4:O12"/>
   <sheetViews>
@@ -5474,26 +7389,26 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="80" t="s">
         <v>244</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72" t="s">
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80" t="s">
         <v>243</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
     </row>
     <row r="5" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="I5" s="73" t="s">
+      <c r="G5" s="81"/>
+      <c r="I5" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="J5" s="73"/>
+      <c r="J5" s="81"/>
     </row>
     <row r="6" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
@@ -5710,7 +7625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FBAE27-4D7B-4D03-B5B4-DAD9C59D9C9D}">
   <dimension ref="B1:Z60"/>
   <sheetViews>
@@ -6178,7 +8093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B6F673-63EF-4D30-A5E9-76FC267124A8}">
   <dimension ref="C2:S16"/>
   <sheetViews>
@@ -6192,48 +8107,48 @@
       <c r="C2" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="83" t="s">
         <v>244</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="M2" s="75" t="s">
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="M2" s="83" t="s">
         <v>243</v>
       </c>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="82" t="s">
         <v>327</v>
       </c>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="I3" s="74" t="s">
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="I3" s="82" t="s">
         <v>328</v>
       </c>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="M3" s="74" t="s">
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="M3" s="82" t="s">
         <v>327</v>
       </c>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
       <c r="P3" s="45"/>
-      <c r="Q3" s="74" t="s">
+      <c r="Q3" s="82" t="s">
         <v>328</v>
       </c>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E4" s="31" t="s">
@@ -6417,51 +8332,51 @@
       <c r="E10" s="43"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="83" t="s">
         <v>244</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
       <c r="L11" s="49"/>
-      <c r="M11" s="75" t="s">
+      <c r="M11" s="83" t="s">
         <v>243</v>
       </c>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="75"/>
-      <c r="Q11" s="75"/>
-      <c r="R11" s="75"/>
-      <c r="S11" s="75"/>
+      <c r="N11" s="83"/>
+      <c r="O11" s="83"/>
+      <c r="P11" s="83"/>
+      <c r="Q11" s="83"/>
+      <c r="R11" s="83"/>
+      <c r="S11" s="83"/>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D12" s="49"/>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="82" t="s">
         <v>327</v>
       </c>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
       <c r="H12" s="49"/>
-      <c r="I12" s="74" t="s">
+      <c r="I12" s="82" t="s">
         <v>328</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="74" t="s">
+      <c r="M12" s="82" t="s">
         <v>327</v>
       </c>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
       <c r="P12" s="49"/>
-      <c r="Q12" s="74" t="s">
+      <c r="Q12" s="82" t="s">
         <v>328</v>
       </c>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D13" s="49"/>
@@ -6657,12 +8572,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC7C8D0-92F2-48FB-9F5D-D6BDDD3DDCD3}">
   <dimension ref="D5:BN30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB16" activeCellId="12" sqref="Q16 S16 U16 W16 AR16 AP16 AN16 AL16 AJ16 AH16 AF16 AD16 AB16"/>
+    <sheetView showGridLines="0" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AJ33" sqref="AJ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6693,109 +8608,109 @@
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
       <c r="F6" s="57"/>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="82" t="s">
         <v>352</v>
       </c>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
-      <c r="Q6" s="74"/>
-      <c r="R6" s="74"/>
-      <c r="S6" s="74"/>
-      <c r="T6" s="74"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="74"/>
-      <c r="W6" s="74"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
       <c r="Y6" s="57"/>
       <c r="Z6" s="57"/>
       <c r="AA6" s="57"/>
-      <c r="AB6" s="74" t="s">
+      <c r="AB6" s="82" t="s">
         <v>355</v>
       </c>
-      <c r="AC6" s="74"/>
-      <c r="AD6" s="74"/>
-      <c r="AE6" s="74"/>
-      <c r="AF6" s="74"/>
-      <c r="AG6" s="74"/>
-      <c r="AH6" s="74"/>
-      <c r="AI6" s="74"/>
-      <c r="AJ6" s="74"/>
-      <c r="AK6" s="74"/>
-      <c r="AL6" s="74"/>
-      <c r="AM6" s="74"/>
-      <c r="AN6" s="74"/>
-      <c r="AO6" s="74"/>
-      <c r="AP6" s="74"/>
-      <c r="AQ6" s="74"/>
-      <c r="AR6" s="74"/>
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="82"/>
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="82"/>
+      <c r="AH6" s="82"/>
+      <c r="AI6" s="82"/>
+      <c r="AJ6" s="82"/>
+      <c r="AK6" s="82"/>
+      <c r="AL6" s="82"/>
+      <c r="AM6" s="82"/>
+      <c r="AN6" s="82"/>
+      <c r="AO6" s="82"/>
+      <c r="AP6" s="82"/>
+      <c r="AQ6" s="82"/>
+      <c r="AR6" s="82"/>
       <c r="BA6" s="57"/>
       <c r="BB6" s="57"/>
       <c r="BC6" s="57"/>
-      <c r="BD6" s="74"/>
-      <c r="BE6" s="74"/>
-      <c r="BF6" s="74"/>
-      <c r="BG6" s="74"/>
-      <c r="BH6" s="74"/>
-      <c r="BI6" s="74"/>
-      <c r="BJ6" s="74"/>
-      <c r="BK6" s="74"/>
-      <c r="BL6" s="74"/>
-      <c r="BM6" s="74"/>
-      <c r="BN6" s="74"/>
+      <c r="BD6" s="82"/>
+      <c r="BE6" s="82"/>
+      <c r="BF6" s="82"/>
+      <c r="BG6" s="82"/>
+      <c r="BH6" s="82"/>
+      <c r="BI6" s="82"/>
+      <c r="BJ6" s="82"/>
+      <c r="BK6" s="82"/>
+      <c r="BL6" s="82"/>
+      <c r="BM6" s="82"/>
+      <c r="BN6" s="82"/>
     </row>
     <row r="7" spans="4:66" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="82" t="s">
+      <c r="G7" s="87" t="s">
         <v>264</v>
       </c>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
       <c r="L7" s="35"/>
-      <c r="M7" s="82" t="s">
+      <c r="M7" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
       <c r="R7" s="35"/>
-      <c r="S7" s="82" t="s">
+      <c r="S7" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="82"/>
-      <c r="U7" s="82"/>
-      <c r="V7" s="82"/>
-      <c r="W7" s="82"/>
-      <c r="AB7" s="82" t="s">
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="AB7" s="87" t="s">
         <v>264</v>
       </c>
-      <c r="AC7" s="82"/>
-      <c r="AD7" s="82"/>
-      <c r="AE7" s="82"/>
-      <c r="AF7" s="82"/>
+      <c r="AC7" s="87"/>
+      <c r="AD7" s="87"/>
+      <c r="AE7" s="87"/>
+      <c r="AF7" s="87"/>
       <c r="AG7" s="35"/>
-      <c r="AH7" s="82" t="s">
+      <c r="AH7" s="87" t="s">
         <v>164</v>
       </c>
-      <c r="AI7" s="82"/>
-      <c r="AJ7" s="82"/>
-      <c r="AK7" s="82"/>
-      <c r="AL7" s="82"/>
+      <c r="AI7" s="87"/>
+      <c r="AJ7" s="87"/>
+      <c r="AK7" s="87"/>
+      <c r="AL7" s="87"/>
       <c r="AM7" s="35"/>
-      <c r="AN7" s="82" t="s">
+      <c r="AN7" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="AO7" s="82"/>
-      <c r="AP7" s="82"/>
-      <c r="AQ7" s="82"/>
-      <c r="AR7" s="82"/>
+      <c r="AO7" s="87"/>
+      <c r="AP7" s="87"/>
+      <c r="AQ7" s="87"/>
+      <c r="AR7" s="87"/>
       <c r="BD7" s="35"/>
       <c r="BE7" s="35"/>
       <c r="BF7" s="35"/>
@@ -6824,27 +8739,27 @@
         <v>351</v>
       </c>
       <c r="L8" s="32"/>
-      <c r="M8" s="78" t="s">
+      <c r="M8" s="73" t="s">
         <v>349</v>
       </c>
-      <c r="N8" s="78"/>
-      <c r="O8" s="78" t="s">
+      <c r="N8" s="73"/>
+      <c r="O8" s="73" t="s">
         <v>350</v>
       </c>
-      <c r="P8" s="78"/>
-      <c r="Q8" s="78" t="s">
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73" t="s">
         <v>351</v>
       </c>
       <c r="R8" s="24"/>
-      <c r="S8" s="78" t="s">
+      <c r="S8" s="73" t="s">
         <v>349</v>
       </c>
       <c r="T8" s="28"/>
-      <c r="U8" s="78" t="s">
+      <c r="U8" s="73" t="s">
         <v>350</v>
       </c>
       <c r="V8" s="28"/>
-      <c r="W8" s="78" t="s">
+      <c r="W8" s="73" t="s">
         <v>351</v>
       </c>
       <c r="Y8" s="57"/>
@@ -6862,27 +8777,27 @@
         <v>351</v>
       </c>
       <c r="AG8" s="32"/>
-      <c r="AH8" s="78" t="s">
+      <c r="AH8" s="73" t="s">
         <v>349</v>
       </c>
-      <c r="AI8" s="78"/>
-      <c r="AJ8" s="78" t="s">
+      <c r="AI8" s="73"/>
+      <c r="AJ8" s="73" t="s">
         <v>350</v>
       </c>
-      <c r="AK8" s="78"/>
-      <c r="AL8" s="78" t="s">
+      <c r="AK8" s="73"/>
+      <c r="AL8" s="73" t="s">
         <v>351</v>
       </c>
       <c r="AM8" s="24"/>
-      <c r="AN8" s="78" t="s">
+      <c r="AN8" s="73" t="s">
         <v>349</v>
       </c>
       <c r="AO8" s="28"/>
-      <c r="AP8" s="78" t="s">
+      <c r="AP8" s="73" t="s">
         <v>350</v>
       </c>
       <c r="AQ8" s="28"/>
-      <c r="AR8" s="78" t="s">
+      <c r="AR8" s="73" t="s">
         <v>351</v>
       </c>
       <c r="BA8" s="57"/>
@@ -6898,7 +8813,7 @@
       <c r="BK8" s="57"/>
       <c r="BL8" s="24"/>
       <c r="BM8" s="24"/>
-      <c r="BN8" s="78"/>
+      <c r="BN8" s="73"/>
     </row>
     <row r="9" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D9" s="57"/>
@@ -6993,10 +8908,10 @@
       <c r="BN9" s="55"/>
     </row>
     <row r="10" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="84" t="s">
         <v>354</v>
       </c>
-      <c r="E10" s="83"/>
+      <c r="E10" s="85"/>
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10" s="57"/>
@@ -7011,10 +8926,10 @@
       <c r="U10" s="57"/>
       <c r="V10" s="57"/>
       <c r="W10" s="57"/>
-      <c r="Y10" s="76" t="s">
+      <c r="Y10" s="84" t="s">
         <v>354</v>
       </c>
-      <c r="Z10" s="83"/>
+      <c r="Z10" s="85"/>
       <c r="AA10" s="57"/>
       <c r="AB10" s="57"/>
       <c r="AC10" s="57"/>
@@ -7033,8 +8948,8 @@
       <c r="AP10" s="57"/>
       <c r="AQ10" s="57"/>
       <c r="AR10" s="57"/>
-      <c r="BA10" s="76"/>
-      <c r="BB10" s="76"/>
+      <c r="BA10" s="84"/>
+      <c r="BB10" s="84"/>
       <c r="BC10" s="57"/>
       <c r="BD10" s="57"/>
       <c r="BE10" s="57"/>
@@ -7049,10 +8964,10 @@
       <c r="BN10" s="57"/>
     </row>
     <row r="11" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D11" s="77" t="s">
+      <c r="D11" s="86" t="s">
         <v>353</v>
       </c>
-      <c r="E11" s="77"/>
+      <c r="E11" s="86"/>
       <c r="F11" s="57"/>
       <c r="G11" s="11">
         <v>0.27</v>
@@ -7088,10 +9003,10 @@
       <c r="W11" s="11">
         <v>-0.63</v>
       </c>
-      <c r="Y11" s="77" t="s">
+      <c r="Y11" s="86" t="s">
         <v>353</v>
       </c>
-      <c r="Z11" s="77"/>
+      <c r="Z11" s="86"/>
       <c r="AA11" s="57"/>
       <c r="AB11" s="11">
         <v>1.51</v>
@@ -7128,8 +9043,8 @@
       <c r="AR11" s="11">
         <v>-0.5</v>
       </c>
-      <c r="BA11" s="77"/>
-      <c r="BB11" s="77"/>
+      <c r="BA11" s="86"/>
+      <c r="BB11" s="86"/>
       <c r="BC11" s="57"/>
       <c r="BD11" s="11"/>
       <c r="BE11" s="65"/>
@@ -7398,10 +9313,10 @@
       <c r="BN15" s="57"/>
     </row>
     <row r="16" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="84" t="s">
         <v>348</v>
       </c>
-      <c r="E16" s="76"/>
+      <c r="E16" s="84"/>
       <c r="F16" s="57"/>
       <c r="G16" s="33" t="s">
         <v>356</v>
@@ -7418,11 +9333,11 @@
       <c r="M16" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="N16" s="84"/>
+      <c r="N16" s="77"/>
       <c r="O16" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="P16" s="84"/>
+      <c r="P16" s="77"/>
       <c r="Q16" s="33" t="s">
         <v>356</v>
       </c>
@@ -7438,10 +9353,10 @@
       <c r="W16" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="Y16" s="76" t="s">
+      <c r="Y16" s="84" t="s">
         <v>348</v>
       </c>
-      <c r="Z16" s="76"/>
+      <c r="Z16" s="84"/>
       <c r="AA16" s="57"/>
       <c r="AB16" s="33" t="s">
         <v>356</v>
@@ -7478,8 +9393,8 @@
       <c r="AR16" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="BA16" s="76"/>
-      <c r="BB16" s="76"/>
+      <c r="BA16" s="84"/>
+      <c r="BB16" s="84"/>
       <c r="BC16" s="57"/>
       <c r="BD16" s="33"/>
       <c r="BE16" s="33"/>
@@ -7501,39 +9416,39 @@
         <v>332</v>
       </c>
       <c r="F17" s="57"/>
-      <c r="G17" s="85">
+      <c r="G17" s="78">
         <v>0.31</v>
       </c>
-      <c r="H17" s="85"/>
-      <c r="I17" s="85">
+      <c r="H17" s="78"/>
+      <c r="I17" s="78">
         <v>0.41</v>
       </c>
-      <c r="J17" s="85"/>
-      <c r="K17" s="85">
+      <c r="J17" s="78"/>
+      <c r="K17" s="78">
         <v>0.48</v>
       </c>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85">
+      <c r="L17" s="78"/>
+      <c r="M17" s="78">
         <v>0.32</v>
       </c>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85">
+      <c r="N17" s="78"/>
+      <c r="O17" s="78">
         <v>0.42</v>
       </c>
-      <c r="P17" s="85"/>
-      <c r="Q17" s="85">
+      <c r="P17" s="78"/>
+      <c r="Q17" s="78">
         <v>0.44</v>
       </c>
-      <c r="R17" s="85"/>
-      <c r="S17" s="85">
+      <c r="R17" s="78"/>
+      <c r="S17" s="78">
         <v>0.44</v>
       </c>
-      <c r="T17" s="85"/>
-      <c r="U17" s="85">
+      <c r="T17" s="78"/>
+      <c r="U17" s="78">
         <v>0.42</v>
       </c>
-      <c r="V17" s="85"/>
-      <c r="W17" s="85">
+      <c r="V17" s="78"/>
+      <c r="W17" s="78">
         <v>0.3</v>
       </c>
       <c r="Y17" s="24" t="s">
@@ -7582,15 +9497,15 @@
       <c r="BB17" s="24"/>
       <c r="BC17" s="57"/>
       <c r="BD17" s="58"/>
-      <c r="BE17" s="79"/>
-      <c r="BF17" s="79"/>
+      <c r="BE17" s="74"/>
+      <c r="BF17" s="74"/>
       <c r="BG17" s="58"/>
-      <c r="BH17" s="80"/>
-      <c r="BI17" s="81"/>
+      <c r="BH17" s="75"/>
+      <c r="BI17" s="76"/>
       <c r="BJ17" s="58"/>
       <c r="BK17" s="58"/>
-      <c r="BL17" s="80"/>
-      <c r="BM17" s="81"/>
+      <c r="BL17" s="75"/>
+      <c r="BM17" s="76"/>
       <c r="BN17" s="58"/>
     </row>
     <row r="18" spans="4:66" x14ac:dyDescent="0.25">
@@ -7601,47 +9516,47 @@
         <v>270</v>
       </c>
       <c r="F18" s="57"/>
-      <c r="G18" s="85">
+      <c r="G18" s="78">
         <f>230691/(230691+191767+30442)</f>
         <v>0.50936409803488625</v>
       </c>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85">
+      <c r="H18" s="78"/>
+      <c r="I18" s="78">
         <f>2820893/(2820893+545171+257136)</f>
         <v>0.77856397659527488</v>
       </c>
-      <c r="J18" s="85"/>
-      <c r="K18" s="85">
+      <c r="J18" s="78"/>
+      <c r="K18" s="78">
         <f>381554/(381554+30884+40462)</f>
         <v>0.84246853610068451</v>
       </c>
-      <c r="L18" s="85"/>
-      <c r="M18" s="85">
+      <c r="L18" s="78"/>
+      <c r="M18" s="78">
         <f>104107/(104107+333270+15522)</f>
         <v>0.22986802797091627</v>
       </c>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85">
+      <c r="N18" s="78"/>
+      <c r="O18" s="78">
         <f>2953008/(2953008+425467+244724)</f>
         <v>0.81502782485864012</v>
       </c>
-      <c r="P18" s="85"/>
-      <c r="Q18" s="85">
+      <c r="P18" s="78"/>
+      <c r="Q18" s="78">
         <f>376023/(376023+9083+57794)</f>
         <v>0.84900203206141345</v>
       </c>
-      <c r="R18" s="85"/>
-      <c r="S18" s="85">
+      <c r="R18" s="78"/>
+      <c r="S18" s="78">
         <f>163116/(163116+266388+23396)</f>
         <v>0.36015897549127845</v>
       </c>
-      <c r="T18" s="85"/>
-      <c r="U18" s="85">
+      <c r="T18" s="78"/>
+      <c r="U18" s="78">
         <f>2875086/(2875086+492074+256039)</f>
         <v>0.79352141574338042</v>
       </c>
-      <c r="V18" s="85"/>
-      <c r="W18" s="85">
+      <c r="V18" s="78"/>
+      <c r="W18" s="78">
         <f>394932/(394932+9360+48605)</f>
         <v>0.87201284177197025</v>
       </c>
@@ -7700,15 +9615,15 @@
       <c r="BB18" s="24"/>
       <c r="BC18" s="57"/>
       <c r="BD18" s="58"/>
-      <c r="BE18" s="81"/>
-      <c r="BF18" s="81"/>
+      <c r="BE18" s="76"/>
+      <c r="BF18" s="76"/>
       <c r="BG18" s="58"/>
       <c r="BH18" s="58"/>
-      <c r="BI18" s="81"/>
+      <c r="BI18" s="76"/>
       <c r="BJ18" s="58"/>
       <c r="BK18" s="58"/>
       <c r="BL18" s="58"/>
-      <c r="BM18" s="81"/>
+      <c r="BM18" s="76"/>
       <c r="BN18" s="58"/>
     </row>
     <row r="19" spans="4:66" x14ac:dyDescent="0.25">
@@ -7717,47 +9632,47 @@
         <v>271</v>
       </c>
       <c r="F19" s="57"/>
-      <c r="G19" s="85">
+      <c r="G19" s="78">
         <f>191767/(230691+191767+30442)</f>
         <v>0.42342018105542062</v>
       </c>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85">
+      <c r="H19" s="78"/>
+      <c r="I19" s="78">
         <f>545171/(2820893+545171+257136)</f>
         <v>0.15046671450651358</v>
       </c>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85">
+      <c r="J19" s="78"/>
+      <c r="K19" s="78">
         <f>30884/(381554+30884+40462)</f>
         <v>6.8191653786707884E-2</v>
       </c>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85">
+      <c r="L19" s="78"/>
+      <c r="M19" s="78">
         <f>333270/(104107+333270+15522)</f>
         <v>0.73585943002744536</v>
       </c>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85">
+      <c r="N19" s="78"/>
+      <c r="O19" s="78">
         <f>425467/(2953008+425467+244724)</f>
         <v>0.11742854863892378</v>
       </c>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85">
+      <c r="P19" s="78"/>
+      <c r="Q19" s="78">
         <f>9083/(376023+9083+57794)</f>
         <v>2.05080153533529E-2</v>
       </c>
-      <c r="R19" s="85"/>
-      <c r="S19" s="85">
+      <c r="R19" s="78"/>
+      <c r="S19" s="78">
         <f>266388/(163116+266388+23396)</f>
         <v>0.58818282181497017</v>
       </c>
-      <c r="T19" s="85"/>
-      <c r="U19" s="85">
+      <c r="T19" s="78"/>
+      <c r="U19" s="78">
         <f>492074/(2875086+492074+256039)</f>
         <v>0.13581202688563337</v>
       </c>
-      <c r="V19" s="85"/>
-      <c r="W19" s="85">
+      <c r="V19" s="78"/>
+      <c r="W19" s="78">
         <f>9360/(394932+9360+48605)</f>
         <v>2.0666950763639415E-2</v>
       </c>
@@ -7814,15 +9729,15 @@
       <c r="BB19" s="24"/>
       <c r="BC19" s="57"/>
       <c r="BD19" s="58"/>
-      <c r="BE19" s="81"/>
-      <c r="BF19" s="81"/>
+      <c r="BE19" s="76"/>
+      <c r="BF19" s="76"/>
       <c r="BG19" s="58"/>
       <c r="BH19" s="58"/>
-      <c r="BI19" s="81"/>
+      <c r="BI19" s="76"/>
       <c r="BJ19" s="58"/>
       <c r="BK19" s="58"/>
       <c r="BL19" s="58"/>
-      <c r="BM19" s="81"/>
+      <c r="BM19" s="76"/>
       <c r="BN19" s="58"/>
     </row>
     <row r="20" spans="4:66" x14ac:dyDescent="0.25">
@@ -7831,47 +9746,47 @@
         <v>272</v>
       </c>
       <c r="F20" s="57"/>
-      <c r="G20" s="85">
+      <c r="G20" s="78">
         <f>30442/(230691+191767+30442)</f>
         <v>6.7215720909693091E-2</v>
       </c>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85">
+      <c r="H20" s="78"/>
+      <c r="I20" s="78">
         <f>257136/(2820893+545171+257136)</f>
         <v>7.0969308898211528E-2</v>
       </c>
-      <c r="J20" s="85"/>
-      <c r="K20" s="85">
+      <c r="J20" s="78"/>
+      <c r="K20" s="78">
         <f>40462/(381554+30884+40462)</f>
         <v>8.9339810112607637E-2</v>
       </c>
-      <c r="L20" s="85"/>
-      <c r="M20" s="85">
+      <c r="L20" s="78"/>
+      <c r="M20" s="78">
         <f>15522/(104107+333270+15522)</f>
         <v>3.4272542001638331E-2</v>
       </c>
-      <c r="N20" s="85"/>
-      <c r="O20" s="85">
+      <c r="N20" s="78"/>
+      <c r="O20" s="78">
         <f>244724/(2953008+425467+244724)</f>
         <v>6.7543626502436102E-2</v>
       </c>
-      <c r="P20" s="85"/>
-      <c r="Q20" s="85">
+      <c r="P20" s="78"/>
+      <c r="Q20" s="78">
         <f>67794/(376023+9083+57794)</f>
         <v>0.15306841273425154</v>
       </c>
-      <c r="R20" s="85"/>
-      <c r="S20" s="85">
+      <c r="R20" s="78"/>
+      <c r="S20" s="78">
         <f>23396/(163116+266388+23396)</f>
         <v>5.1658202693751383E-2</v>
       </c>
-      <c r="T20" s="85"/>
-      <c r="U20" s="85">
+      <c r="T20" s="78"/>
+      <c r="U20" s="78">
         <f>256039/(2875086+492074+256039)</f>
         <v>7.0666557370986247E-2</v>
       </c>
-      <c r="V20" s="85"/>
-      <c r="W20" s="85">
+      <c r="V20" s="78"/>
+      <c r="W20" s="78">
         <f>48605/(394932+9360+48605)</f>
         <v>0.10732020746439036</v>
       </c>
@@ -7928,15 +9843,15 @@
       <c r="BB20" s="24"/>
       <c r="BC20" s="57"/>
       <c r="BD20" s="58"/>
-      <c r="BE20" s="81"/>
-      <c r="BF20" s="81"/>
+      <c r="BE20" s="76"/>
+      <c r="BF20" s="76"/>
       <c r="BG20" s="58"/>
       <c r="BH20" s="58"/>
-      <c r="BI20" s="81"/>
+      <c r="BI20" s="76"/>
       <c r="BJ20" s="58"/>
       <c r="BK20" s="58"/>
       <c r="BL20" s="58"/>
-      <c r="BM20" s="81"/>
+      <c r="BM20" s="76"/>
       <c r="BN20" s="58"/>
     </row>
     <row r="21" spans="4:66" x14ac:dyDescent="0.25">
@@ -8028,16 +9943,16 @@
       <c r="BB21" s="57"/>
       <c r="BC21" s="57"/>
       <c r="BD21" s="58"/>
-      <c r="BE21" s="81"/>
-      <c r="BF21" s="79"/>
+      <c r="BE21" s="76"/>
+      <c r="BF21" s="74"/>
       <c r="BG21" s="58"/>
       <c r="BH21" s="58"/>
-      <c r="BI21" s="81"/>
-      <c r="BJ21" s="79"/>
+      <c r="BI21" s="76"/>
+      <c r="BJ21" s="74"/>
       <c r="BK21" s="58"/>
       <c r="BL21" s="58"/>
-      <c r="BM21" s="81"/>
-      <c r="BN21" s="79"/>
+      <c r="BM21" s="76"/>
+      <c r="BN21" s="74"/>
     </row>
     <row r="22" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D22" s="24"/>
@@ -8102,7 +10017,7 @@
       </c>
       <c r="AI22" s="11"/>
       <c r="AJ22" s="11">
-        <v>0.86</v>
+        <v>0.09</v>
       </c>
       <c r="AK22" s="11"/>
       <c r="AL22" s="11">
@@ -8124,16 +10039,16 @@
       <c r="BB22" s="57"/>
       <c r="BC22" s="57"/>
       <c r="BD22" s="58"/>
-      <c r="BE22" s="81"/>
-      <c r="BF22" s="79"/>
+      <c r="BE22" s="76"/>
+      <c r="BF22" s="74"/>
       <c r="BG22" s="58"/>
       <c r="BH22" s="58"/>
-      <c r="BI22" s="81"/>
-      <c r="BJ22" s="79"/>
+      <c r="BI22" s="76"/>
+      <c r="BJ22" s="74"/>
       <c r="BK22" s="58"/>
       <c r="BL22" s="58"/>
-      <c r="BM22" s="81"/>
-      <c r="BN22" s="79"/>
+      <c r="BM22" s="76"/>
+      <c r="BN22" s="74"/>
     </row>
     <row r="23" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D23" s="24"/>
@@ -8220,16 +10135,16 @@
       <c r="BB23" s="57"/>
       <c r="BC23" s="57"/>
       <c r="BD23" s="58"/>
-      <c r="BE23" s="81"/>
-      <c r="BF23" s="79"/>
+      <c r="BE23" s="76"/>
+      <c r="BF23" s="74"/>
       <c r="BG23" s="58"/>
       <c r="BH23" s="58"/>
-      <c r="BI23" s="81"/>
-      <c r="BJ23" s="79"/>
+      <c r="BI23" s="76"/>
+      <c r="BJ23" s="74"/>
       <c r="BK23" s="58"/>
       <c r="BL23" s="58"/>
-      <c r="BM23" s="81"/>
-      <c r="BN23" s="79"/>
+      <c r="BM23" s="76"/>
+      <c r="BN23" s="74"/>
     </row>
     <row r="24" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D24" s="24"/>
@@ -8316,16 +10231,16 @@
       <c r="BB24" s="57"/>
       <c r="BC24" s="57"/>
       <c r="BD24" s="58"/>
-      <c r="BE24" s="81"/>
-      <c r="BF24" s="79"/>
+      <c r="BE24" s="76"/>
+      <c r="BF24" s="74"/>
       <c r="BG24" s="58"/>
       <c r="BH24" s="58"/>
-      <c r="BI24" s="81"/>
-      <c r="BJ24" s="79"/>
+      <c r="BI24" s="76"/>
+      <c r="BJ24" s="74"/>
       <c r="BK24" s="58"/>
       <c r="BL24" s="58"/>
-      <c r="BM24" s="81"/>
-      <c r="BN24" s="79"/>
+      <c r="BM24" s="76"/>
+      <c r="BN24" s="74"/>
     </row>
     <row r="25" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D25" s="24"/>
@@ -8412,16 +10327,16 @@
       <c r="BB25" s="57"/>
       <c r="BC25" s="57"/>
       <c r="BD25" s="58"/>
-      <c r="BE25" s="81"/>
-      <c r="BF25" s="79"/>
+      <c r="BE25" s="76"/>
+      <c r="BF25" s="74"/>
       <c r="BG25" s="58"/>
       <c r="BH25" s="58"/>
-      <c r="BI25" s="81"/>
-      <c r="BJ25" s="79"/>
+      <c r="BI25" s="76"/>
+      <c r="BJ25" s="74"/>
       <c r="BK25" s="58"/>
       <c r="BL25" s="58"/>
-      <c r="BM25" s="81"/>
-      <c r="BN25" s="79"/>
+      <c r="BM25" s="76"/>
+      <c r="BN25" s="74"/>
     </row>
     <row r="26" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D26" s="24"/>
@@ -8508,16 +10423,16 @@
       <c r="BB26" s="57"/>
       <c r="BC26" s="57"/>
       <c r="BD26" s="58"/>
-      <c r="BE26" s="81"/>
-      <c r="BF26" s="79"/>
+      <c r="BE26" s="76"/>
+      <c r="BF26" s="74"/>
       <c r="BG26" s="58"/>
       <c r="BH26" s="58"/>
-      <c r="BI26" s="81"/>
-      <c r="BJ26" s="79"/>
+      <c r="BI26" s="76"/>
+      <c r="BJ26" s="74"/>
       <c r="BK26" s="58"/>
       <c r="BL26" s="58"/>
-      <c r="BM26" s="81"/>
-      <c r="BN26" s="79"/>
+      <c r="BM26" s="76"/>
+      <c r="BN26" s="74"/>
     </row>
     <row r="27" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D27" s="24"/>
@@ -8604,16 +10519,16 @@
       <c r="BB27" s="57"/>
       <c r="BC27" s="57"/>
       <c r="BD27" s="58"/>
-      <c r="BE27" s="81"/>
-      <c r="BF27" s="79"/>
+      <c r="BE27" s="76"/>
+      <c r="BF27" s="74"/>
       <c r="BG27" s="58"/>
       <c r="BH27" s="58"/>
-      <c r="BI27" s="81"/>
-      <c r="BJ27" s="79"/>
+      <c r="BI27" s="76"/>
+      <c r="BJ27" s="74"/>
       <c r="BK27" s="58"/>
       <c r="BL27" s="58"/>
-      <c r="BM27" s="81"/>
-      <c r="BN27" s="79"/>
+      <c r="BM27" s="76"/>
+      <c r="BN27" s="74"/>
     </row>
     <row r="28" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D28" s="24"/>
@@ -8700,16 +10615,16 @@
       <c r="BB28" s="57"/>
       <c r="BC28" s="57"/>
       <c r="BD28" s="58"/>
-      <c r="BE28" s="81"/>
-      <c r="BF28" s="79"/>
+      <c r="BE28" s="76"/>
+      <c r="BF28" s="74"/>
       <c r="BG28" s="58"/>
       <c r="BH28" s="58"/>
-      <c r="BI28" s="81"/>
-      <c r="BJ28" s="79"/>
+      <c r="BI28" s="76"/>
+      <c r="BJ28" s="74"/>
       <c r="BK28" s="58"/>
       <c r="BL28" s="58"/>
-      <c r="BM28" s="81"/>
-      <c r="BN28" s="79"/>
+      <c r="BM28" s="76"/>
+      <c r="BN28" s="74"/>
     </row>
     <row r="29" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D29" s="24"/>
@@ -8796,16 +10711,16 @@
       <c r="BB29" s="57"/>
       <c r="BC29" s="57"/>
       <c r="BD29" s="58"/>
-      <c r="BE29" s="81"/>
-      <c r="BF29" s="79"/>
+      <c r="BE29" s="76"/>
+      <c r="BF29" s="74"/>
       <c r="BG29" s="58"/>
       <c r="BH29" s="58"/>
-      <c r="BI29" s="81"/>
-      <c r="BJ29" s="79"/>
+      <c r="BI29" s="76"/>
+      <c r="BJ29" s="74"/>
       <c r="BK29" s="58"/>
       <c r="BL29" s="58"/>
-      <c r="BM29" s="81"/>
-      <c r="BN29" s="79"/>
+      <c r="BM29" s="76"/>
+      <c r="BN29" s="74"/>
     </row>
     <row r="30" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D30" s="24"/>
@@ -8892,27 +10807,24 @@
       <c r="BB30" s="57"/>
       <c r="BC30" s="57"/>
       <c r="BD30" s="58"/>
-      <c r="BE30" s="81"/>
-      <c r="BF30" s="79"/>
+      <c r="BE30" s="76"/>
+      <c r="BF30" s="74"/>
       <c r="BG30" s="58"/>
       <c r="BH30" s="58"/>
-      <c r="BI30" s="81"/>
-      <c r="BJ30" s="79"/>
+      <c r="BI30" s="76"/>
+      <c r="BJ30" s="74"/>
       <c r="BK30" s="58"/>
       <c r="BL30" s="58"/>
-      <c r="BM30" s="81"/>
-      <c r="BN30" s="79"/>
+      <c r="BM30" s="76"/>
+      <c r="BN30" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="S7:W7"/>
-    <mergeCell ref="AB6:AR6"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="AH7:AL7"/>
     <mergeCell ref="AN7:AR7"/>
     <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="BD6:BN6"/>
     <mergeCell ref="BA10:BB10"/>
     <mergeCell ref="BA11:BB11"/>
@@ -8920,1365 +10832,12 @@
     <mergeCell ref="G6:W6"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB6589B6-0C3E-46EB-9A34-8AB789243ADA}">
-  <dimension ref="C1:W15"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" t="s">
-        <v>334</v>
-      </c>
-      <c r="N2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="3" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>341</v>
-      </c>
-      <c r="D3" t="s">
-        <v>342</v>
-      </c>
-      <c r="E3" t="s">
-        <v>343</v>
-      </c>
-      <c r="F3" t="s">
-        <v>270</v>
-      </c>
-      <c r="G3" t="s">
-        <v>271</v>
-      </c>
-      <c r="H3" t="s">
-        <v>272</v>
-      </c>
-      <c r="I3" t="s">
-        <v>332</v>
-      </c>
-      <c r="J3" t="s">
-        <v>333</v>
-      </c>
-      <c r="K3" t="s">
-        <v>336</v>
-      </c>
-      <c r="L3" t="s">
-        <v>337</v>
-      </c>
-      <c r="M3" t="s">
-        <v>338</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3">
-        <v>5</v>
-      </c>
-      <c r="S3">
-        <v>6</v>
-      </c>
-      <c r="T3">
-        <v>7</v>
-      </c>
-      <c r="U3">
-        <v>8</v>
-      </c>
-      <c r="V3">
-        <v>9</v>
-      </c>
-      <c r="W3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E4" s="36">
-        <v>-0.18870000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E5" s="36">
-        <v>0.57339390000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="41" t="s">
-        <v>340</v>
-      </c>
-      <c r="E6" s="36">
-        <v>-1.032214</v>
-      </c>
-    </row>
-    <row r="7" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="E7" s="36">
-        <v>0.36380000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E8" s="36">
-        <v>4.1099999999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="D9" s="25" t="s">
-        <v>339</v>
-      </c>
-      <c r="E9" s="36">
-        <v>0.49000709999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="41" t="s">
-        <v>340</v>
-      </c>
-      <c r="E10" s="36">
-        <v>-0.440552</v>
-      </c>
-    </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="D11" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="E11" s="36">
-        <v>0.57040000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E12" s="36">
-        <v>-1.9599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="D13" s="41" t="s">
-        <v>339</v>
-      </c>
-      <c r="E13" s="36">
-        <v>0.29692429999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="41" t="s">
-        <v>340</v>
-      </c>
-      <c r="E14" s="36">
-        <v>-0.3664499</v>
-      </c>
-    </row>
-    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="D15" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="E15" s="36">
-        <v>0.47920000000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C71D8DF-2DF6-476F-91B9-DD47201B35C2}">
-  <dimension ref="D3:AB30"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O30" sqref="D2:P30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="74" t="s">
-        <v>253</v>
-      </c>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="74"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="35"/>
-      <c r="S3" s="74" t="s">
-        <v>258</v>
-      </c>
-      <c r="T3" s="74"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="74"/>
-      <c r="W3" s="74"/>
-      <c r="X3" s="74"/>
-      <c r="Y3" s="74"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
-    </row>
-    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="F4" s="13"/>
-      <c r="G4" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="H4" t="s">
-        <v>261</v>
-      </c>
-      <c r="I4" s="24">
-        <v>3918</v>
-      </c>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="O4" s="24">
-        <v>611</v>
-      </c>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="T4" s="41" t="s">
-        <v>261</v>
-      </c>
-      <c r="U4" s="24">
-        <v>23047018</v>
-      </c>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="Z4" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="AA4" s="24">
-        <v>2359143</v>
-      </c>
-      <c r="AB4" s="23">
-        <f>AA4/SUM(U4,AA4)</f>
-        <v>9.2857122333437153E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="F5" s="24"/>
-      <c r="G5" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="I5" s="31"/>
-      <c r="K5" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="N5" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="O5" s="31"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="U5" s="40"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="Z5" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="AA5" s="40"/>
-      <c r="AB5" s="41"/>
-    </row>
-    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="76" t="s">
-        <v>257</v>
-      </c>
-      <c r="E6" s="76"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-    </row>
-    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="77" t="s">
-        <v>319</v>
-      </c>
-      <c r="E7" s="77"/>
-      <c r="G7">
-        <v>127.98</v>
-      </c>
-      <c r="H7" s="36">
-        <v>18.384840000000001</v>
-      </c>
-      <c r="M7">
-        <v>128.34</v>
-      </c>
-      <c r="N7" s="36">
-        <v>19.25619</v>
-      </c>
-      <c r="S7" s="41">
-        <v>126.923238</v>
-      </c>
-      <c r="T7" s="36">
-        <v>18.110648999999999</v>
-      </c>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41">
-        <v>126.06586059999999</v>
-      </c>
-      <c r="Z7" s="37">
-        <v>18.439636100000001</v>
-      </c>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-    </row>
-    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G8">
-        <v>29.6</v>
-      </c>
-      <c r="H8" s="36">
-        <v>5.9282329999999996</v>
-      </c>
-      <c r="M8">
-        <v>30.76</v>
-      </c>
-      <c r="N8" s="36">
-        <v>6.3475760000000001</v>
-      </c>
-      <c r="S8" s="36">
-        <v>29.662302499999999</v>
-      </c>
-      <c r="T8" s="36">
-        <v>5.9267823000000002</v>
-      </c>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41">
-        <v>29.959577500000002</v>
-      </c>
-      <c r="Z8" s="37">
-        <v>6.2308531</v>
-      </c>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41"/>
-    </row>
-    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="77"/>
-      <c r="G9">
-        <v>40.1</v>
-      </c>
-      <c r="H9" s="36">
-        <v>5.7592100000000004</v>
-      </c>
-      <c r="M9">
-        <v>40.619999999999997</v>
-      </c>
-      <c r="N9" s="36">
-        <v>5.5369099999999998</v>
-      </c>
-      <c r="S9" s="36">
-        <v>40.103714400000001</v>
-      </c>
-      <c r="T9" s="36">
-        <v>5.8665503000000001</v>
-      </c>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="36">
-        <v>40.107512399999997</v>
-      </c>
-      <c r="Z9" s="37">
-        <v>5.6566346999999997</v>
-      </c>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="41"/>
-    </row>
-    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="S10" s="41"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-    </row>
-    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D11" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="S11" s="41"/>
-      <c r="T11" s="36"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="37"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
-    </row>
-    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D12" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="37">
-        <v>70.12</v>
-      </c>
-      <c r="H12" s="37">
-        <v>9.8203709999999997</v>
-      </c>
-      <c r="M12" s="37">
-        <v>65.349999999999994</v>
-      </c>
-      <c r="N12" s="37">
-        <v>8.5174970000000005</v>
-      </c>
-      <c r="S12" s="37">
-        <v>67.901583500000001</v>
-      </c>
-      <c r="T12" s="36">
-        <v>9.2750620000000001</v>
-      </c>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="37">
-        <v>64.861546799999999</v>
-      </c>
-      <c r="Z12" s="37">
-        <v>8.3972078000000003</v>
-      </c>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-    </row>
-    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D13" s="24"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="37"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-    </row>
-    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D14" s="24"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-    </row>
-    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D15" s="24"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-    </row>
-    <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="76" t="s">
-        <v>315</v>
-      </c>
-      <c r="E16" s="76"/>
-      <c r="G16" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>314</v>
-      </c>
-      <c r="M16" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="N16" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="O16" s="38" t="s">
-        <v>314</v>
-      </c>
-      <c r="S16" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="T16" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="U16" s="40" t="s">
-        <v>314</v>
-      </c>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="Z16" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA16" s="38" t="s">
-        <v>314</v>
-      </c>
-      <c r="AB16" s="41"/>
-    </row>
-    <row r="17" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D17" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="G17">
-        <f>H17*I4</f>
-        <v>1578.9540000000002</v>
-      </c>
-      <c r="H17" s="26">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="M17" s="39">
-        <f>N17*O4</f>
-        <v>267.00700000000001</v>
-      </c>
-      <c r="N17" s="23">
-        <v>0.437</v>
-      </c>
-      <c r="S17" s="47">
-        <f>T17*U4</f>
-        <v>9945516.5527688004</v>
-      </c>
-      <c r="T17" s="26">
-        <v>0.43153160000000002</v>
-      </c>
-      <c r="U17" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="39">
-        <f>Z17*AA4</f>
-        <v>1143629.0127377999</v>
-      </c>
-      <c r="Z17" s="23">
-        <v>0.48476459999999999</v>
-      </c>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="41"/>
-    </row>
-    <row r="18" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D18" s="24" t="s">
-        <v>269</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="G18">
-        <v>3246</v>
-      </c>
-      <c r="H18" s="23">
-        <f t="shared" ref="H18:H30" si="0">G18/$I$4</f>
-        <v>0.82848392036753449</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="M18">
-        <v>187</v>
-      </c>
-      <c r="N18" s="23">
-        <f>M18/$O$4</f>
-        <v>0.30605564648117839</v>
-      </c>
-      <c r="S18" s="47">
-        <v>20959837</v>
-      </c>
-      <c r="T18" s="23">
-        <f t="shared" ref="T18:T30" si="1">S18/$U$4</f>
-        <v>0.90943813208285773</v>
-      </c>
-      <c r="U18" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="V18" s="41"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="41"/>
-      <c r="Y18" s="41">
-        <v>1054148</v>
-      </c>
-      <c r="Z18" s="46">
-        <f t="shared" ref="Z18:Z30" si="2">Y18/$AA$4</f>
-        <v>0.44683514310069378</v>
-      </c>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="41"/>
-    </row>
-    <row r="19" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D19" s="27"/>
-      <c r="E19" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="G19">
-        <v>445</v>
-      </c>
-      <c r="H19" s="23">
-        <f t="shared" si="0"/>
-        <v>0.11357835630423685</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="M19">
-        <v>323</v>
-      </c>
-      <c r="N19" s="23">
-        <f t="shared" ref="N19:N20" si="3">M19/$O$4</f>
-        <v>0.52864157119476274</v>
-      </c>
-      <c r="S19" s="47">
-        <v>1137593</v>
-      </c>
-      <c r="T19" s="23">
-        <f t="shared" si="1"/>
-        <v>4.9359661193478482E-2</v>
-      </c>
-      <c r="U19" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="V19" s="41"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
-      <c r="Y19" s="41">
-        <v>877192</v>
-      </c>
-      <c r="Z19" s="23">
-        <f t="shared" si="2"/>
-        <v>0.37182654887813077</v>
-      </c>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="41"/>
-    </row>
-    <row r="20" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D20" s="27"/>
-      <c r="E20" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="G20">
-        <v>227</v>
-      </c>
-      <c r="H20" s="23">
-        <f t="shared" si="0"/>
-        <v>5.7937723328228691E-2</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="M20">
-        <v>101</v>
-      </c>
-      <c r="N20" s="23">
-        <f t="shared" si="3"/>
-        <v>0.16530278232405893</v>
-      </c>
-      <c r="S20" s="47">
-        <v>949588</v>
-      </c>
-      <c r="T20" s="23">
-        <f t="shared" si="1"/>
-        <v>4.1202206723663773E-2</v>
-      </c>
-      <c r="U20" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="41"/>
-      <c r="Y20" s="41">
-        <v>427803</v>
-      </c>
-      <c r="Z20" s="23">
-        <f t="shared" si="2"/>
-        <v>0.18133830802117548</v>
-      </c>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="41"/>
-    </row>
-    <row r="21" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D21" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>339</v>
-      </c>
-      <c r="H21" s="23">
-        <f t="shared" si="0"/>
-        <v>8.6523736600306281E-2</v>
-      </c>
-      <c r="I21" s="26">
-        <f>SUM($H$21)</f>
-        <v>8.6523736600306281E-2</v>
-      </c>
-      <c r="M21">
-        <v>110</v>
-      </c>
-      <c r="N21" s="23">
-        <f t="shared" ref="N21:N30" si="4">M21/$O$4</f>
-        <v>0.18003273322422259</v>
-      </c>
-      <c r="O21" s="26">
-        <f>N21</f>
-        <v>0.18003273322422259</v>
-      </c>
-      <c r="S21" s="47">
-        <v>1559571</v>
-      </c>
-      <c r="T21" s="23">
-        <f t="shared" si="1"/>
-        <v>6.7669101486361488E-2</v>
-      </c>
-      <c r="U21" s="26">
-        <f>SUM($T$21)</f>
-        <v>6.7669101486361488E-2</v>
-      </c>
-      <c r="V21" s="41"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="41"/>
-      <c r="Y21" s="41">
-        <v>404485</v>
-      </c>
-      <c r="Z21" s="23">
-        <f t="shared" si="2"/>
-        <v>0.17145421027890212</v>
-      </c>
-      <c r="AA21" s="23">
-        <f>Z21</f>
-        <v>0.17145421027890212</v>
-      </c>
-      <c r="AB21" s="41"/>
-    </row>
-    <row r="22" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D22" s="24"/>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>342</v>
-      </c>
-      <c r="H22" s="23">
-        <f t="shared" si="0"/>
-        <v>8.7289433384379791E-2</v>
-      </c>
-      <c r="I22" s="26">
-        <f>SUM($H$21:$H22)</f>
-        <v>0.17381316998468607</v>
-      </c>
-      <c r="M22">
-        <v>92</v>
-      </c>
-      <c r="N22" s="23">
-        <f t="shared" si="4"/>
-        <v>0.15057283142389524</v>
-      </c>
-      <c r="O22" s="26">
-        <f>SUM($N$21:N22)</f>
-        <v>0.33060556464811786</v>
-      </c>
-      <c r="S22" s="47">
-        <v>1461268</v>
-      </c>
-      <c r="T22" s="23">
-        <f t="shared" si="1"/>
-        <v>6.3403777443138201E-2</v>
-      </c>
-      <c r="U22" s="26">
-        <f>SUM($T$21:$T22)</f>
-        <v>0.1310728789294997</v>
-      </c>
-      <c r="V22" s="41"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="41">
-        <v>240757</v>
-      </c>
-      <c r="Z22" s="23">
-        <f t="shared" si="2"/>
-        <v>0.10205273694727281</v>
-      </c>
-      <c r="AA22" s="23">
-        <f>SUM($Z$21:Z22)</f>
-        <v>0.27350694722617491</v>
-      </c>
-      <c r="AB22" s="41"/>
-    </row>
-    <row r="23" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D23" s="24"/>
-      <c r="E23">
-        <v>3</v>
-      </c>
-      <c r="G23">
-        <v>365</v>
-      </c>
-      <c r="H23" s="23">
-        <f t="shared" si="0"/>
-        <v>9.3159775395610003E-2</v>
-      </c>
-      <c r="I23" s="26">
-        <f>SUM($H$21:$H23)</f>
-        <v>0.26697294538029609</v>
-      </c>
-      <c r="M23">
-        <v>87</v>
-      </c>
-      <c r="N23" s="23">
-        <f t="shared" si="4"/>
-        <v>0.14238952536824878</v>
-      </c>
-      <c r="O23" s="26">
-        <f>SUM($N$21:N23)</f>
-        <v>0.47299509001636664</v>
-      </c>
-      <c r="S23" s="47">
-        <v>2051140</v>
-      </c>
-      <c r="T23" s="23">
-        <f t="shared" si="1"/>
-        <v>8.8998064738787463E-2</v>
-      </c>
-      <c r="U23" s="26">
-        <f>SUM($T$21:$T23)</f>
-        <v>0.22007094366828717</v>
-      </c>
-      <c r="V23" s="41"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="41">
-        <v>339098</v>
-      </c>
-      <c r="Z23" s="23">
-        <f t="shared" si="2"/>
-        <v>0.14373778952780733</v>
-      </c>
-      <c r="AA23" s="23">
-        <f>SUM($Z$21:Z23)</f>
-        <v>0.41724473675398221</v>
-      </c>
-      <c r="AB23" s="41"/>
-    </row>
-    <row r="24" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D24" s="24"/>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="G24">
-        <v>368</v>
-      </c>
-      <c r="H24" s="23">
-        <f t="shared" si="0"/>
-        <v>9.3925472179683514E-2</v>
-      </c>
-      <c r="I24" s="26">
-        <f>SUM($H$21:$H24)</f>
-        <v>0.36089841755997959</v>
-      </c>
-      <c r="M24">
-        <v>83</v>
-      </c>
-      <c r="N24" s="23">
-        <f t="shared" si="4"/>
-        <v>0.13584288052373159</v>
-      </c>
-      <c r="O24" s="26">
-        <f>SUM($N$21:N24)</f>
-        <v>0.60883797054009825</v>
-      </c>
-      <c r="S24" s="47">
-        <v>2002854</v>
-      </c>
-      <c r="T24" s="23">
-        <f t="shared" si="1"/>
-        <v>8.6902956382469962E-2</v>
-      </c>
-      <c r="U24" s="26">
-        <f>SUM($T$21:$T24)</f>
-        <v>0.30697390005075714</v>
-      </c>
-      <c r="V24" s="41"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
-      <c r="Y24" s="41">
-        <v>311698</v>
-      </c>
-      <c r="Z24" s="23">
-        <f t="shared" si="2"/>
-        <v>0.1321234024389365</v>
-      </c>
-      <c r="AA24" s="23">
-        <f>SUM($Z$21:Z24)</f>
-        <v>0.54936813919291871</v>
-      </c>
-      <c r="AB24" s="41"/>
-    </row>
-    <row r="25" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D25" s="24"/>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <v>397</v>
-      </c>
-      <c r="H25" s="23">
-        <f t="shared" si="0"/>
-        <v>0.10132720775906075</v>
-      </c>
-      <c r="I25" s="26">
-        <f>SUM($H$21:$H25)</f>
-        <v>0.46222562531904032</v>
-      </c>
-      <c r="M25">
-        <v>61</v>
-      </c>
-      <c r="N25" s="23">
-        <f t="shared" si="4"/>
-        <v>9.9836333878887074E-2</v>
-      </c>
-      <c r="O25" s="26">
-        <f>SUM($N$21:N25)</f>
-        <v>0.70867430441898538</v>
-      </c>
-      <c r="S25" s="47">
-        <v>2308963</v>
-      </c>
-      <c r="T25" s="23">
-        <f t="shared" si="1"/>
-        <v>0.10018489159855735</v>
-      </c>
-      <c r="U25" s="26">
-        <f>SUM($T$21:$T25)</f>
-        <v>0.40715879164931451</v>
-      </c>
-      <c r="V25" s="41"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="41">
-        <v>183943</v>
-      </c>
-      <c r="Z25" s="23">
-        <f t="shared" si="2"/>
-        <v>7.797026293022509E-2</v>
-      </c>
-      <c r="AA25" s="23">
-        <f>SUM($Z$21:Z25)</f>
-        <v>0.62733840212314385</v>
-      </c>
-      <c r="AB25" s="41"/>
-    </row>
-    <row r="26" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D26" s="24"/>
-      <c r="E26">
-        <v>6</v>
-      </c>
-      <c r="G26">
-        <v>412</v>
-      </c>
-      <c r="H26" s="23">
-        <f t="shared" si="0"/>
-        <v>0.10515569167942827</v>
-      </c>
-      <c r="I26" s="26">
-        <f>SUM($H$21:$H26)</f>
-        <v>0.56738131699846861</v>
-      </c>
-      <c r="M26">
-        <v>42</v>
-      </c>
-      <c r="N26" s="23">
-        <f t="shared" si="4"/>
-        <v>6.8739770867430439E-2</v>
-      </c>
-      <c r="O26" s="26">
-        <f>SUM($N$21:N26)</f>
-        <v>0.77741407528641582</v>
-      </c>
-      <c r="S26" s="47">
-        <v>2389812</v>
-      </c>
-      <c r="T26" s="23">
-        <f t="shared" si="1"/>
-        <v>0.10369289423907249</v>
-      </c>
-      <c r="U26" s="26">
-        <f>SUM($T$21:$T26)</f>
-        <v>0.51085168588838703</v>
-      </c>
-      <c r="V26" s="41"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="41"/>
-      <c r="Y26" s="41">
-        <v>153145</v>
-      </c>
-      <c r="Z26" s="23">
-        <f t="shared" si="2"/>
-        <v>6.4915522289238081E-2</v>
-      </c>
-      <c r="AA26" s="23">
-        <f>SUM($Z$21:Z26)</f>
-        <v>0.69225392441238198</v>
-      </c>
-      <c r="AB26" s="41"/>
-    </row>
-    <row r="27" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D27" s="24"/>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="G27">
-        <v>414</v>
-      </c>
-      <c r="H27" s="23">
-        <f t="shared" si="0"/>
-        <v>0.10566615620214395</v>
-      </c>
-      <c r="I27" s="26">
-        <f>SUM($H$21:$H27)</f>
-        <v>0.67304747320061253</v>
-      </c>
-      <c r="M27">
-        <v>43</v>
-      </c>
-      <c r="N27" s="23">
-        <f t="shared" si="4"/>
-        <v>7.0376432078559745E-2</v>
-      </c>
-      <c r="O27" s="26">
-        <f>SUM($N$21:N27)</f>
-        <v>0.84779050736497552</v>
-      </c>
-      <c r="S27" s="47">
-        <v>2556546</v>
-      </c>
-      <c r="T27" s="23">
-        <f t="shared" si="1"/>
-        <v>0.11092740935074551</v>
-      </c>
-      <c r="U27" s="26">
-        <f>SUM($T$21:$T27)</f>
-        <v>0.62177909523913255</v>
-      </c>
-      <c r="V27" s="41"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
-      <c r="Y27" s="41">
-        <v>171274</v>
-      </c>
-      <c r="Z27" s="23">
-        <f t="shared" si="2"/>
-        <v>7.2600092491213977E-2</v>
-      </c>
-      <c r="AA27" s="23">
-        <f>SUM($Z$21:Z27)</f>
-        <v>0.764854016903596</v>
-      </c>
-      <c r="AB27" s="41"/>
-    </row>
-    <row r="28" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D28" s="24"/>
-      <c r="E28">
-        <v>8</v>
-      </c>
-      <c r="G28">
-        <v>426</v>
-      </c>
-      <c r="H28" s="23">
-        <f t="shared" si="0"/>
-        <v>0.10872894333843798</v>
-      </c>
-      <c r="I28" s="26">
-        <f>SUM($H$21:$H28)</f>
-        <v>0.7817764165390505</v>
-      </c>
-      <c r="M28">
-        <v>30</v>
-      </c>
-      <c r="N28" s="23">
-        <f t="shared" si="4"/>
-        <v>4.9099836333878884E-2</v>
-      </c>
-      <c r="O28" s="26">
-        <f>SUM($N$21:N28)</f>
-        <v>0.89689034369885445</v>
-      </c>
-      <c r="S28" s="47">
-        <v>2805331</v>
-      </c>
-      <c r="T28" s="23">
-        <f t="shared" si="1"/>
-        <v>0.12172208135560098</v>
-      </c>
-      <c r="U28" s="26">
-        <f>SUM($T$21:$T28)</f>
-        <v>0.74350117659473347</v>
-      </c>
-      <c r="V28" s="41"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41">
-        <v>127970</v>
-      </c>
-      <c r="Z28" s="23">
-        <f t="shared" si="2"/>
-        <v>5.4244274297912419E-2</v>
-      </c>
-      <c r="AA28" s="23">
-        <f>SUM($Z$21:Z28)</f>
-        <v>0.81909829120150845</v>
-      </c>
-      <c r="AB28" s="41"/>
-    </row>
-    <row r="29" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D29" s="24"/>
-      <c r="E29">
-        <v>9</v>
-      </c>
-      <c r="G29">
-        <v>421</v>
-      </c>
-      <c r="H29" s="23">
-        <f t="shared" si="0"/>
-        <v>0.10745278203164881</v>
-      </c>
-      <c r="I29" s="26">
-        <f>SUM($H$21:$H29)</f>
-        <v>0.88922919857069926</v>
-      </c>
-      <c r="M29">
-        <v>38</v>
-      </c>
-      <c r="N29" s="23">
-        <f t="shared" si="4"/>
-        <v>6.2193126022913256E-2</v>
-      </c>
-      <c r="O29" s="26">
-        <f>SUM($N$21:N29)</f>
-        <v>0.95908346972176772</v>
-      </c>
-      <c r="S29" s="47">
-        <v>2756844</v>
-      </c>
-      <c r="T29" s="23">
-        <f t="shared" si="1"/>
-        <v>0.11961825169746472</v>
-      </c>
-      <c r="U29" s="26">
-        <f>SUM($T$21:$T29)</f>
-        <v>0.86311942829219823</v>
-      </c>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41">
-        <v>274731</v>
-      </c>
-      <c r="Z29" s="23">
-        <f t="shared" si="2"/>
-        <v>0.11645372917199169</v>
-      </c>
-      <c r="AA29" s="23">
-        <f>SUM($Z$21:Z29)</f>
-        <v>0.93555202037350016</v>
-      </c>
-      <c r="AB29" s="41"/>
-    </row>
-    <row r="30" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D30" s="24"/>
-      <c r="E30">
-        <v>10</v>
-      </c>
-      <c r="G30">
-        <v>434</v>
-      </c>
-      <c r="H30" s="23">
-        <f t="shared" si="0"/>
-        <v>0.11077080142930067</v>
-      </c>
-      <c r="I30" s="26">
-        <f>SUM($H$21:$H30)</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="M30">
-        <v>25</v>
-      </c>
-      <c r="N30" s="23">
-        <f t="shared" si="4"/>
-        <v>4.0916530278232409E-2</v>
-      </c>
-      <c r="O30" s="26">
-        <f>SUM($N$21:N30)</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="S30" s="47">
-        <v>3154689</v>
-      </c>
-      <c r="T30" s="23">
-        <f t="shared" si="1"/>
-        <v>0.13688057170780185</v>
-      </c>
-      <c r="U30" s="26">
-        <f>SUM($T$21:$T30)</f>
-        <v>1</v>
-      </c>
-      <c r="V30" s="41"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="41"/>
-      <c r="Y30" s="41">
-        <v>152042</v>
-      </c>
-      <c r="Z30" s="23">
-        <f t="shared" si="2"/>
-        <v>6.4447979626499965E-2</v>
-      </c>
-      <c r="AA30" s="23">
-        <f>SUM($Z$21:Z30)</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="AB30" s="41"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="S3:AB3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G3:P3"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="S7:W7"/>
+    <mergeCell ref="AB6:AR6"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="AH7:AL7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update discussion code and tables in excel
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE2090B-1BA1-416B-8EEE-C60D75C64070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7E4FE7-6BE9-4316-9118-EB56CDF96752}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="570" windowWidth="24480" windowHeight="10080" activeTab="4" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
@@ -1480,12 +1480,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -3161,10 +3161,10 @@
       <c r="AB5" s="41"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="85" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="84"/>
+      <c r="E6" s="85"/>
       <c r="S6" s="41"/>
       <c r="T6" s="41"/>
       <c r="U6" s="41"/>
@@ -3177,10 +3177,10 @@
       <c r="AB6" s="41"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="86"/>
+      <c r="E7" s="87"/>
       <c r="G7">
         <v>127.98</v>
       </c>
@@ -3248,10 +3248,10 @@
       <c r="AB8" s="41"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="86"/>
+      <c r="E9" s="87"/>
       <c r="G9">
         <v>40.1</v>
       </c>
@@ -3388,10 +3388,10 @@
       <c r="AB15" s="41"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="84" t="s">
+      <c r="D16" s="85" t="s">
         <v>315</v>
       </c>
-      <c r="E16" s="84"/>
+      <c r="E16" s="85"/>
       <c r="G16" s="33" t="s">
         <v>313</v>
       </c>
@@ -4311,16 +4311,16 @@
       <c r="AA5" s="50"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="85" t="s">
         <v>346</v>
       </c>
-      <c r="E6" s="84"/>
+      <c r="E6" s="85"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="86"/>
+      <c r="E7" s="87"/>
       <c r="G7" s="70">
         <v>-0.13370000000000001</v>
       </c>
@@ -4404,10 +4404,10 @@
       <c r="AB8" s="58"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="86"/>
+      <c r="E9" s="87"/>
       <c r="G9" s="70">
         <v>0.46750000000000003</v>
       </c>
@@ -4560,10 +4560,10 @@
       <c r="U15" s="30"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="84" t="s">
+      <c r="D16" s="85" t="s">
         <v>315</v>
       </c>
-      <c r="E16" s="84"/>
+      <c r="E16" s="85"/>
       <c r="G16" s="33" t="s">
         <v>313</v>
       </c>
@@ -6791,8 +6791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
   <dimension ref="C2:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7114,7 +7114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E776B9-4EC5-46CF-B1E5-E124814149F5}">
   <dimension ref="A2:K13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -8554,18 +8554,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="Q12:S12"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="M11:S11"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="E2:K2"/>
     <mergeCell ref="M2:S2"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="Q12:S12"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="M11:S11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -8665,52 +8665,52 @@
       <c r="BN6" s="82"/>
     </row>
     <row r="7" spans="4:66" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="84" t="s">
         <v>264</v>
       </c>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
       <c r="L7" s="35"/>
-      <c r="M7" s="87" t="s">
+      <c r="M7" s="84" t="s">
         <v>164</v>
       </c>
-      <c r="N7" s="87"/>
-      <c r="O7" s="87"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="87"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="84"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="84"/>
       <c r="R7" s="35"/>
-      <c r="S7" s="87" t="s">
+      <c r="S7" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="87"/>
-      <c r="U7" s="87"/>
-      <c r="V7" s="87"/>
-      <c r="W7" s="87"/>
-      <c r="AB7" s="87" t="s">
+      <c r="T7" s="84"/>
+      <c r="U7" s="84"/>
+      <c r="V7" s="84"/>
+      <c r="W7" s="84"/>
+      <c r="AB7" s="84" t="s">
         <v>264</v>
       </c>
-      <c r="AC7" s="87"/>
-      <c r="AD7" s="87"/>
-      <c r="AE7" s="87"/>
-      <c r="AF7" s="87"/>
+      <c r="AC7" s="84"/>
+      <c r="AD7" s="84"/>
+      <c r="AE7" s="84"/>
+      <c r="AF7" s="84"/>
       <c r="AG7" s="35"/>
-      <c r="AH7" s="87" t="s">
+      <c r="AH7" s="84" t="s">
         <v>164</v>
       </c>
-      <c r="AI7" s="87"/>
-      <c r="AJ7" s="87"/>
-      <c r="AK7" s="87"/>
-      <c r="AL7" s="87"/>
+      <c r="AI7" s="84"/>
+      <c r="AJ7" s="84"/>
+      <c r="AK7" s="84"/>
+      <c r="AL7" s="84"/>
       <c r="AM7" s="35"/>
-      <c r="AN7" s="87" t="s">
+      <c r="AN7" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="AO7" s="87"/>
-      <c r="AP7" s="87"/>
-      <c r="AQ7" s="87"/>
-      <c r="AR7" s="87"/>
+      <c r="AO7" s="84"/>
+      <c r="AP7" s="84"/>
+      <c r="AQ7" s="84"/>
+      <c r="AR7" s="84"/>
       <c r="BD7" s="35"/>
       <c r="BE7" s="35"/>
       <c r="BF7" s="35"/>
@@ -8908,10 +8908,10 @@
       <c r="BN9" s="55"/>
     </row>
     <row r="10" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="85" t="s">
         <v>354</v>
       </c>
-      <c r="E10" s="85"/>
+      <c r="E10" s="86"/>
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10" s="57"/>
@@ -8926,10 +8926,10 @@
       <c r="U10" s="57"/>
       <c r="V10" s="57"/>
       <c r="W10" s="57"/>
-      <c r="Y10" s="84" t="s">
+      <c r="Y10" s="85" t="s">
         <v>354</v>
       </c>
-      <c r="Z10" s="85"/>
+      <c r="Z10" s="86"/>
       <c r="AA10" s="57"/>
       <c r="AB10" s="57"/>
       <c r="AC10" s="57"/>
@@ -8948,8 +8948,8 @@
       <c r="AP10" s="57"/>
       <c r="AQ10" s="57"/>
       <c r="AR10" s="57"/>
-      <c r="BA10" s="84"/>
-      <c r="BB10" s="84"/>
+      <c r="BA10" s="85"/>
+      <c r="BB10" s="85"/>
       <c r="BC10" s="57"/>
       <c r="BD10" s="57"/>
       <c r="BE10" s="57"/>
@@ -8964,10 +8964,10 @@
       <c r="BN10" s="57"/>
     </row>
     <row r="11" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="87" t="s">
         <v>353</v>
       </c>
-      <c r="E11" s="86"/>
+      <c r="E11" s="87"/>
       <c r="F11" s="57"/>
       <c r="G11" s="11">
         <v>0.27</v>
@@ -9003,10 +9003,10 @@
       <c r="W11" s="11">
         <v>-0.63</v>
       </c>
-      <c r="Y11" s="86" t="s">
+      <c r="Y11" s="87" t="s">
         <v>353</v>
       </c>
-      <c r="Z11" s="86"/>
+      <c r="Z11" s="87"/>
       <c r="AA11" s="57"/>
       <c r="AB11" s="11">
         <v>1.51</v>
@@ -9043,8 +9043,8 @@
       <c r="AR11" s="11">
         <v>-0.5</v>
       </c>
-      <c r="BA11" s="86"/>
-      <c r="BB11" s="86"/>
+      <c r="BA11" s="87"/>
+      <c r="BB11" s="87"/>
       <c r="BC11" s="57"/>
       <c r="BD11" s="11"/>
       <c r="BE11" s="65"/>
@@ -9313,10 +9313,10 @@
       <c r="BN15" s="57"/>
     </row>
     <row r="16" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D16" s="84" t="s">
+      <c r="D16" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="E16" s="84"/>
+      <c r="E16" s="85"/>
       <c r="F16" s="57"/>
       <c r="G16" s="33" t="s">
         <v>356</v>
@@ -9353,10 +9353,10 @@
       <c r="W16" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="Y16" s="84" t="s">
+      <c r="Y16" s="85" t="s">
         <v>348</v>
       </c>
-      <c r="Z16" s="84"/>
+      <c r="Z16" s="85"/>
       <c r="AA16" s="57"/>
       <c r="AB16" s="33" t="s">
         <v>356</v>
@@ -9393,8 +9393,8 @@
       <c r="AR16" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="BA16" s="84"/>
-      <c r="BB16" s="84"/>
+      <c r="BA16" s="85"/>
+      <c r="BB16" s="85"/>
       <c r="BC16" s="57"/>
       <c r="BD16" s="33"/>
       <c r="BE16" s="33"/>
@@ -10820,11 +10820,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AN7:AR7"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
     <mergeCell ref="BD6:BN6"/>
     <mergeCell ref="BA10:BB10"/>
     <mergeCell ref="BA11:BB11"/>
@@ -10838,6 +10833,11 @@
     <mergeCell ref="AB6:AR6"/>
     <mergeCell ref="AB7:AF7"/>
     <mergeCell ref="AH7:AL7"/>
+    <mergeCell ref="AN7:AR7"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update tables; New CATE Graphs; update dos
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7E4FE7-6BE9-4316-9118-EB56CDF96752}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF8F2FE-F30A-4761-846A-5DA7B18A5910}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="12" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="383">
   <si>
     <t>Variable group</t>
   </si>
@@ -714,12 +714,6 @@
     <t>r11drinkn</t>
   </si>
   <si>
-    <t>double (set 99 to 7)</t>
-  </si>
-  <si>
-    <t>double (set 99 to maxvalue after 99)</t>
-  </si>
-  <si>
     <t>Drop variables with very large amounts of missing values</t>
   </si>
   <si>
@@ -1171,6 +1165,51 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>Appendix tables</t>
+  </si>
+  <si>
+    <t>RAND HRS 2016</t>
+  </si>
+  <si>
+    <t>Condition for removal observations or variable</t>
+  </si>
+  <si>
+    <t>Drop variables</t>
+  </si>
+  <si>
+    <t>nSmoke_mos, everSmoke, nSmoke_pw</t>
+  </si>
+  <si>
+    <t>Married, smokeNow</t>
+  </si>
+  <si>
+    <t>Impute variables</t>
+  </si>
+  <si>
+    <t>Education - mode</t>
+  </si>
+  <si>
+    <t>Mother Eduction - kNN</t>
+  </si>
+  <si>
+    <t>Drop if missing activity</t>
+  </si>
+  <si>
+    <t>Drop if missing smoker or drinker</t>
+  </si>
+  <si>
+    <t>Drop if missing Sex, wealth bin, race and age</t>
+  </si>
+  <si>
+    <t>Missing health outcomes or perceived discrimination, or unrelealistic health measurements: SYSBPM's &lt;30, &gt;500, wLBS of &lt;30, &gt;500, hIn of &lt;40, &gt;95, waist of &lt;15, &gt;95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropped nSmoke_mos, everSmoke, nSmoke_pw </t>
+  </si>
+  <si>
+    <t>mStat, smoker, drinker, nnDrink, nGdrink</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1379,6 +1418,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1387,7 +1437,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1473,19 +1523,27 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1806,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006A8C7B-518B-429B-BD58-DE85D1D8E44A}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="C2:H39"/>
+    <sheetView showGridLines="0" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,7 +2298,7 @@
         <v>139</v>
       </c>
       <c r="G19" t="s">
-        <v>217</v>
+        <v>99</v>
       </c>
       <c r="J19" t="s">
         <v>137</v>
@@ -2259,7 +2317,7 @@
         <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>217</v>
+        <v>99</v>
       </c>
       <c r="I20" t="s">
         <v>26</v>
@@ -2285,7 +2343,7 @@
         <v>142</v>
       </c>
       <c r="G21" t="s">
-        <v>218</v>
+        <v>99</v>
       </c>
       <c r="J21" t="s">
         <v>141</v>
@@ -2305,7 +2363,7 @@
         <v>143</v>
       </c>
       <c r="G22" t="s">
-        <v>218</v>
+        <v>99</v>
       </c>
       <c r="J22" t="s">
         <v>141</v>
@@ -2833,7 +2891,7 @@
   <sheetData>
     <row r="1" spans="3:23" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="3:23" x14ac:dyDescent="0.25">
@@ -2844,45 +2902,45 @@
         <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" t="s">
         <v>341</v>
       </c>
-      <c r="D3" t="s">
-        <v>342</v>
-      </c>
-      <c r="E3" t="s">
-        <v>343</v>
-      </c>
       <c r="F3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H3" t="s">
         <v>270</v>
       </c>
-      <c r="G3" t="s">
-        <v>271</v>
-      </c>
-      <c r="H3" t="s">
-        <v>272</v>
-      </c>
       <c r="I3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K3" t="s">
+        <v>334</v>
+      </c>
+      <c r="L3" t="s">
+        <v>335</v>
+      </c>
+      <c r="M3" t="s">
         <v>336</v>
-      </c>
-      <c r="L3" t="s">
-        <v>337</v>
-      </c>
-      <c r="M3" t="s">
-        <v>338</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -2920,7 +2978,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E4" s="36">
         <v>-0.18870000000000001</v>
@@ -2928,7 +2986,7 @@
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E5" s="36">
         <v>0.57339390000000001</v>
@@ -2936,7 +2994,7 @@
     </row>
     <row r="6" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="41" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E6" s="36">
         <v>-1.032214</v>
@@ -2944,7 +3002,7 @@
     </row>
     <row r="7" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="25" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E7" s="36">
         <v>0.36380000000000001</v>
@@ -2955,7 +3013,7 @@
         <v>164</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E8" s="36">
         <v>4.1099999999999998E-2</v>
@@ -2963,7 +3021,7 @@
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D9" s="25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E9" s="36">
         <v>0.49000709999999997</v>
@@ -2971,7 +3029,7 @@
     </row>
     <row r="10" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="41" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E10" s="36">
         <v>-0.440552</v>
@@ -2979,7 +3037,7 @@
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D11" s="25" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E11" s="36">
         <v>0.57040000000000002</v>
@@ -2990,7 +3048,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E12" s="36">
         <v>-1.9599999999999999E-2</v>
@@ -2998,7 +3056,7 @@
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D13" s="41" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E13" s="36">
         <v>0.29692429999999997</v>
@@ -3006,7 +3064,7 @@
     </row>
     <row r="14" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="41" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E14" s="36">
         <v>-0.3664499</v>
@@ -3014,7 +3072,7 @@
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D15" s="25" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E15" s="36">
         <v>0.47920000000000001</v>
@@ -3043,49 +3101,49 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="82" t="s">
-        <v>253</v>
-      </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
+      <c r="G3" s="90" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="82" t="s">
-        <v>258</v>
-      </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="82"/>
-      <c r="W3" s="82"/>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="82"/>
-      <c r="Z3" s="82"/>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="82"/>
+      <c r="S3" s="90" t="s">
+        <v>256</v>
+      </c>
+      <c r="T3" s="90"/>
+      <c r="U3" s="90"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="90"/>
+      <c r="Y3" s="90"/>
+      <c r="Z3" s="90"/>
+      <c r="AA3" s="90"/>
+      <c r="AB3" s="90"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
       <c r="G4" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I4" s="24">
         <v>3918</v>
       </c>
       <c r="L4" s="24"/>
       <c r="M4" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O4" s="24">
         <v>611</v>
@@ -3093,10 +3151,10 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="13"/>
       <c r="S4" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="T4" s="41" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="U4" s="24">
         <v>23047018</v>
@@ -3105,10 +3163,10 @@
       <c r="W4" s="41"/>
       <c r="X4" s="24"/>
       <c r="Y4" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA4" s="24">
         <v>2359143</v>
@@ -3121,50 +3179,50 @@
     <row r="5" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F5" s="24"/>
       <c r="G5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I5" s="31"/>
       <c r="K5" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L5" s="24"/>
       <c r="M5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O5" s="31"/>
       <c r="R5" s="24"/>
       <c r="S5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="U5" s="40"/>
       <c r="V5" s="41"/>
       <c r="W5" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Z5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AA5" s="40"/>
       <c r="AB5" s="41"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="85" t="s">
-        <v>257</v>
-      </c>
-      <c r="E6" s="85"/>
+      <c r="D6" s="92" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6" s="92"/>
       <c r="S6" s="41"/>
       <c r="T6" s="41"/>
       <c r="U6" s="41"/>
@@ -3177,10 +3235,10 @@
       <c r="AB6" s="41"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="87" t="s">
-        <v>319</v>
-      </c>
-      <c r="E7" s="87"/>
+      <c r="D7" s="94" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" s="94"/>
       <c r="G7">
         <v>127.98</v>
       </c>
@@ -3248,10 +3306,10 @@
       <c r="AB8" s="41"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="87"/>
+      <c r="E9" s="94"/>
       <c r="G9">
         <v>40.1</v>
       </c>
@@ -3297,7 +3355,7 @@
     </row>
     <row r="11" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D11" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S11" s="41"/>
       <c r="T11" s="36"/>
@@ -3388,48 +3446,48 @@
       <c r="AB15" s="41"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="85" t="s">
-        <v>315</v>
-      </c>
-      <c r="E16" s="85"/>
+      <c r="D16" s="92" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" s="92"/>
       <c r="G16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O16" s="38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="S16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="T16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U16" s="40" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="V16" s="41"/>
       <c r="W16" s="41"/>
       <c r="X16" s="41"/>
       <c r="Y16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Z16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AA16" s="38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AB16" s="41"/>
     </row>
@@ -3438,7 +3496,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G17">
         <f>H17*I4</f>
@@ -3448,7 +3506,7 @@
         <v>0.40300000000000002</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M17" s="39">
         <f>N17*O4</f>
@@ -3465,7 +3523,7 @@
         <v>0.43153160000000002</v>
       </c>
       <c r="U17" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V17" s="41"/>
       <c r="W17" s="41"/>
@@ -3482,10 +3540,10 @@
     </row>
     <row r="18" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D18" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G18">
         <v>3246</v>
@@ -3495,7 +3553,7 @@
         <v>0.82848392036753449</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M18">
         <v>187</v>
@@ -3512,7 +3570,7 @@
         <v>0.90943813208285773</v>
       </c>
       <c r="U18" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V18" s="41"/>
       <c r="W18" s="41"/>
@@ -3530,7 +3588,7 @@
     <row r="19" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D19" s="27"/>
       <c r="E19" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G19">
         <v>445</v>
@@ -3540,7 +3598,7 @@
         <v>0.11357835630423685</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M19">
         <v>323</v>
@@ -3557,7 +3615,7 @@
         <v>4.9359661193478482E-2</v>
       </c>
       <c r="U19" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V19" s="41"/>
       <c r="W19" s="41"/>
@@ -3575,7 +3633,7 @@
     <row r="20" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D20" s="27"/>
       <c r="E20" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G20">
         <v>227</v>
@@ -3585,7 +3643,7 @@
         <v>5.7937723328228691E-2</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M20">
         <v>101</v>
@@ -3602,7 +3660,7 @@
         <v>4.1202206723663773E-2</v>
       </c>
       <c r="U20" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V20" s="41"/>
       <c r="W20" s="41"/>
@@ -3619,7 +3677,7 @@
     </row>
     <row r="21" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -4197,49 +4255,49 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="82" t="s">
-        <v>253</v>
-      </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
+      <c r="G3" s="90" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="82" t="s">
-        <v>258</v>
-      </c>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="82"/>
-      <c r="W3" s="82"/>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="82"/>
-      <c r="Z3" s="82"/>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="82"/>
+      <c r="S3" s="90" t="s">
+        <v>256</v>
+      </c>
+      <c r="T3" s="90"/>
+      <c r="U3" s="90"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
+      <c r="X3" s="90"/>
+      <c r="Y3" s="90"/>
+      <c r="Z3" s="90"/>
+      <c r="AA3" s="90"/>
+      <c r="AB3" s="90"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
       <c r="G4" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I4" s="11">
         <v>3521</v>
       </c>
       <c r="L4" s="24"/>
       <c r="M4" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O4" s="11">
         <v>536</v>
@@ -4247,20 +4305,20 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="13"/>
       <c r="S4" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="T4" s="52" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="U4" s="11">
         <v>20856866</v>
       </c>
       <c r="X4" s="24"/>
       <c r="Y4" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AA4" s="11">
         <v>2088210</v>
@@ -4273,54 +4331,54 @@
     <row r="5" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F5" s="24"/>
       <c r="G5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I5" s="50"/>
       <c r="K5" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L5" s="24"/>
       <c r="M5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O5" s="50"/>
       <c r="R5" s="24"/>
       <c r="S5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="U5" s="50"/>
       <c r="W5" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Z5" s="33" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AA5" s="50"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="85" t="s">
-        <v>346</v>
-      </c>
-      <c r="E6" s="85"/>
+      <c r="D6" s="92" t="s">
+        <v>344</v>
+      </c>
+      <c r="E6" s="92"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="87" t="s">
-        <v>319</v>
-      </c>
-      <c r="E7" s="87"/>
+      <c r="D7" s="94" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" s="94"/>
       <c r="G7" s="70">
         <v>-0.13370000000000001</v>
       </c>
@@ -4404,10 +4462,10 @@
       <c r="AB8" s="58"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="87"/>
+      <c r="E9" s="94"/>
       <c r="G9" s="70">
         <v>0.46750000000000003</v>
       </c>
@@ -4473,7 +4531,7 @@
     </row>
     <row r="11" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D11" s="51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -4560,45 +4618,45 @@
       <c r="U15" s="30"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="85" t="s">
-        <v>315</v>
-      </c>
-      <c r="E16" s="85"/>
+      <c r="D16" s="92" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" s="92"/>
       <c r="G16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I16" s="50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O16" s="38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="S16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="T16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U16" s="50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Y16" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="Z16" s="33" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AA16" s="38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="4:27" x14ac:dyDescent="0.25">
@@ -4606,7 +4664,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G17" s="64">
         <f>H17*I4</f>
@@ -4616,7 +4674,7 @@
         <v>0.4078</v>
       </c>
       <c r="I17" s="62" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J17" s="58"/>
       <c r="K17" s="58"/>
@@ -4640,7 +4698,7 @@
         <v>0.43648000599999998</v>
       </c>
       <c r="U17" s="62" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V17" s="58"/>
       <c r="W17" s="58"/>
@@ -4653,15 +4711,15 @@
         <v>0.48712987400000002</v>
       </c>
       <c r="AA17" s="62" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G18" s="11">
         <v>2939</v>
@@ -4671,7 +4729,7 @@
         <v>0.83470604941777904</v>
       </c>
       <c r="I18" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J18" s="58"/>
       <c r="K18" s="58"/>
@@ -4695,7 +4753,7 @@
         <v>0.91431531467862914</v>
       </c>
       <c r="U18" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V18" s="58"/>
       <c r="W18" s="58"/>
@@ -4708,13 +4766,13 @@
         <v>0.46681751356424883</v>
       </c>
       <c r="AA18" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="51"/>
       <c r="E19" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G19" s="11">
         <v>387</v>
@@ -4724,7 +4782,7 @@
         <v>0.1099119568304459</v>
       </c>
       <c r="I19" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J19" s="58"/>
       <c r="K19" s="58"/>
@@ -4748,7 +4806,7 @@
         <v>4.5933027521968067E-2</v>
       </c>
       <c r="U19" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V19" s="58"/>
       <c r="W19" s="58"/>
@@ -4761,13 +4819,13 @@
         <v>0.35627547037893698</v>
       </c>
       <c r="AA19" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D20" s="51"/>
       <c r="E20" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G20" s="11">
         <v>195</v>
@@ -4777,7 +4835,7 @@
         <v>5.5381993751775063E-2</v>
       </c>
       <c r="I20" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J20" s="58"/>
       <c r="K20" s="58"/>
@@ -4801,7 +4859,7 @@
         <v>3.9751657799402845E-2</v>
       </c>
       <c r="U20" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V20" s="58"/>
       <c r="W20" s="58"/>
@@ -4814,12 +4872,12 @@
         <v>0.1770363133975989</v>
       </c>
       <c r="AA20" s="63" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E21" s="52">
         <v>1</v>
@@ -5431,8 +5489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
   <dimension ref="C2:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5554,7 +5612,7 @@
         <v>0.21015069024303129</v>
       </c>
       <c r="F7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -5569,7 +5627,7 @@
         <v>0.21015069024303129</v>
       </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -5584,22 +5642,22 @@
         <v>0.20861381226499479</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>4073</v>
       </c>
-      <c r="D10">
-        <v>22945346</v>
+      <c r="D10" s="82">
+        <v>23012867</v>
       </c>
       <c r="E10" s="23">
         <f t="shared" si="0"/>
-        <v>0.20800172802455902</v>
+        <v>0.20861381226499479</v>
       </c>
       <c r="F10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -5614,7 +5672,7 @@
         <v>0.20800172802455902</v>
       </c>
       <c r="F11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
@@ -5629,7 +5687,7 @@
         <v>0.20800172802455902</v>
       </c>
       <c r="F12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
@@ -5644,7 +5702,7 @@
         <v>0.20800172802455902</v>
       </c>
       <c r="F13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -6108,18 +6166,18 @@
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D6" t="s">
+        <v>356</v>
+      </c>
+      <c r="E6" t="s">
         <v>358</v>
-      </c>
-      <c r="E6" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -6130,7 +6188,7 @@
         <v>30121997</v>
       </c>
       <c r="E8" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
@@ -6141,7 +6199,7 @@
         <v>13022021</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -6152,7 +6210,7 @@
         <v>14022021</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
@@ -6163,7 +6221,7 @@
         <v>15022021</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
@@ -6174,7 +6232,7 @@
         <v>16022021</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
@@ -6185,7 +6243,7 @@
         <v>17022021</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
@@ -6196,7 +6254,7 @@
         <v>18022021</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
@@ -6207,7 +6265,7 @@
         <v>19022021</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
@@ -6218,7 +6276,7 @@
         <v>20022021</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
@@ -6229,7 +6287,7 @@
         <v>21022021</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
@@ -6240,7 +6298,7 @@
         <v>22022021</v>
       </c>
       <c r="E18" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
@@ -6251,7 +6309,7 @@
         <v>23022021</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
@@ -6262,7 +6320,7 @@
         <v>24022021</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
@@ -6273,7 +6331,7 @@
         <v>25022021</v>
       </c>
       <c r="E21" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -6284,7 +6342,7 @@
         <v>26022021</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
@@ -6295,7 +6353,7 @@
         <v>27022021</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -6306,7 +6364,7 @@
         <v>28022021</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
@@ -6317,7 +6375,7 @@
         <v>29022021</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
@@ -6328,7 +6386,7 @@
         <v>30022021</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
@@ -6339,7 +6397,7 @@
         <v>31022021</v>
       </c>
       <c r="E27" s="72" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -6351,7 +6409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D37E278C-1DAC-4F67-8E1E-CC1E987D4B76}">
   <dimension ref="C2:I49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -6791,8 +6849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE37440-C046-4752-9983-B7C8940AC835}">
   <dimension ref="C2:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6826,7 +6884,7 @@
         <v>203</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
@@ -6863,7 +6921,7 @@
         <v>-15361</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -6888,7 +6946,7 @@
         <v>205</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
@@ -6913,7 +6971,7 @@
         <v>207</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
@@ -6928,7 +6986,7 @@
         <v>0.23268087648621202</v>
       </c>
       <c r="F7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G7">
         <f>C7-C6</f>
@@ -6938,7 +6996,7 @@
         <v>212</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
@@ -6953,17 +7011,17 @@
         <v>0.23268087648621202</v>
       </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G8">
         <f t="shared" ref="G8:G13" si="1">C8-C7</f>
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -6978,14 +7036,14 @@
         <v>0.23106275713196983</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
         <v>-33</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
@@ -7000,17 +7058,17 @@
         <v>0.23106275713196983</v>
       </c>
       <c r="F10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
@@ -7025,17 +7083,17 @@
         <v>0.23020732043178821</v>
       </c>
       <c r="F11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
         <v>-19</v>
       </c>
       <c r="H11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
@@ -7050,17 +7108,17 @@
         <v>0.23020732043178821</v>
       </c>
       <c r="F12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
@@ -7075,17 +7133,17 @@
         <v>0.23020732043178821</v>
       </c>
       <c r="F13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
@@ -7125,10 +7183,10 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -7136,22 +7194,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I4" s="79" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J4" s="79" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K4" s="79" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -7159,7 +7217,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C5">
         <v>9.61</v>
@@ -7174,7 +7232,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I5">
         <v>29.95</v>
@@ -7188,7 +7246,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C6">
         <v>8.7469999999999999</v>
@@ -7201,7 +7259,7 @@
       </c>
       <c r="G6" s="79"/>
       <c r="H6" s="79" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I6">
         <v>29.58</v>
@@ -7222,7 +7280,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C8">
         <v>9.6</v>
@@ -7237,7 +7295,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I8">
         <v>29.76</v>
@@ -7251,7 +7309,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C9">
         <v>9.6</v>
@@ -7264,7 +7322,7 @@
       </c>
       <c r="G9" s="79"/>
       <c r="H9" s="79" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I9">
         <v>29.12</v>
@@ -7278,7 +7336,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C10">
         <v>8.4</v>
@@ -7291,7 +7349,7 @@
       </c>
       <c r="G10" s="79"/>
       <c r="H10" s="79" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I10">
         <v>27.84</v>
@@ -7312,7 +7370,7 @@
         <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C12">
         <v>8.83</v>
@@ -7327,7 +7385,7 @@
         <v>55</v>
       </c>
       <c r="H12" s="79" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I12">
         <v>37.93</v>
@@ -7341,7 +7399,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C13">
         <v>10.1</v>
@@ -7354,7 +7412,7 @@
       </c>
       <c r="G13" s="79"/>
       <c r="H13" s="79" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I13">
         <v>23.05</v>
@@ -7374,65 +7432,69 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60364F5B-DCE9-46C6-A586-3092036B5563}">
-  <dimension ref="D4:O12"/>
+  <dimension ref="D4:P43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView showGridLines="0" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="80" t="s">
+    <row r="4" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="89" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="89" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+    </row>
+    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F5" s="88" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="88"/>
+      <c r="H5" s="30"/>
+      <c r="J5" s="88" t="s">
+        <v>243</v>
+      </c>
+      <c r="K5" s="88"/>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" t="s">
         <v>244</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80" t="s">
-        <v>243</v>
-      </c>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-    </row>
-    <row r="5" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="81" t="s">
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" t="s">
+        <v>240</v>
+      </c>
+      <c r="K6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
         <v>245</v>
-      </c>
-      <c r="G5" s="81"/>
-      <c r="I5" s="81" t="s">
-        <v>245</v>
-      </c>
-      <c r="J5" s="81"/>
-    </row>
-    <row r="6" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F6" t="s">
-        <v>242</v>
-      </c>
-      <c r="G6" t="s">
-        <v>246</v>
-      </c>
-      <c r="H6" t="s">
-        <v>241</v>
-      </c>
-      <c r="I6" t="s">
-        <v>242</v>
-      </c>
-      <c r="J6" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>247</v>
       </c>
       <c r="E7">
         <f>Dataset_1!C3</f>
@@ -7446,24 +7508,25 @@
         <f>F7/$F$7</f>
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="23"/>
+      <c r="I7">
         <f>Dataset_2!C3</f>
         <v>20912</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f>Dataset_2!D3</f>
         <v>110313247</v>
       </c>
-      <c r="J7" s="23">
-        <f>I7/$I$7</f>
+      <c r="K7" s="23">
+        <f>J7/$J$7</f>
         <v>1</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="O7" s="11"/>
-    </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L7" s="23"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E8">
         <f>Dataset_1!C5-Dataset_1!C3</f>
@@ -7477,23 +7540,24 @@
         <f t="shared" ref="G8:G12" si="0">F8/$F$7</f>
         <v>-0.72796028748931663</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="23"/>
+      <c r="I8">
         <f>Dataset_2!C5-Dataset_2!C3</f>
         <v>-16715</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>Dataset_2!D5-Dataset_2!D3</f>
         <v>-86931543</v>
       </c>
-      <c r="J8" s="23">
-        <f t="shared" ref="J8:J12" si="1">I8/$I$7</f>
+      <c r="K8" s="23">
+        <f t="shared" ref="K8:K12" si="1">J8/$J$7</f>
         <v>-0.78804264550385317</v>
       </c>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L8" s="23"/>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E9">
         <f>Dataset_1!C6-Dataset_1!C5</f>
@@ -7507,23 +7571,24 @@
         <f t="shared" si="0"/>
         <v>-3.9358836024471294E-2</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="23"/>
+      <c r="I9">
         <f>Dataset_2!C6-Dataset_2!C5</f>
         <v>-94</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f>Dataset_2!D6-Dataset_2!D5</f>
         <v>-199299</v>
       </c>
-      <c r="J9" s="23">
+      <c r="K9" s="23">
         <f t="shared" si="1"/>
         <v>-1.806664253115494E-3</v>
       </c>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L9" s="23"/>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E10">
         <f>Dataset_1!C9-Dataset_1!C6</f>
@@ -7537,23 +7602,24 @@
         <f t="shared" si="0"/>
         <v>-1.6181193542421973E-3</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="23"/>
+      <c r="I10">
         <f>Dataset_2!C9-Dataset_2!C6</f>
         <v>-30</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f>Dataset_2!D9-Dataset_2!D6</f>
         <v>-169538</v>
       </c>
-      <c r="J10" s="23">
+      <c r="K10" s="23">
         <f t="shared" si="1"/>
         <v>-1.5368779780364908E-3</v>
       </c>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L10" s="23"/>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E11">
         <f>Dataset_1!C11-Dataset_1!C9</f>
@@ -7567,23 +7633,24 @@
         <f t="shared" si="0"/>
         <v>-8.5543670018162004E-4</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="23"/>
+      <c r="I11">
         <f>Dataset_2!C11-Dataset_2!C9</f>
         <v>-14</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f>Dataset_2!D11-Dataset_2!D9</f>
         <v>-67521</v>
       </c>
-      <c r="J11" s="23">
+      <c r="K11" s="23">
         <f t="shared" si="1"/>
         <v>-6.1208424043578374E-4</v>
       </c>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L11" s="23"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E12">
         <f>SUM(E7:E11)</f>
@@ -7597,26 +7664,548 @@
         <f t="shared" si="0"/>
         <v>0.23020732043178821</v>
       </c>
-      <c r="H12">
-        <f>SUM(H7:H11)</f>
-        <v>4059</v>
-      </c>
+      <c r="H12" s="23"/>
       <c r="I12">
         <f>SUM(I7:I11)</f>
+        <v>4059</v>
+      </c>
+      <c r="J12">
+        <f>SUM(J7:J11)</f>
         <v>22945346</v>
       </c>
-      <c r="J12" s="23">
+      <c r="K12" s="23">
         <f t="shared" si="1"/>
         <v>0.20800172802455902</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M14" s="83"/>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M15" s="83"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>368</v>
+      </c>
+      <c r="M16" s="83"/>
+    </row>
+    <row r="17" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="89" t="s">
+        <v>242</v>
+      </c>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="M17" s="83"/>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="88" t="s">
+        <v>243</v>
+      </c>
+      <c r="G18" s="88"/>
+      <c r="H18" s="87" t="s">
+        <v>374</v>
+      </c>
+      <c r="I18" s="87" t="s">
+        <v>371</v>
+      </c>
+      <c r="J18" s="88" t="s">
+        <v>370</v>
+      </c>
+      <c r="K18" s="88"/>
+      <c r="M18" s="83"/>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D19" s="81"/>
+      <c r="E19" s="81" t="s">
+        <v>239</v>
+      </c>
+      <c r="F19" s="81" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19" s="81" t="s">
+        <v>244</v>
+      </c>
+      <c r="I19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="83"/>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D20" s="81" t="s">
+        <v>369</v>
+      </c>
+      <c r="E20" s="81">
+        <v>20912</v>
+      </c>
+      <c r="F20" s="81">
+        <v>110313247</v>
+      </c>
+      <c r="G20" s="23">
+        <f>F20/$F$7</f>
+        <v>1</v>
+      </c>
+      <c r="H20" s="23"/>
+      <c r="I20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="84"/>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D21" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" s="81">
+        <v>5551</v>
+      </c>
+      <c r="F21" s="81">
+        <v>30222610</v>
+      </c>
+      <c r="G21" s="23">
+        <f t="shared" ref="G21:G30" si="2">F21/$F$7</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81" t="s">
+        <v>380</v>
+      </c>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="85"/>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D22" s="81" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="81">
+        <v>5512</v>
+      </c>
+      <c r="F22" s="81">
+        <v>30009584</v>
+      </c>
+      <c r="G22" s="23">
+        <f t="shared" si="2"/>
+        <v>0.27203971251068332</v>
+      </c>
+      <c r="H22" s="23"/>
+      <c r="I22" s="81"/>
+      <c r="J22" s="81" t="s">
+        <v>379</v>
+      </c>
+      <c r="K22" s="81"/>
+      <c r="L22" s="81"/>
+      <c r="M22" s="86"/>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D23" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" s="81">
+        <v>4581</v>
+      </c>
+      <c r="F23" s="81">
+        <v>25667783</v>
+      </c>
+      <c r="G23" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="81" t="s">
+        <v>372</v>
+      </c>
+      <c r="J23" s="81" t="s">
+        <v>381</v>
+      </c>
+      <c r="K23" s="81"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="86"/>
+    </row>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D24" s="81" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="81">
+        <v>4581</v>
+      </c>
+      <c r="F24" s="81">
+        <v>25667783</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="81" t="s">
+        <v>373</v>
+      </c>
+      <c r="J24" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="85"/>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="81" t="s">
+        <v>218</v>
+      </c>
+      <c r="E25" s="81">
+        <v>4581</v>
+      </c>
+      <c r="F25" s="81">
+        <v>25667783</v>
+      </c>
+      <c r="G25" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="H25" s="23"/>
+      <c r="I25" s="81"/>
+      <c r="K25" s="81"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="85"/>
+    </row>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D26" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E26" s="81">
+        <v>4548</v>
+      </c>
+      <c r="F26" s="81">
+        <v>25489283</v>
+      </c>
+      <c r="G26" s="23">
+        <f>F26/$F$7</f>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="H26" s="23"/>
+      <c r="J26" t="s">
+        <v>377</v>
+      </c>
+      <c r="K26" s="81"/>
+      <c r="L26" s="81"/>
+      <c r="M26" s="85"/>
+    </row>
+    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="81" t="s">
+        <v>223</v>
+      </c>
+      <c r="E27" s="81">
+        <v>4548</v>
+      </c>
+      <c r="F27" s="81">
+        <v>25489283</v>
+      </c>
+      <c r="G27" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="J27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="85"/>
+    </row>
+    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="81" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="81">
+        <v>4529</v>
+      </c>
+      <c r="F28" s="81">
+        <v>25394917</v>
+      </c>
+      <c r="G28" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="J28" s="81" t="s">
+        <v>378</v>
+      </c>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="85"/>
+    </row>
+    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D29" s="81" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="81">
+        <v>4529</v>
+      </c>
+      <c r="F29" s="81">
+        <v>25394917</v>
+      </c>
+      <c r="G29" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="J29" s="81" t="s">
+        <v>236</v>
+      </c>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="85"/>
+    </row>
+    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D30" s="81" t="s">
+        <v>234</v>
+      </c>
+      <c r="E30" s="81">
+        <v>4529</v>
+      </c>
+      <c r="F30" s="81">
+        <v>25394917</v>
+      </c>
+      <c r="G30" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="J30" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="M30" s="83"/>
+    </row>
+    <row r="31" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="81"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="M31" s="83"/>
+    </row>
+    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E32" s="82"/>
+      <c r="F32" s="88" t="s">
+        <v>243</v>
+      </c>
+      <c r="G32" s="88"/>
+      <c r="H32" s="87" t="s">
+        <v>374</v>
+      </c>
+      <c r="I32" s="87" t="s">
+        <v>371</v>
+      </c>
+      <c r="J32" s="88" t="s">
+        <v>370</v>
+      </c>
+      <c r="K32" s="88"/>
+      <c r="M32" s="83"/>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="82" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33" s="82">
+        <v>20912</v>
+      </c>
+      <c r="F33" s="82">
+        <v>110313247</v>
+      </c>
+      <c r="G33" s="23">
+        <f>F33/$F$33</f>
+        <v>1</v>
+      </c>
+      <c r="I33" s="82"/>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="82" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" s="82">
+        <v>5551</v>
+      </c>
+      <c r="F34" s="82">
+        <v>30222610</v>
+      </c>
+      <c r="G34" s="23">
+        <f t="shared" ref="G34:G43" si="3">F34/$F$33</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="I34" s="82"/>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" s="82">
+        <f>E34+I35</f>
+        <v>5551</v>
+      </c>
+      <c r="F35" s="82">
+        <v>23381704</v>
+      </c>
+      <c r="G35" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21195735449614678</v>
+      </c>
+      <c r="I35" s="82"/>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="82" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" s="82">
+        <v>4103</v>
+      </c>
+      <c r="F36" s="82">
+        <v>23182405</v>
+      </c>
+      <c r="G36" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="I36" s="82"/>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="82" t="s">
+        <v>217</v>
+      </c>
+      <c r="E37" s="82">
+        <v>4103</v>
+      </c>
+      <c r="F37" s="82">
+        <v>23182405</v>
+      </c>
+      <c r="G37" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="I37" s="82"/>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="E38" s="82">
+        <v>4103</v>
+      </c>
+      <c r="F38" s="82">
+        <v>23182405</v>
+      </c>
+      <c r="G38" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="I38" s="82"/>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E39" s="82">
+        <v>4073</v>
+      </c>
+      <c r="F39" s="82">
+        <v>23012867</v>
+      </c>
+      <c r="G39" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20861381226499479</v>
+      </c>
+      <c r="I39" s="82"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" s="82">
+        <v>4073</v>
+      </c>
+      <c r="F40" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G40" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="I40" s="82"/>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="E41" s="82">
+        <v>4059</v>
+      </c>
+      <c r="F41" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G41" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="I41" s="82"/>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="82" t="s">
+        <v>233</v>
+      </c>
+      <c r="E42" s="82">
+        <v>4059</v>
+      </c>
+      <c r="F42" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G42" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="H42" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="I42" s="82"/>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="E43" s="82">
+        <v>4059</v>
+      </c>
+      <c r="F43" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G43" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="I43" s="82"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="10">
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="J18:K18"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="I4:K4"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="I31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -7663,38 +8252,38 @@
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
       <c r="K1" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
       <c r="N1" s="24"/>
       <c r="O1" s="24"/>
       <c r="P1" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
       <c r="V1" s="24"/>
       <c r="W1" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="X1" s="24"/>
       <c r="Y1" s="24"/>
@@ -7702,74 +8291,74 @@
     </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>256</v>
-      </c>
       <c r="G2" s="32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H2" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="J2" s="33" t="s">
         <v>254</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>256</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="M2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="N2" s="33" t="s">
         <v>254</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>256</v>
       </c>
       <c r="O2" s="24"/>
       <c r="P2" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="R2" s="33" t="s">
         <v>254</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>256</v>
       </c>
       <c r="S2" s="24"/>
       <c r="T2" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="U2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="V2" s="33" t="s">
         <v>254</v>
-      </c>
-      <c r="U2" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="V2" s="33" t="s">
-        <v>256</v>
       </c>
       <c r="W2" s="24"/>
       <c r="X2" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z2" s="33" t="s">
         <v>254</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="Z2" s="33" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28"/>
@@ -7782,7 +8371,7 @@
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -7798,19 +8387,19 @@
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C8" s="27"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C10" s="27"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" s="27"/>
     </row>
@@ -7819,32 +8408,32 @@
         <v>55</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -7854,60 +8443,60 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C21" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="24" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -7917,130 +8506,130 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="24" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="24" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C40" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="24"/>
       <c r="C41" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="24"/>
       <c r="C42" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="24"/>
       <c r="C43" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="24" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C44" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="24"/>
       <c r="C45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
       <c r="C46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
       <c r="C47" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C48" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="24"/>
       <c r="C49" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="24"/>
       <c r="C50" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="24"/>
       <c r="C51" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -8050,42 +8639,42 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -8105,94 +8694,94 @@
   <sheetData>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C2" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="E2" s="83" t="s">
-        <v>244</v>
-      </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="M2" s="83" t="s">
-        <v>243</v>
-      </c>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
+        <v>342</v>
+      </c>
+      <c r="E2" s="91" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="M2" s="91" t="s">
+        <v>241</v>
+      </c>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="E3" s="82" t="s">
-        <v>327</v>
-      </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="I3" s="82" t="s">
-        <v>328</v>
-      </c>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="M3" s="82" t="s">
-        <v>327</v>
-      </c>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
+      <c r="E3" s="90" t="s">
+        <v>325</v>
+      </c>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="I3" s="90" t="s">
+        <v>326</v>
+      </c>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="M3" s="90" t="s">
+        <v>325</v>
+      </c>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
       <c r="P3" s="45"/>
-      <c r="Q3" s="82" t="s">
-        <v>328</v>
-      </c>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82"/>
+      <c r="Q3" s="90" t="s">
+        <v>326</v>
+      </c>
+      <c r="R3" s="90"/>
+      <c r="S3" s="90"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E4" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>323</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>325</v>
       </c>
       <c r="H4" s="31"/>
       <c r="I4" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>324</v>
+      </c>
+      <c r="M4" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="O4" s="44" t="s">
         <v>323</v>
-      </c>
-      <c r="J4" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="K4" s="42" t="s">
-        <v>326</v>
-      </c>
-      <c r="M4" s="44" t="s">
-        <v>323</v>
-      </c>
-      <c r="N4" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="O4" s="44" t="s">
-        <v>325</v>
       </c>
       <c r="P4" s="44"/>
       <c r="Q4" s="44" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="R4" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="S4" s="42" t="s">
         <v>324</v>
-      </c>
-      <c r="S4" s="42" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E5" s="43">
         <v>0.82180149999999996</v>
@@ -8235,7 +8824,7 @@
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E6" s="43">
         <v>0.8236696</v>
@@ -8278,7 +8867,7 @@
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E7" s="43">
         <v>0.82320090000000001</v>
@@ -8325,104 +8914,104 @@
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E10" s="43"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E11" s="83" t="s">
-        <v>244</v>
-      </c>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
+      <c r="E11" s="91" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
       <c r="L11" s="49"/>
-      <c r="M11" s="83" t="s">
-        <v>243</v>
-      </c>
-      <c r="N11" s="83"/>
-      <c r="O11" s="83"/>
-      <c r="P11" s="83"/>
-      <c r="Q11" s="83"/>
-      <c r="R11" s="83"/>
-      <c r="S11" s="83"/>
+      <c r="M11" s="91" t="s">
+        <v>241</v>
+      </c>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="91"/>
+      <c r="Q11" s="91"/>
+      <c r="R11" s="91"/>
+      <c r="S11" s="91"/>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D12" s="49"/>
-      <c r="E12" s="82" t="s">
-        <v>327</v>
-      </c>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
+      <c r="E12" s="90" t="s">
+        <v>325</v>
+      </c>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
       <c r="H12" s="49"/>
-      <c r="I12" s="82" t="s">
-        <v>328</v>
-      </c>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
+      <c r="I12" s="90" t="s">
+        <v>326</v>
+      </c>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="82" t="s">
-        <v>327</v>
-      </c>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
+      <c r="M12" s="90" t="s">
+        <v>325</v>
+      </c>
+      <c r="N12" s="90"/>
+      <c r="O12" s="90"/>
       <c r="P12" s="49"/>
-      <c r="Q12" s="82" t="s">
-        <v>328</v>
-      </c>
-      <c r="R12" s="82"/>
-      <c r="S12" s="82"/>
+      <c r="Q12" s="90" t="s">
+        <v>326</v>
+      </c>
+      <c r="R12" s="90"/>
+      <c r="S12" s="90"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D13" s="49"/>
       <c r="E13" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="G13" s="48" t="s">
         <v>323</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>324</v>
-      </c>
-      <c r="G13" s="48" t="s">
-        <v>325</v>
       </c>
       <c r="H13" s="48"/>
       <c r="I13" s="48" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J13" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="K13" s="42" t="s">
         <v>324</v>
-      </c>
-      <c r="K13" s="42" t="s">
-        <v>326</v>
       </c>
       <c r="L13" s="49"/>
       <c r="M13" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="N13" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="O13" s="48" t="s">
         <v>323</v>
-      </c>
-      <c r="N13" s="48" t="s">
-        <v>324</v>
-      </c>
-      <c r="O13" s="48" t="s">
-        <v>325</v>
       </c>
       <c r="P13" s="48"/>
       <c r="Q13" s="48" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="R13" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="S13" s="42" t="s">
         <v>324</v>
-      </c>
-      <c r="S13" s="42" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D14" s="49" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E14" s="43">
         <v>0.84530419999999995</v>
@@ -8466,7 +9055,7 @@
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D15" s="49" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E15" s="53">
         <v>0.84761169999999997</v>
@@ -8510,7 +9099,7 @@
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D16" s="49" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E16" s="43">
         <v>0.84655320000000001</v>
@@ -8608,109 +9197,109 @@
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
       <c r="F6" s="57"/>
-      <c r="G6" s="82" t="s">
-        <v>352</v>
-      </c>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
+      <c r="G6" s="90" t="s">
+        <v>350</v>
+      </c>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
       <c r="Y6" s="57"/>
       <c r="Z6" s="57"/>
       <c r="AA6" s="57"/>
-      <c r="AB6" s="82" t="s">
-        <v>355</v>
-      </c>
-      <c r="AC6" s="82"/>
-      <c r="AD6" s="82"/>
-      <c r="AE6" s="82"/>
-      <c r="AF6" s="82"/>
-      <c r="AG6" s="82"/>
-      <c r="AH6" s="82"/>
-      <c r="AI6" s="82"/>
-      <c r="AJ6" s="82"/>
-      <c r="AK6" s="82"/>
-      <c r="AL6" s="82"/>
-      <c r="AM6" s="82"/>
-      <c r="AN6" s="82"/>
-      <c r="AO6" s="82"/>
-      <c r="AP6" s="82"/>
-      <c r="AQ6" s="82"/>
-      <c r="AR6" s="82"/>
+      <c r="AB6" s="90" t="s">
+        <v>353</v>
+      </c>
+      <c r="AC6" s="90"/>
+      <c r="AD6" s="90"/>
+      <c r="AE6" s="90"/>
+      <c r="AF6" s="90"/>
+      <c r="AG6" s="90"/>
+      <c r="AH6" s="90"/>
+      <c r="AI6" s="90"/>
+      <c r="AJ6" s="90"/>
+      <c r="AK6" s="90"/>
+      <c r="AL6" s="90"/>
+      <c r="AM6" s="90"/>
+      <c r="AN6" s="90"/>
+      <c r="AO6" s="90"/>
+      <c r="AP6" s="90"/>
+      <c r="AQ6" s="90"/>
+      <c r="AR6" s="90"/>
       <c r="BA6" s="57"/>
       <c r="BB6" s="57"/>
       <c r="BC6" s="57"/>
-      <c r="BD6" s="82"/>
-      <c r="BE6" s="82"/>
-      <c r="BF6" s="82"/>
-      <c r="BG6" s="82"/>
-      <c r="BH6" s="82"/>
-      <c r="BI6" s="82"/>
-      <c r="BJ6" s="82"/>
-      <c r="BK6" s="82"/>
-      <c r="BL6" s="82"/>
-      <c r="BM6" s="82"/>
-      <c r="BN6" s="82"/>
+      <c r="BD6" s="90"/>
+      <c r="BE6" s="90"/>
+      <c r="BF6" s="90"/>
+      <c r="BG6" s="90"/>
+      <c r="BH6" s="90"/>
+      <c r="BI6" s="90"/>
+      <c r="BJ6" s="90"/>
+      <c r="BK6" s="90"/>
+      <c r="BL6" s="90"/>
+      <c r="BM6" s="90"/>
+      <c r="BN6" s="90"/>
     </row>
     <row r="7" spans="4:66" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="84" t="s">
-        <v>264</v>
-      </c>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
+      <c r="G7" s="95" t="s">
+        <v>262</v>
+      </c>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
       <c r="L7" s="35"/>
-      <c r="M7" s="84" t="s">
+      <c r="M7" s="95" t="s">
         <v>164</v>
       </c>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="84"/>
+      <c r="N7" s="95"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
       <c r="R7" s="35"/>
-      <c r="S7" s="84" t="s">
+      <c r="S7" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="84"/>
-      <c r="U7" s="84"/>
-      <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="AB7" s="84" t="s">
-        <v>264</v>
-      </c>
-      <c r="AC7" s="84"/>
-      <c r="AD7" s="84"/>
-      <c r="AE7" s="84"/>
-      <c r="AF7" s="84"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="95"/>
+      <c r="W7" s="95"/>
+      <c r="AB7" s="95" t="s">
+        <v>262</v>
+      </c>
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
       <c r="AG7" s="35"/>
-      <c r="AH7" s="84" t="s">
+      <c r="AH7" s="95" t="s">
         <v>164</v>
       </c>
-      <c r="AI7" s="84"/>
-      <c r="AJ7" s="84"/>
-      <c r="AK7" s="84"/>
-      <c r="AL7" s="84"/>
+      <c r="AI7" s="95"/>
+      <c r="AJ7" s="95"/>
+      <c r="AK7" s="95"/>
+      <c r="AL7" s="95"/>
       <c r="AM7" s="35"/>
-      <c r="AN7" s="84" t="s">
+      <c r="AN7" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="AO7" s="84"/>
-      <c r="AP7" s="84"/>
-      <c r="AQ7" s="84"/>
-      <c r="AR7" s="84"/>
+      <c r="AO7" s="95"/>
+      <c r="AP7" s="95"/>
+      <c r="AQ7" s="95"/>
+      <c r="AR7" s="95"/>
       <c r="BD7" s="35"/>
       <c r="BE7" s="35"/>
       <c r="BF7" s="35"/>
@@ -8728,77 +9317,77 @@
       <c r="E8" s="57"/>
       <c r="F8" s="13"/>
       <c r="G8" s="24" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H8" s="57"/>
       <c r="I8" s="24" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J8" s="57"/>
       <c r="K8" s="24" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="73" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="N8" s="73"/>
       <c r="O8" s="73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="P8" s="73"/>
       <c r="Q8" s="73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R8" s="24"/>
       <c r="S8" s="73" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="T8" s="28"/>
       <c r="U8" s="73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="V8" s="28"/>
       <c r="W8" s="73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Y8" s="57"/>
       <c r="Z8" s="57"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="24" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AC8" s="57"/>
       <c r="AD8" s="24" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AE8" s="57"/>
       <c r="AF8" s="24" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AG8" s="32"/>
       <c r="AH8" s="73" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AI8" s="73"/>
       <c r="AJ8" s="73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AK8" s="73"/>
       <c r="AL8" s="73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AM8" s="24"/>
       <c r="AN8" s="73" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AO8" s="28"/>
       <c r="AP8" s="73" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AQ8" s="28"/>
       <c r="AR8" s="73" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="BA8" s="57"/>
       <c r="BB8" s="57"/>
@@ -8820,77 +9409,77 @@
       <c r="E9" s="57"/>
       <c r="F9" s="24"/>
       <c r="G9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J9" s="55"/>
       <c r="K9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L9" s="55"/>
       <c r="M9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N9" s="33"/>
       <c r="O9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="P9" s="33"/>
       <c r="Q9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="R9" s="33"/>
       <c r="S9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T9" s="55"/>
       <c r="U9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="V9" s="55"/>
       <c r="W9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Y9" s="57"/>
       <c r="Z9" s="57"/>
       <c r="AA9" s="24"/>
       <c r="AB9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AC9" s="55"/>
       <c r="AD9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AE9" s="55"/>
       <c r="AF9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AG9" s="55"/>
       <c r="AH9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AI9" s="33"/>
       <c r="AJ9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AK9" s="33"/>
       <c r="AL9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AM9" s="33"/>
       <c r="AN9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AO9" s="55"/>
       <c r="AP9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AQ9" s="55"/>
       <c r="AR9" s="33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="BA9" s="57"/>
       <c r="BB9" s="57"/>
@@ -8908,10 +9497,10 @@
       <c r="BN9" s="55"/>
     </row>
     <row r="10" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D10" s="85" t="s">
-        <v>354</v>
-      </c>
-      <c r="E10" s="86"/>
+      <c r="D10" s="92" t="s">
+        <v>352</v>
+      </c>
+      <c r="E10" s="93"/>
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10" s="57"/>
@@ -8926,10 +9515,10 @@
       <c r="U10" s="57"/>
       <c r="V10" s="57"/>
       <c r="W10" s="57"/>
-      <c r="Y10" s="85" t="s">
-        <v>354</v>
-      </c>
-      <c r="Z10" s="86"/>
+      <c r="Y10" s="92" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z10" s="93"/>
       <c r="AA10" s="57"/>
       <c r="AB10" s="57"/>
       <c r="AC10" s="57"/>
@@ -8948,8 +9537,8 @@
       <c r="AP10" s="57"/>
       <c r="AQ10" s="57"/>
       <c r="AR10" s="57"/>
-      <c r="BA10" s="85"/>
-      <c r="BB10" s="85"/>
+      <c r="BA10" s="92"/>
+      <c r="BB10" s="92"/>
       <c r="BC10" s="57"/>
       <c r="BD10" s="57"/>
       <c r="BE10" s="57"/>
@@ -8964,10 +9553,10 @@
       <c r="BN10" s="57"/>
     </row>
     <row r="11" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D11" s="87" t="s">
-        <v>353</v>
-      </c>
-      <c r="E11" s="87"/>
+      <c r="D11" s="94" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" s="94"/>
       <c r="F11" s="57"/>
       <c r="G11" s="11">
         <v>0.27</v>
@@ -9003,10 +9592,10 @@
       <c r="W11" s="11">
         <v>-0.63</v>
       </c>
-      <c r="Y11" s="87" t="s">
-        <v>353</v>
-      </c>
-      <c r="Z11" s="87"/>
+      <c r="Y11" s="94" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z11" s="94"/>
       <c r="AA11" s="57"/>
       <c r="AB11" s="11">
         <v>1.51</v>
@@ -9043,8 +9632,8 @@
       <c r="AR11" s="11">
         <v>-0.5</v>
       </c>
-      <c r="BA11" s="87"/>
-      <c r="BB11" s="87"/>
+      <c r="BA11" s="94"/>
+      <c r="BB11" s="94"/>
       <c r="BC11" s="57"/>
       <c r="BD11" s="11"/>
       <c r="BE11" s="65"/>
@@ -9104,7 +9693,7 @@
     </row>
     <row r="13" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D13" s="56" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E13" s="57"/>
       <c r="F13" s="57"/>
@@ -9125,7 +9714,7 @@
       <c r="V13" s="58"/>
       <c r="W13" s="58"/>
       <c r="Y13" s="56" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="Z13" s="57"/>
       <c r="AA13" s="57"/>
@@ -9313,88 +9902,88 @@
       <c r="BN15" s="57"/>
     </row>
     <row r="16" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D16" s="85" t="s">
-        <v>348</v>
-      </c>
-      <c r="E16" s="85"/>
+      <c r="D16" s="92" t="s">
+        <v>346</v>
+      </c>
+      <c r="E16" s="92"/>
       <c r="F16" s="57"/>
       <c r="G16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="H16" s="55"/>
       <c r="I16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J16" s="55"/>
       <c r="K16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L16" s="33"/>
       <c r="M16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N16" s="77"/>
       <c r="O16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="P16" s="77"/>
       <c r="Q16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="R16" s="33"/>
       <c r="S16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="T16" s="55"/>
       <c r="U16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="V16" s="55"/>
       <c r="W16" s="33" t="s">
-        <v>356</v>
-      </c>
-      <c r="Y16" s="85" t="s">
-        <v>348</v>
-      </c>
-      <c r="Z16" s="85"/>
+        <v>354</v>
+      </c>
+      <c r="Y16" s="92" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z16" s="92"/>
       <c r="AA16" s="57"/>
       <c r="AB16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AC16" s="55"/>
       <c r="AD16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AE16" s="55"/>
       <c r="AF16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AG16" s="33"/>
       <c r="AH16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AI16" s="33"/>
       <c r="AJ16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AK16" s="33"/>
       <c r="AL16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AM16" s="33"/>
       <c r="AN16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AO16" s="55"/>
       <c r="AP16" s="33" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AQ16" s="55"/>
       <c r="AR16" s="33" t="s">
-        <v>356</v>
-      </c>
-      <c r="BA16" s="85"/>
-      <c r="BB16" s="85"/>
+        <v>354</v>
+      </c>
+      <c r="BA16" s="92"/>
+      <c r="BB16" s="92"/>
       <c r="BC16" s="57"/>
       <c r="BD16" s="33"/>
       <c r="BE16" s="33"/>
@@ -9413,7 +10002,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F17" s="57"/>
       <c r="G17" s="78">
@@ -9455,7 +10044,7 @@
         <v>55</v>
       </c>
       <c r="Z17" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AA17" s="57"/>
       <c r="AB17" s="63">
@@ -9510,10 +10099,10 @@
     </row>
     <row r="18" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D18" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F18" s="57"/>
       <c r="G18" s="78">
@@ -9561,10 +10150,10 @@
         <v>0.87201284177197025</v>
       </c>
       <c r="Y18" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Z18" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AA18" s="57"/>
       <c r="AB18" s="63">
@@ -9629,7 +10218,7 @@
     <row r="19" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D19" s="56"/>
       <c r="E19" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F19" s="57"/>
       <c r="G19" s="78">
@@ -9678,7 +10267,7 @@
       </c>
       <c r="Y19" s="56"/>
       <c r="Z19" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AA19" s="57"/>
       <c r="AB19" s="63">
@@ -9743,7 +10332,7 @@
     <row r="20" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D20" s="56"/>
       <c r="E20" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F20" s="57"/>
       <c r="G20" s="78">
@@ -9792,7 +10381,7 @@
       </c>
       <c r="Y20" s="56"/>
       <c r="Z20" s="24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AA20" s="57"/>
       <c r="AB20" s="63">
@@ -9856,7 +10445,7 @@
     </row>
     <row r="21" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E21" s="57">
         <v>1</v>
@@ -9898,7 +10487,7 @@
         <v>0.06</v>
       </c>
       <c r="Y21" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Z21" s="57">
         <v>1</v>
@@ -10820,6 +11409,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AN7:AR7"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="BD6:BN6"/>
     <mergeCell ref="BA10:BB10"/>
     <mergeCell ref="BA11:BB11"/>
@@ -10833,11 +11427,6 @@
     <mergeCell ref="AB6:AR6"/>
     <mergeCell ref="AB7:AF7"/>
     <mergeCell ref="AH7:AL7"/>
-    <mergeCell ref="AN7:AR7"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Wrote code for comments march
</commit_message>
<xml_diff>
--- a/Programming_admin.xlsx
+++ b/Programming_admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimva\Documents\Studie\Thesis\Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF8F2FE-F30A-4761-846A-5DA7B18A5910}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B8F9FA-CCFB-4B55-9259-E7EBFF7BCC1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="12" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{0342F312-4DE5-442D-8282-6B7D8F998C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_and_prep" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Model_data_1" sheetId="2" r:id="rId3"/>
     <sheet name="Dataset_1" sheetId="5" r:id="rId4"/>
     <sheet name="Discussion_table" sheetId="15" r:id="rId5"/>
-    <sheet name="Text_table_sample_cons" sheetId="7" r:id="rId6"/>
-    <sheet name="Table_summary_stats" sheetId="8" r:id="rId7"/>
+    <sheet name="Table_summary_stats" sheetId="8" r:id="rId6"/>
+    <sheet name="Text_table_sample_cons" sheetId="7" r:id="rId7"/>
     <sheet name="Text_table_AUCs" sheetId="10" r:id="rId8"/>
     <sheet name="Tables_quantiles" sheetId="13" r:id="rId9"/>
     <sheet name="Unweighted results table" sheetId="11" r:id="rId10"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="386">
   <si>
     <t>Variable group</t>
   </si>
@@ -801,9 +801,6 @@
     <t xml:space="preserve">RAND HRS 2016 </t>
   </si>
   <si>
-    <t>No measure health or discrimination</t>
-  </si>
-  <si>
     <t>Missing moderator variables</t>
   </si>
   <si>
@@ -1210,6 +1207,18 @@
   </si>
   <si>
     <t>mStat, smoker, drinker, nnDrink, nGdrink</t>
+  </si>
+  <si>
+    <t>No answer on discrimination</t>
+  </si>
+  <si>
+    <t>No health measurements</t>
+  </si>
+  <si>
+    <t>No answer on discirmination</t>
+  </si>
+  <si>
+    <t>No health measurements 2016</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1446,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1530,6 +1539,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1538,12 +1548,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2891,7 +2901,7 @@
   <sheetData>
     <row r="1" spans="3:23" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="3:23" x14ac:dyDescent="0.25">
@@ -2902,45 +2912,45 @@
         <v>55</v>
       </c>
       <c r="K2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N2" t="s">
         <v>332</v>
-      </c>
-      <c r="N2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="3" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" t="s">
         <v>339</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>340</v>
       </c>
-      <c r="E3" t="s">
-        <v>341</v>
-      </c>
       <c r="F3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G3" t="s">
         <v>268</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>269</v>
       </c>
-      <c r="H3" t="s">
-        <v>270</v>
-      </c>
       <c r="I3" t="s">
+        <v>329</v>
+      </c>
+      <c r="J3" t="s">
         <v>330</v>
       </c>
-      <c r="J3" t="s">
-        <v>331</v>
-      </c>
       <c r="K3" t="s">
+        <v>333</v>
+      </c>
+      <c r="L3" t="s">
         <v>334</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>335</v>
-      </c>
-      <c r="M3" t="s">
-        <v>336</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -2978,7 +2988,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E4" s="36">
         <v>-0.18870000000000001</v>
@@ -2986,7 +2996,7 @@
     </row>
     <row r="5" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E5" s="36">
         <v>0.57339390000000001</v>
@@ -2994,7 +3004,7 @@
     </row>
     <row r="6" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E6" s="36">
         <v>-1.032214</v>
@@ -3002,7 +3012,7 @@
     </row>
     <row r="7" spans="3:23" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E7" s="36">
         <v>0.36380000000000001</v>
@@ -3013,7 +3023,7 @@
         <v>164</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E8" s="36">
         <v>4.1099999999999998E-2</v>
@@ -3021,7 +3031,7 @@
     </row>
     <row r="9" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D9" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E9" s="36">
         <v>0.49000709999999997</v>
@@ -3029,7 +3039,7 @@
     </row>
     <row r="10" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D10" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E10" s="36">
         <v>-0.440552</v>
@@ -3037,7 +3047,7 @@
     </row>
     <row r="11" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D11" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E11" s="36">
         <v>0.57040000000000002</v>
@@ -3048,7 +3058,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E12" s="36">
         <v>-1.9599999999999999E-2</v>
@@ -3056,7 +3066,7 @@
     </row>
     <row r="13" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D13" s="41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E13" s="36">
         <v>0.29692429999999997</v>
@@ -3064,7 +3074,7 @@
     </row>
     <row r="14" spans="3:23" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E14" s="36">
         <v>-0.3664499</v>
@@ -3072,7 +3082,7 @@
     </row>
     <row r="15" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D15" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E15" s="36">
         <v>0.47920000000000001</v>
@@ -3101,49 +3111,49 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="90" t="s">
-        <v>251</v>
-      </c>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="G3" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="90" t="s">
-        <v>256</v>
-      </c>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="90"/>
+      <c r="S3" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="91"/>
+      <c r="X3" s="91"/>
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="91"/>
+      <c r="AA3" s="91"/>
+      <c r="AB3" s="91"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
       <c r="G4" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I4" s="24">
         <v>3918</v>
       </c>
       <c r="L4" s="24"/>
       <c r="M4" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O4" s="24">
         <v>611</v>
@@ -3151,10 +3161,10 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="13"/>
       <c r="S4" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T4" s="41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U4" s="24">
         <v>23047018</v>
@@ -3163,10 +3173,10 @@
       <c r="W4" s="41"/>
       <c r="X4" s="24"/>
       <c r="Y4" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA4" s="24">
         <v>2359143</v>
@@ -3179,50 +3189,50 @@
     <row r="5" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F5" s="24"/>
       <c r="G5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="I5" s="31"/>
       <c r="K5" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L5" s="24"/>
       <c r="M5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="N5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="N5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="O5" s="31"/>
       <c r="R5" s="24"/>
       <c r="S5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="T5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="U5" s="40"/>
       <c r="V5" s="41"/>
       <c r="W5" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="Z5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="AA5" s="40"/>
       <c r="AB5" s="41"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="92" t="s">
-        <v>255</v>
-      </c>
-      <c r="E6" s="92"/>
+      <c r="D6" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" s="94"/>
       <c r="S6" s="41"/>
       <c r="T6" s="41"/>
       <c r="U6" s="41"/>
@@ -3235,10 +3245,10 @@
       <c r="AB6" s="41"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="94" t="s">
-        <v>317</v>
-      </c>
-      <c r="E7" s="94"/>
+      <c r="D7" s="96" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" s="96"/>
       <c r="G7">
         <v>127.98</v>
       </c>
@@ -3306,10 +3316,10 @@
       <c r="AB8" s="41"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="94"/>
+      <c r="E9" s="96"/>
       <c r="G9">
         <v>40.1</v>
       </c>
@@ -3355,7 +3365,7 @@
     </row>
     <row r="11" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D11" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S11" s="41"/>
       <c r="T11" s="36"/>
@@ -3446,48 +3456,48 @@
       <c r="AB15" s="41"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="92" t="s">
-        <v>313</v>
-      </c>
-      <c r="E16" s="92"/>
+      <c r="D16" s="94" t="s">
+        <v>312</v>
+      </c>
+      <c r="E16" s="94"/>
       <c r="G16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="I16" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>312</v>
-      </c>
       <c r="M16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="O16" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="N16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="O16" s="38" t="s">
-        <v>312</v>
-      </c>
       <c r="S16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="U16" s="40" t="s">
         <v>311</v>
-      </c>
-      <c r="T16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="U16" s="40" t="s">
-        <v>312</v>
       </c>
       <c r="V16" s="41"/>
       <c r="W16" s="41"/>
       <c r="X16" s="41"/>
       <c r="Y16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA16" s="38" t="s">
         <v>311</v>
-      </c>
-      <c r="Z16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="AA16" s="38" t="s">
-        <v>312</v>
       </c>
       <c r="AB16" s="41"/>
     </row>
@@ -3496,7 +3506,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G17">
         <f>H17*I4</f>
@@ -3506,7 +3516,7 @@
         <v>0.40300000000000002</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M17" s="39">
         <f>N17*O4</f>
@@ -3523,7 +3533,7 @@
         <v>0.43153160000000002</v>
       </c>
       <c r="U17" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V17" s="41"/>
       <c r="W17" s="41"/>
@@ -3540,10 +3550,10 @@
     </row>
     <row r="18" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D18" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>267</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>268</v>
       </c>
       <c r="G18">
         <v>3246</v>
@@ -3553,7 +3563,7 @@
         <v>0.82848392036753449</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M18">
         <v>187</v>
@@ -3570,7 +3580,7 @@
         <v>0.90943813208285773</v>
       </c>
       <c r="U18" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V18" s="41"/>
       <c r="W18" s="41"/>
@@ -3588,7 +3598,7 @@
     <row r="19" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D19" s="27"/>
       <c r="E19" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G19">
         <v>445</v>
@@ -3598,7 +3608,7 @@
         <v>0.11357835630423685</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M19">
         <v>323</v>
@@ -3615,7 +3625,7 @@
         <v>4.9359661193478482E-2</v>
       </c>
       <c r="U19" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V19" s="41"/>
       <c r="W19" s="41"/>
@@ -3633,7 +3643,7 @@
     <row r="20" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D20" s="27"/>
       <c r="E20" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G20">
         <v>227</v>
@@ -3643,7 +3653,7 @@
         <v>5.7937723328228691E-2</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M20">
         <v>101</v>
@@ -3660,7 +3670,7 @@
         <v>4.1202206723663773E-2</v>
       </c>
       <c r="U20" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V20" s="41"/>
       <c r="W20" s="41"/>
@@ -3677,7 +3687,7 @@
     </row>
     <row r="21" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -4255,49 +4265,49 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="G3" s="90" t="s">
-        <v>251</v>
-      </c>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
+      <c r="G3" s="91" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
       <c r="Q3" s="35"/>
-      <c r="S3" s="90" t="s">
-        <v>256</v>
-      </c>
-      <c r="T3" s="90"/>
-      <c r="U3" s="90"/>
-      <c r="V3" s="90"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="90"/>
+      <c r="S3" s="91" t="s">
+        <v>255</v>
+      </c>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="91"/>
+      <c r="X3" s="91"/>
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="91"/>
+      <c r="AA3" s="91"/>
+      <c r="AB3" s="91"/>
     </row>
     <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F4" s="13"/>
       <c r="G4" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I4" s="11">
         <v>3521</v>
       </c>
       <c r="L4" s="24"/>
       <c r="M4" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="N4" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O4" s="11">
         <v>536</v>
@@ -4305,20 +4315,20 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="13"/>
       <c r="S4" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T4" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U4" s="11">
         <v>20856866</v>
       </c>
       <c r="X4" s="24"/>
       <c r="Y4" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Z4" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AA4" s="11">
         <v>2088210</v>
@@ -4331,54 +4341,54 @@
     <row r="5" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F5" s="24"/>
       <c r="G5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="I5" s="50"/>
       <c r="K5" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L5" s="24"/>
       <c r="M5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="N5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="N5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="O5" s="50"/>
       <c r="R5" s="24"/>
       <c r="S5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="T5" s="33" t="s">
         <v>252</v>
-      </c>
-      <c r="T5" s="33" t="s">
-        <v>253</v>
       </c>
       <c r="U5" s="50"/>
       <c r="W5" s="34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X5" s="24"/>
       <c r="Y5" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z5" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="Z5" s="33" t="s">
-        <v>253</v>
-      </c>
       <c r="AA5" s="50"/>
     </row>
     <row r="6" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="92" t="s">
-        <v>344</v>
-      </c>
-      <c r="E6" s="92"/>
+      <c r="D6" s="94" t="s">
+        <v>343</v>
+      </c>
+      <c r="E6" s="94"/>
     </row>
     <row r="7" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D7" s="94" t="s">
-        <v>317</v>
-      </c>
-      <c r="E7" s="94"/>
+      <c r="D7" s="96" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" s="96"/>
       <c r="G7" s="70">
         <v>-0.13370000000000001</v>
       </c>
@@ -4462,10 +4472,10 @@
       <c r="AB8" s="58"/>
     </row>
     <row r="9" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="94"/>
+      <c r="E9" s="96"/>
       <c r="G9" s="70">
         <v>0.46750000000000003</v>
       </c>
@@ -4531,7 +4541,7 @@
     </row>
     <row r="11" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D11" s="51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -4618,45 +4628,45 @@
       <c r="U15" s="30"/>
     </row>
     <row r="16" spans="4:28" x14ac:dyDescent="0.25">
-      <c r="D16" s="92" t="s">
-        <v>313</v>
-      </c>
-      <c r="E16" s="92"/>
+      <c r="D16" s="94" t="s">
+        <v>312</v>
+      </c>
+      <c r="E16" s="94"/>
       <c r="G16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="I16" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="I16" s="50" t="s">
-        <v>312</v>
-      </c>
       <c r="M16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="O16" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="N16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="O16" s="38" t="s">
-        <v>312</v>
-      </c>
       <c r="S16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="U16" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="T16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="U16" s="50" t="s">
-        <v>312</v>
-      </c>
       <c r="Y16" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z16" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="AA16" s="38" t="s">
         <v>311</v>
-      </c>
-      <c r="Z16" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="AA16" s="38" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="17" spans="4:27" x14ac:dyDescent="0.25">
@@ -4664,7 +4674,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G17" s="64">
         <f>H17*I4</f>
@@ -4674,7 +4684,7 @@
         <v>0.4078</v>
       </c>
       <c r="I17" s="62" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J17" s="58"/>
       <c r="K17" s="58"/>
@@ -4698,7 +4708,7 @@
         <v>0.43648000599999998</v>
       </c>
       <c r="U17" s="62" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V17" s="58"/>
       <c r="W17" s="58"/>
@@ -4711,15 +4721,15 @@
         <v>0.48712987400000002</v>
       </c>
       <c r="AA17" s="62" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D18" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>267</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>268</v>
       </c>
       <c r="G18" s="11">
         <v>2939</v>
@@ -4729,7 +4739,7 @@
         <v>0.83470604941777904</v>
       </c>
       <c r="I18" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J18" s="58"/>
       <c r="K18" s="58"/>
@@ -4753,7 +4763,7 @@
         <v>0.91431531467862914</v>
       </c>
       <c r="U18" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V18" s="58"/>
       <c r="W18" s="58"/>
@@ -4766,13 +4776,13 @@
         <v>0.46681751356424883</v>
       </c>
       <c r="AA18" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D19" s="51"/>
       <c r="E19" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G19" s="11">
         <v>387</v>
@@ -4782,7 +4792,7 @@
         <v>0.1099119568304459</v>
       </c>
       <c r="I19" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J19" s="58"/>
       <c r="K19" s="58"/>
@@ -4806,7 +4816,7 @@
         <v>4.5933027521968067E-2</v>
       </c>
       <c r="U19" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V19" s="58"/>
       <c r="W19" s="58"/>
@@ -4819,13 +4829,13 @@
         <v>0.35627547037893698</v>
       </c>
       <c r="AA19" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D20" s="51"/>
       <c r="E20" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G20" s="11">
         <v>195</v>
@@ -4835,7 +4845,7 @@
         <v>5.5381993751775063E-2</v>
       </c>
       <c r="I20" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J20" s="58"/>
       <c r="K20" s="58"/>
@@ -4859,7 +4869,7 @@
         <v>3.9751657799402845E-2</v>
       </c>
       <c r="U20" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V20" s="58"/>
       <c r="W20" s="58"/>
@@ -4872,12 +4882,12 @@
         <v>0.1770363133975989</v>
       </c>
       <c r="AA20" s="63" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E21" s="52">
         <v>1</v>
@@ -5489,8 +5499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F80AE8-B842-48F2-9DD2-193B54D25AC7}">
   <dimension ref="C2:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6166,18 +6176,18 @@
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" t="s">
+        <v>355</v>
+      </c>
+      <c r="E6" t="s">
         <v>357</v>
-      </c>
-      <c r="D6" t="s">
-        <v>356</v>
-      </c>
-      <c r="E6" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
@@ -6188,7 +6198,7 @@
         <v>30121997</v>
       </c>
       <c r="E8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
@@ -6199,7 +6209,7 @@
         <v>13022021</v>
       </c>
       <c r="E9" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
@@ -6210,7 +6220,7 @@
         <v>14022021</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
@@ -6221,7 +6231,7 @@
         <v>15022021</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
@@ -6232,7 +6242,7 @@
         <v>16022021</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
@@ -6243,7 +6253,7 @@
         <v>17022021</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
@@ -6254,7 +6264,7 @@
         <v>18022021</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
@@ -6265,7 +6275,7 @@
         <v>19022021</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
@@ -6276,7 +6286,7 @@
         <v>20022021</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
@@ -6287,7 +6297,7 @@
         <v>21022021</v>
       </c>
       <c r="E17" s="72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
@@ -6298,7 +6308,7 @@
         <v>22022021</v>
       </c>
       <c r="E18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
@@ -6309,7 +6319,7 @@
         <v>23022021</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
@@ -6320,7 +6330,7 @@
         <v>24022021</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
@@ -6331,7 +6341,7 @@
         <v>25022021</v>
       </c>
       <c r="E21" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -6342,7 +6352,7 @@
         <v>26022021</v>
       </c>
       <c r="E22" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
@@ -6353,7 +6363,7 @@
         <v>27022021</v>
       </c>
       <c r="E23" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -6364,7 +6374,7 @@
         <v>28022021</v>
       </c>
       <c r="E24" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
@@ -6375,7 +6385,7 @@
         <v>29022021</v>
       </c>
       <c r="E25" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
@@ -6386,7 +6396,7 @@
         <v>30022021</v>
       </c>
       <c r="E26" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
@@ -6397,7 +6407,7 @@
         <v>31022021</v>
       </c>
       <c r="E27" s="72" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -7172,8 +7182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E776B9-4EC5-46CF-B1E5-E124814149F5}">
   <dimension ref="A2:K13"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I10" sqref="I9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7183,10 +7193,10 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>361</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -7194,22 +7204,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E4" t="s">
         <v>363</v>
       </c>
-      <c r="E4" t="s">
-        <v>364</v>
-      </c>
       <c r="I4" s="79" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J4" s="79" t="s">
+        <v>362</v>
+      </c>
+      <c r="K4" s="79" t="s">
         <v>363</v>
-      </c>
-      <c r="K4" s="79" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -7217,7 +7227,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C5">
         <v>9.61</v>
@@ -7232,7 +7242,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I5">
         <v>29.95</v>
@@ -7246,7 +7256,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C6">
         <v>8.7469999999999999</v>
@@ -7259,7 +7269,7 @@
       </c>
       <c r="G6" s="79"/>
       <c r="H6" s="79" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I6">
         <v>29.58</v>
@@ -7280,7 +7290,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C8">
         <v>9.6</v>
@@ -7295,7 +7305,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="79" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I8">
         <v>29.76</v>
@@ -7309,7 +7319,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C9">
         <v>9.6</v>
@@ -7322,7 +7332,7 @@
       </c>
       <c r="G9" s="79"/>
       <c r="H9" s="79" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I9">
         <v>29.12</v>
@@ -7336,7 +7346,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C10">
         <v>8.4</v>
@@ -7349,7 +7359,7 @@
       </c>
       <c r="G10" s="79"/>
       <c r="H10" s="79" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="I10">
         <v>27.84</v>
@@ -7370,7 +7380,7 @@
         <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C12">
         <v>8.83</v>
@@ -7385,7 +7395,7 @@
         <v>55</v>
       </c>
       <c r="H12" s="79" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I12">
         <v>37.93</v>
@@ -7399,7 +7409,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13">
         <v>10.1</v>
@@ -7412,7 +7422,7 @@
       </c>
       <c r="G13" s="79"/>
       <c r="H13" s="79" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I13">
         <v>23.05</v>
@@ -7431,794 +7441,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60364F5B-DCE9-46C6-A586-3092036B5563}">
-  <dimension ref="D4:P43"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="60.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="81" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="89" t="s">
-        <v>242</v>
-      </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="89" t="s">
-        <v>241</v>
-      </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-    </row>
-    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="F5" s="88" t="s">
-        <v>243</v>
-      </c>
-      <c r="G5" s="88"/>
-      <c r="H5" s="30"/>
-      <c r="J5" s="88" t="s">
-        <v>243</v>
-      </c>
-      <c r="K5" s="88"/>
-    </row>
-    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>239</v>
-      </c>
-      <c r="F6" t="s">
-        <v>240</v>
-      </c>
-      <c r="G6" t="s">
-        <v>244</v>
-      </c>
-      <c r="I6" t="s">
-        <v>239</v>
-      </c>
-      <c r="J6" t="s">
-        <v>240</v>
-      </c>
-      <c r="K6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7">
-        <f>Dataset_1!C3</f>
-        <v>20912</v>
-      </c>
-      <c r="F7">
-        <f>Dataset_1!D3</f>
-        <v>110313247</v>
-      </c>
-      <c r="G7" s="23">
-        <f>F7/$F$7</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="23"/>
-      <c r="I7">
-        <f>Dataset_2!C3</f>
-        <v>20912</v>
-      </c>
-      <c r="J7">
-        <f>Dataset_2!D3</f>
-        <v>110313247</v>
-      </c>
-      <c r="K7" s="23">
-        <f>J7/$J$7</f>
-        <v>1</v>
-      </c>
-      <c r="L7" s="23"/>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>246</v>
-      </c>
-      <c r="E8">
-        <f>Dataset_1!C5-Dataset_1!C3</f>
-        <v>-15400</v>
-      </c>
-      <c r="F8">
-        <f>Dataset_1!D5-Dataset_1!D3</f>
-        <v>-80303663</v>
-      </c>
-      <c r="G8" s="23">
-        <f t="shared" ref="G8:G12" si="0">F8/$F$7</f>
-        <v>-0.72796028748931663</v>
-      </c>
-      <c r="H8" s="23"/>
-      <c r="I8">
-        <f>Dataset_2!C5-Dataset_2!C3</f>
-        <v>-16715</v>
-      </c>
-      <c r="J8">
-        <f>Dataset_2!D5-Dataset_2!D3</f>
-        <v>-86931543</v>
-      </c>
-      <c r="K8" s="23">
-        <f t="shared" ref="K8:K12" si="1">J8/$J$7</f>
-        <v>-0.78804264550385317</v>
-      </c>
-      <c r="L8" s="23"/>
-    </row>
-    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9">
-        <f>Dataset_1!C6-Dataset_1!C5</f>
-        <v>-931</v>
-      </c>
-      <c r="F9">
-        <f>Dataset_1!D6-Dataset_1!D5</f>
-        <v>-4341801</v>
-      </c>
-      <c r="G9" s="23">
-        <f t="shared" si="0"/>
-        <v>-3.9358836024471294E-2</v>
-      </c>
-      <c r="H9" s="23"/>
-      <c r="I9">
-        <f>Dataset_2!C6-Dataset_2!C5</f>
-        <v>-94</v>
-      </c>
-      <c r="J9">
-        <f>Dataset_2!D6-Dataset_2!D5</f>
-        <v>-199299</v>
-      </c>
-      <c r="K9" s="23">
-        <f t="shared" si="1"/>
-        <v>-1.806664253115494E-3</v>
-      </c>
-      <c r="L9" s="23"/>
-    </row>
-    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>249</v>
-      </c>
-      <c r="E10">
-        <f>Dataset_1!C9-Dataset_1!C6</f>
-        <v>-33</v>
-      </c>
-      <c r="F10">
-        <f>Dataset_1!D9-Dataset_1!D6</f>
-        <v>-178500</v>
-      </c>
-      <c r="G10" s="23">
-        <f t="shared" si="0"/>
-        <v>-1.6181193542421973E-3</v>
-      </c>
-      <c r="H10" s="23"/>
-      <c r="I10">
-        <f>Dataset_2!C9-Dataset_2!C6</f>
-        <v>-30</v>
-      </c>
-      <c r="J10">
-        <f>Dataset_2!D9-Dataset_2!D6</f>
-        <v>-169538</v>
-      </c>
-      <c r="K10" s="23">
-        <f t="shared" si="1"/>
-        <v>-1.5368779780364908E-3</v>
-      </c>
-      <c r="L10" s="23"/>
-    </row>
-    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E11">
-        <f>Dataset_1!C11-Dataset_1!C9</f>
-        <v>-19</v>
-      </c>
-      <c r="F11">
-        <f>Dataset_1!D11-Dataset_1!D9</f>
-        <v>-94366</v>
-      </c>
-      <c r="G11" s="23">
-        <f t="shared" si="0"/>
-        <v>-8.5543670018162004E-4</v>
-      </c>
-      <c r="H11" s="23"/>
-      <c r="I11">
-        <f>Dataset_2!C11-Dataset_2!C9</f>
-        <v>-14</v>
-      </c>
-      <c r="J11">
-        <f>Dataset_2!D11-Dataset_2!D9</f>
-        <v>-67521</v>
-      </c>
-      <c r="K11" s="23">
-        <f t="shared" si="1"/>
-        <v>-6.1208424043578374E-4</v>
-      </c>
-      <c r="L11" s="23"/>
-    </row>
-    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>250</v>
-      </c>
-      <c r="E12">
-        <f>SUM(E7:E11)</f>
-        <v>4529</v>
-      </c>
-      <c r="F12">
-        <f>SUM(F7:F11)</f>
-        <v>25394917</v>
-      </c>
-      <c r="G12" s="23">
-        <f t="shared" si="0"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12">
-        <f>SUM(I7:I11)</f>
-        <v>4059</v>
-      </c>
-      <c r="J12">
-        <f>SUM(J7:J11)</f>
-        <v>22945346</v>
-      </c>
-      <c r="K12" s="23">
-        <f t="shared" si="1"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="L12" s="23"/>
-    </row>
-    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="M14" s="83"/>
-    </row>
-    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="M15" s="83"/>
-    </row>
-    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>368</v>
-      </c>
-      <c r="M16" s="83"/>
-    </row>
-    <row r="17" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E17" s="89" t="s">
-        <v>242</v>
-      </c>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="M17" s="83"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="88" t="s">
-        <v>243</v>
-      </c>
-      <c r="G18" s="88"/>
-      <c r="H18" s="87" t="s">
-        <v>374</v>
-      </c>
-      <c r="I18" s="87" t="s">
-        <v>371</v>
-      </c>
-      <c r="J18" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="K18" s="88"/>
-      <c r="M18" s="83"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D19" s="81"/>
-      <c r="E19" s="81" t="s">
-        <v>239</v>
-      </c>
-      <c r="F19" s="81" t="s">
-        <v>240</v>
-      </c>
-      <c r="G19" s="81" t="s">
-        <v>244</v>
-      </c>
-      <c r="I19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="83"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D20" s="81" t="s">
-        <v>369</v>
-      </c>
-      <c r="E20" s="81">
-        <v>20912</v>
-      </c>
-      <c r="F20" s="81">
-        <v>110313247</v>
-      </c>
-      <c r="G20" s="23">
-        <f>F20/$F$7</f>
-        <v>1</v>
-      </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="84"/>
-    </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D21" s="81" t="s">
-        <v>202</v>
-      </c>
-      <c r="E21" s="81">
-        <v>5551</v>
-      </c>
-      <c r="F21" s="81">
-        <v>30222610</v>
-      </c>
-      <c r="G21" s="23">
-        <f t="shared" ref="G21:G30" si="2">F21/$F$7</f>
-        <v>0.27397081331492307</v>
-      </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81" t="s">
-        <v>380</v>
-      </c>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="85"/>
-    </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D22" s="81" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="81">
-        <v>5512</v>
-      </c>
-      <c r="F22" s="81">
-        <v>30009584</v>
-      </c>
-      <c r="G22" s="23">
-        <f t="shared" si="2"/>
-        <v>0.27203971251068332</v>
-      </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81" t="s">
-        <v>379</v>
-      </c>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="86"/>
-    </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D23" s="81" t="s">
-        <v>206</v>
-      </c>
-      <c r="E23" s="81">
-        <v>4581</v>
-      </c>
-      <c r="F23" s="81">
-        <v>25667783</v>
-      </c>
-      <c r="G23" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23268087648621202</v>
-      </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="81" t="s">
-        <v>372</v>
-      </c>
-      <c r="J23" s="81" t="s">
-        <v>381</v>
-      </c>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="86"/>
-    </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D24" s="81" t="s">
-        <v>217</v>
-      </c>
-      <c r="E24" s="81">
-        <v>4581</v>
-      </c>
-      <c r="F24" s="81">
-        <v>25667783</v>
-      </c>
-      <c r="G24" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23268087648621202</v>
-      </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="81" t="s">
-        <v>373</v>
-      </c>
-      <c r="J24" s="81" t="s">
-        <v>219</v>
-      </c>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
-      <c r="M24" s="85"/>
-    </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D25" s="81" t="s">
-        <v>218</v>
-      </c>
-      <c r="E25" s="81">
-        <v>4581</v>
-      </c>
-      <c r="F25" s="81">
-        <v>25667783</v>
-      </c>
-      <c r="G25" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23268087648621202</v>
-      </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="85"/>
-    </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D26" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="E26" s="81">
-        <v>4548</v>
-      </c>
-      <c r="F26" s="81">
-        <v>25489283</v>
-      </c>
-      <c r="G26" s="23">
-        <f>F26/$F$7</f>
-        <v>0.23106275713196983</v>
-      </c>
-      <c r="H26" s="23"/>
-      <c r="J26" t="s">
-        <v>377</v>
-      </c>
-      <c r="K26" s="81"/>
-      <c r="L26" s="81"/>
-      <c r="M26" s="85"/>
-    </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D27" s="81" t="s">
-        <v>223</v>
-      </c>
-      <c r="E27" s="81">
-        <v>4548</v>
-      </c>
-      <c r="F27" s="81">
-        <v>25489283</v>
-      </c>
-      <c r="G27" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23106275713196983</v>
-      </c>
-      <c r="H27" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="J27" s="81"/>
-      <c r="K27" s="81"/>
-      <c r="L27" s="81"/>
-      <c r="M27" s="85"/>
-    </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D28" s="81" t="s">
-        <v>221</v>
-      </c>
-      <c r="E28" s="81">
-        <v>4529</v>
-      </c>
-      <c r="F28" s="81">
-        <v>25394917</v>
-      </c>
-      <c r="G28" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="H28" s="23"/>
-      <c r="J28" s="81" t="s">
-        <v>378</v>
-      </c>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="85"/>
-    </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D29" s="81" t="s">
-        <v>233</v>
-      </c>
-      <c r="E29" s="81">
-        <v>4529</v>
-      </c>
-      <c r="F29" s="81">
-        <v>25394917</v>
-      </c>
-      <c r="G29" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="H29" s="23" t="s">
-        <v>376</v>
-      </c>
-      <c r="J29" s="81" t="s">
-        <v>236</v>
-      </c>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="85"/>
-    </row>
-    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D30" s="81" t="s">
-        <v>234</v>
-      </c>
-      <c r="E30" s="81">
-        <v>4529</v>
-      </c>
-      <c r="F30" s="81">
-        <v>25394917</v>
-      </c>
-      <c r="G30" s="23">
-        <f t="shared" si="2"/>
-        <v>0.23020732043178821</v>
-      </c>
-      <c r="H30" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="J30" s="81" t="s">
-        <v>235</v>
-      </c>
-      <c r="M30" s="83"/>
-    </row>
-    <row r="31" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="81"/>
-      <c r="H31" s="80"/>
-      <c r="I31" s="89"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="M31" s="83"/>
-    </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="E32" s="82"/>
-      <c r="F32" s="88" t="s">
-        <v>243</v>
-      </c>
-      <c r="G32" s="88"/>
-      <c r="H32" s="87" t="s">
-        <v>374</v>
-      </c>
-      <c r="I32" s="87" t="s">
-        <v>371</v>
-      </c>
-      <c r="J32" s="88" t="s">
-        <v>370</v>
-      </c>
-      <c r="K32" s="88"/>
-      <c r="M32" s="83"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="82" t="s">
-        <v>201</v>
-      </c>
-      <c r="E33" s="82">
-        <v>20912</v>
-      </c>
-      <c r="F33" s="82">
-        <v>110313247</v>
-      </c>
-      <c r="G33" s="23">
-        <f>F33/$F$33</f>
-        <v>1</v>
-      </c>
-      <c r="I33" s="82"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D34" s="82" t="s">
-        <v>209</v>
-      </c>
-      <c r="E34" s="82">
-        <v>5551</v>
-      </c>
-      <c r="F34" s="82">
-        <v>30222610</v>
-      </c>
-      <c r="G34" s="23">
-        <f t="shared" ref="G34:G43" si="3">F34/$F$33</f>
-        <v>0.27397081331492307</v>
-      </c>
-      <c r="I34" s="82"/>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D35" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="E35" s="82">
-        <f>E34+I35</f>
-        <v>5551</v>
-      </c>
-      <c r="F35" s="82">
-        <v>23381704</v>
-      </c>
-      <c r="G35" s="23">
-        <f t="shared" si="3"/>
-        <v>0.21195735449614678</v>
-      </c>
-      <c r="I35" s="82"/>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D36" s="82" t="s">
-        <v>206</v>
-      </c>
-      <c r="E36" s="82">
-        <v>4103</v>
-      </c>
-      <c r="F36" s="82">
-        <v>23182405</v>
-      </c>
-      <c r="G36" s="23">
-        <f t="shared" si="3"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="I36" s="82"/>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="82" t="s">
-        <v>217</v>
-      </c>
-      <c r="E37" s="82">
-        <v>4103</v>
-      </c>
-      <c r="F37" s="82">
-        <v>23182405</v>
-      </c>
-      <c r="G37" s="23">
-        <f t="shared" si="3"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="I37" s="82"/>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="82" t="s">
-        <v>218</v>
-      </c>
-      <c r="E38" s="82">
-        <v>4103</v>
-      </c>
-      <c r="F38" s="82">
-        <v>23182405</v>
-      </c>
-      <c r="G38" s="23">
-        <f t="shared" si="3"/>
-        <v>0.21015069024303129</v>
-      </c>
-      <c r="I38" s="82"/>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="E39" s="82">
-        <v>4073</v>
-      </c>
-      <c r="F39" s="82">
-        <v>23012867</v>
-      </c>
-      <c r="G39" s="23">
-        <f t="shared" si="3"/>
-        <v>0.20861381226499479</v>
-      </c>
-      <c r="I39" s="82"/>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="82" t="s">
-        <v>223</v>
-      </c>
-      <c r="E40" s="82">
-        <v>4073</v>
-      </c>
-      <c r="F40" s="82">
-        <v>22945346</v>
-      </c>
-      <c r="G40" s="23">
-        <f t="shared" si="3"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="H40" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="I40" s="82"/>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D41" s="82" t="s">
-        <v>221</v>
-      </c>
-      <c r="E41" s="82">
-        <v>4059</v>
-      </c>
-      <c r="F41" s="82">
-        <v>22945346</v>
-      </c>
-      <c r="G41" s="23">
-        <f t="shared" si="3"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="I41" s="82"/>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="82" t="s">
-        <v>233</v>
-      </c>
-      <c r="E42" s="82">
-        <v>4059</v>
-      </c>
-      <c r="F42" s="82">
-        <v>22945346</v>
-      </c>
-      <c r="G42" s="23">
-        <f t="shared" si="3"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="H42" s="23" t="s">
-        <v>376</v>
-      </c>
-      <c r="I42" s="82"/>
-    </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D43" s="82" t="s">
-        <v>234</v>
-      </c>
-      <c r="E43" s="82">
-        <v>4059</v>
-      </c>
-      <c r="F43" s="82">
-        <v>22945346</v>
-      </c>
-      <c r="G43" s="23">
-        <f t="shared" si="3"/>
-        <v>0.20800172802455902</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>375</v>
-      </c>
-      <c r="I43" s="82"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="I31:K31"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="G12" formula="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FBAE27-4D7B-4D03-B5B4-DAD9C59D9C9D}">
   <dimension ref="B1:Z60"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:Z2"/>
     </sheetView>
   </sheetViews>
@@ -8252,38 +7478,38 @@
   <sheetData>
     <row r="1" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B1" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
       <c r="J1" s="24"/>
       <c r="K1" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
       <c r="N1" s="24"/>
       <c r="O1" s="24"/>
       <c r="P1" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
       <c r="S1" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
       <c r="V1" s="24"/>
       <c r="W1" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="X1" s="24"/>
       <c r="Y1" s="24"/>
@@ -8291,74 +7517,74 @@
     </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>252</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="F2" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>254</v>
-      </c>
       <c r="G2" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="J2" s="33" t="s">
         <v>253</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>254</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="N2" s="33" t="s">
         <v>253</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>254</v>
       </c>
       <c r="O2" s="24"/>
       <c r="P2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q2" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="R2" s="33" t="s">
         <v>253</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>254</v>
       </c>
       <c r="S2" s="24"/>
       <c r="T2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="U2" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="U2" s="33" t="s">
+      <c r="V2" s="33" t="s">
         <v>253</v>
-      </c>
-      <c r="V2" s="33" t="s">
-        <v>254</v>
       </c>
       <c r="W2" s="24"/>
       <c r="X2" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y2" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="Y2" s="33" t="s">
+      <c r="Z2" s="33" t="s">
         <v>253</v>
-      </c>
-      <c r="Z2" s="33" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28"/>
@@ -8371,7 +7597,7 @@
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -8387,19 +7613,19 @@
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="27"/>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C10" s="27"/>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C11" s="27"/>
     </row>
@@ -8408,32 +7634,32 @@
         <v>55</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>267</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -8443,60 +7669,60 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" t="s">
         <v>275</v>
-      </c>
-      <c r="C21" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -8506,130 +7732,130 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C40" t="s">
         <v>294</v>
-      </c>
-      <c r="C40" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="24"/>
       <c r="C41" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="24"/>
       <c r="C42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="24"/>
       <c r="C43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="24"/>
       <c r="C45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
       <c r="C46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
       <c r="C47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C48" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="24"/>
       <c r="C49" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="24"/>
       <c r="C50" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="24"/>
       <c r="C51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
@@ -8639,45 +7865,902 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60364F5B-DCE9-46C6-A586-3092036B5563}">
+  <dimension ref="D4:P46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="81" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="90" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="90" t="s">
+        <v>241</v>
+      </c>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+    </row>
+    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="F5" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="G5" s="89"/>
+      <c r="H5" s="30"/>
+      <c r="J5" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="K5" s="89"/>
+    </row>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" t="s">
+        <v>244</v>
+      </c>
+      <c r="I6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J6" t="s">
+        <v>240</v>
+      </c>
+      <c r="K6" t="s">
+        <v>244</v>
+      </c>
+      <c r="N6" s="88"/>
+    </row>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7">
+        <f>Dataset_1!C3</f>
+        <v>20912</v>
+      </c>
+      <c r="F7">
+        <f>Dataset_1!D3</f>
+        <v>110313247</v>
+      </c>
+      <c r="G7" s="23">
+        <f>F7/$F$7</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7">
+        <f>Dataset_2!C3</f>
+        <v>20912</v>
+      </c>
+      <c r="J7">
+        <f>Dataset_2!D3</f>
+        <v>110313247</v>
+      </c>
+      <c r="K7" s="23">
+        <f>J7/$J$7</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="N7" s="88"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E8">
+        <f>6282-E7</f>
+        <v>-14630</v>
+      </c>
+      <c r="F8">
+        <v>-76395979</v>
+      </c>
+      <c r="G8" s="23">
+        <f>F8/$F$7</f>
+        <v>-0.69253676305983447</v>
+      </c>
+      <c r="H8" s="23"/>
+      <c r="I8">
+        <v>-14630</v>
+      </c>
+      <c r="J8">
+        <v>-80090637</v>
+      </c>
+      <c r="K8" s="23">
+        <f t="shared" ref="K8:K13" si="0">J8/$J$7</f>
+        <v>-0.72602918668507688</v>
+      </c>
+      <c r="L8" s="23"/>
+      <c r="N8" s="88"/>
+    </row>
+    <row r="9" spans="4:16" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="88" t="s">
+        <v>383</v>
+      </c>
+      <c r="E9">
+        <v>-770</v>
+      </c>
+      <c r="F9">
+        <v>-3907684</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" ref="G9:G13" si="1">F9/$F$7</f>
+        <v>-3.5423524429482163E-2</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="88">
+        <v>-2085</v>
+      </c>
+      <c r="J9" s="88">
+        <v>-6840906</v>
+      </c>
+      <c r="K9" s="23">
+        <f t="shared" si="0"/>
+        <v>-6.2013458818776318E-2</v>
+      </c>
+      <c r="L9" s="23"/>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10">
+        <f>Dataset_1!C6-Dataset_1!C5</f>
+        <v>-931</v>
+      </c>
+      <c r="F10">
+        <f>Dataset_1!D6-Dataset_1!D5</f>
+        <v>-4341801</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="1"/>
+        <v>-3.9358836024471294E-2</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10">
+        <f>Dataset_2!C6-Dataset_2!C5</f>
+        <v>-94</v>
+      </c>
+      <c r="J10">
+        <f>Dataset_2!D6-Dataset_2!D5</f>
+        <v>-199299</v>
+      </c>
+      <c r="K10" s="23">
+        <f t="shared" si="0"/>
+        <v>-1.806664253115494E-3</v>
+      </c>
+      <c r="L10" s="23"/>
+      <c r="N10" s="88"/>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E11">
+        <f>Dataset_1!C9-Dataset_1!C6</f>
+        <v>-33</v>
+      </c>
+      <c r="F11">
+        <f>Dataset_1!D9-Dataset_1!D6</f>
+        <v>-178500</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="1"/>
+        <v>-1.6181193542421973E-3</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11">
+        <f>Dataset_2!C9-Dataset_2!C6</f>
+        <v>-30</v>
+      </c>
+      <c r="J11">
+        <f>Dataset_2!D9-Dataset_2!D6</f>
+        <v>-169538</v>
+      </c>
+      <c r="K11" s="23">
+        <f t="shared" si="0"/>
+        <v>-1.5368779780364908E-3</v>
+      </c>
+      <c r="L11" s="23"/>
+      <c r="N11" s="88"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12">
+        <f>Dataset_1!C11-Dataset_1!C9</f>
+        <v>-19</v>
+      </c>
+      <c r="F12">
+        <f>Dataset_1!D11-Dataset_1!D9</f>
+        <v>-94366</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="1"/>
+        <v>-8.5543670018162004E-4</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12">
+        <f>Dataset_2!C11-Dataset_2!C9</f>
+        <v>-14</v>
+      </c>
+      <c r="J12">
+        <f>Dataset_2!D11-Dataset_2!D9</f>
+        <v>-67521</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="0"/>
+        <v>-6.1208424043578374E-4</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="N12" s="88"/>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13">
+        <f>SUM(E7:E12)</f>
+        <v>4529</v>
+      </c>
+      <c r="F13">
+        <f>SUM(F7:F12)</f>
+        <v>25394917</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="1"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13">
+        <f>SUM(I7:I12)</f>
+        <v>4059</v>
+      </c>
+      <c r="J13">
+        <f>SUM(J7:J12)</f>
+        <v>22945346</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="0"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="L13" s="23"/>
+      <c r="N13" s="88"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N14" s="88"/>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M15" s="83"/>
+      <c r="N15" s="88"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M16" s="83"/>
+      <c r="N16" s="88"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>367</v>
+      </c>
+      <c r="M17" s="83"/>
+      <c r="N17" s="88"/>
+    </row>
+    <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="90" t="s">
+        <v>242</v>
+      </c>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="M18" s="83"/>
+      <c r="N18" s="88"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="G19" s="89"/>
+      <c r="H19" s="87" t="s">
+        <v>373</v>
+      </c>
+      <c r="I19" s="87" t="s">
+        <v>370</v>
+      </c>
+      <c r="J19" s="89" t="s">
+        <v>369</v>
+      </c>
+      <c r="K19" s="89"/>
+      <c r="M19" s="83"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D20" s="81"/>
+      <c r="E20" s="81" t="s">
+        <v>239</v>
+      </c>
+      <c r="F20" s="81" t="s">
+        <v>240</v>
+      </c>
+      <c r="G20" s="81" t="s">
+        <v>244</v>
+      </c>
+      <c r="I20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="83"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="81" t="s">
+        <v>368</v>
+      </c>
+      <c r="E21" s="81">
+        <v>20912</v>
+      </c>
+      <c r="F21" s="81">
+        <v>110313247</v>
+      </c>
+      <c r="G21" s="23">
+        <f>F21/$F$21</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="84"/>
+    </row>
+    <row r="22" spans="4:14" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="88" t="s">
+        <v>382</v>
+      </c>
+      <c r="E22" s="88">
+        <v>6282</v>
+      </c>
+      <c r="F22" s="88">
+        <v>33917268</v>
+      </c>
+      <c r="G22" s="23">
+        <f t="shared" ref="G22:G32" si="2">F22/$F$21</f>
+        <v>0.30746323694016547</v>
+      </c>
+      <c r="H22" s="23"/>
+      <c r="M22" s="84"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D23" s="81" t="s">
+        <v>385</v>
+      </c>
+      <c r="E23" s="81">
+        <v>5551</v>
+      </c>
+      <c r="F23" s="81">
+        <v>30222610</v>
+      </c>
+      <c r="G23" s="23">
+        <f t="shared" si="2"/>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="H23" s="23"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="81" t="s">
+        <v>379</v>
+      </c>
+      <c r="K23" s="81"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="85"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D24" s="81" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="81">
+        <v>5512</v>
+      </c>
+      <c r="F24" s="81">
+        <v>30009584</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="2"/>
+        <v>0.27203971251068332</v>
+      </c>
+      <c r="H24" s="23"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81" t="s">
+        <v>378</v>
+      </c>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="86"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D25" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="81">
+        <v>4581</v>
+      </c>
+      <c r="F25" s="81">
+        <v>25667783</v>
+      </c>
+      <c r="G25" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="H25" s="23"/>
+      <c r="I25" s="81" t="s">
+        <v>371</v>
+      </c>
+      <c r="J25" s="81" t="s">
+        <v>380</v>
+      </c>
+      <c r="K25" s="81"/>
+      <c r="L25" s="81"/>
+      <c r="M25" s="86"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D26" s="81" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="81">
+        <v>4581</v>
+      </c>
+      <c r="F26" s="81">
+        <v>25667783</v>
+      </c>
+      <c r="G26" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="H26" s="23"/>
+      <c r="I26" s="81" t="s">
+        <v>372</v>
+      </c>
+      <c r="J26" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="K26" s="81"/>
+      <c r="L26" s="81"/>
+      <c r="M26" s="85"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D27" s="81" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" s="81">
+        <v>4581</v>
+      </c>
+      <c r="F27" s="81">
+        <v>25667783</v>
+      </c>
+      <c r="G27" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23268087648621202</v>
+      </c>
+      <c r="H27" s="23"/>
+      <c r="I27" s="81"/>
+      <c r="K27" s="81"/>
+      <c r="L27" s="81"/>
+      <c r="M27" s="85"/>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D28" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E28" s="81">
+        <v>4548</v>
+      </c>
+      <c r="F28" s="81">
+        <v>25489283</v>
+      </c>
+      <c r="G28" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="H28" s="23"/>
+      <c r="J28" t="s">
+        <v>376</v>
+      </c>
+      <c r="K28" s="81"/>
+      <c r="L28" s="81"/>
+      <c r="M28" s="85"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D29" s="81" t="s">
+        <v>223</v>
+      </c>
+      <c r="E29" s="81">
+        <v>4548</v>
+      </c>
+      <c r="F29" s="81">
+        <v>25489283</v>
+      </c>
+      <c r="G29" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23106275713196983</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="85"/>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D30" s="81" t="s">
+        <v>221</v>
+      </c>
+      <c r="E30" s="81">
+        <v>4529</v>
+      </c>
+      <c r="F30" s="81">
+        <v>25394917</v>
+      </c>
+      <c r="G30" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="J30" s="81" t="s">
+        <v>377</v>
+      </c>
+      <c r="K30" s="81"/>
+      <c r="L30" s="81"/>
+      <c r="M30" s="85"/>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D31" s="81" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="81">
+        <v>4529</v>
+      </c>
+      <c r="F31" s="81">
+        <v>25394917</v>
+      </c>
+      <c r="G31" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="J31" s="81" t="s">
+        <v>236</v>
+      </c>
+      <c r="K31" s="81"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="85"/>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D32" s="81" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" s="81">
+        <v>4529</v>
+      </c>
+      <c r="F32" s="81">
+        <v>25394917</v>
+      </c>
+      <c r="G32" s="23">
+        <f t="shared" si="2"/>
+        <v>0.23020732043178821</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="J32" s="81" t="s">
+        <v>235</v>
+      </c>
+      <c r="M32" s="83"/>
+    </row>
+    <row r="33" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="81"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="M33" s="83"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="82"/>
+      <c r="F34" s="89" t="s">
+        <v>243</v>
+      </c>
+      <c r="G34" s="89"/>
+      <c r="H34" s="87" t="s">
+        <v>373</v>
+      </c>
+      <c r="I34" s="87" t="s">
+        <v>370</v>
+      </c>
+      <c r="J34" s="89" t="s">
+        <v>369</v>
+      </c>
+      <c r="K34" s="89"/>
+      <c r="M34" s="83"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D35" s="82" t="s">
+        <v>201</v>
+      </c>
+      <c r="E35" s="82">
+        <v>20912</v>
+      </c>
+      <c r="F35" s="82">
+        <v>110313247</v>
+      </c>
+      <c r="G35" s="23">
+        <f>F35/$F$35</f>
+        <v>1</v>
+      </c>
+      <c r="I35" s="82"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D36" s="82" t="s">
+        <v>382</v>
+      </c>
+      <c r="E36" s="88">
+        <v>6282</v>
+      </c>
+      <c r="F36" s="82">
+        <v>30222610</v>
+      </c>
+      <c r="G36" s="23">
+        <f t="shared" ref="G36:G46" si="3">F36/$F$35</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="I36" s="82"/>
+    </row>
+    <row r="37" spans="4:13" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="88" t="s">
+        <v>385</v>
+      </c>
+      <c r="E37" s="88">
+        <v>5551</v>
+      </c>
+      <c r="F37" s="88">
+        <v>30222610</v>
+      </c>
+      <c r="G37" s="23">
+        <f>F37/$F$35</f>
+        <v>0.27397081331492307</v>
+      </c>
+      <c r="H37" s="23"/>
+      <c r="J37" s="88" t="s">
+        <v>379</v>
+      </c>
+      <c r="M37" s="85"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D38" s="82" t="s">
+        <v>210</v>
+      </c>
+      <c r="E38" s="82">
+        <f>Dataset_2!C5</f>
+        <v>4197</v>
+      </c>
+      <c r="F38" s="82">
+        <v>23381704</v>
+      </c>
+      <c r="G38" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21195735449614678</v>
+      </c>
+      <c r="I38" s="82"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D39" s="82" t="s">
+        <v>206</v>
+      </c>
+      <c r="E39" s="82">
+        <v>4103</v>
+      </c>
+      <c r="F39" s="82">
+        <v>23182405</v>
+      </c>
+      <c r="G39" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="I39" s="82"/>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D40" s="82" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" s="82">
+        <v>4103</v>
+      </c>
+      <c r="F40" s="82">
+        <v>23182405</v>
+      </c>
+      <c r="G40" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="I40" s="82"/>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D41" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="E41" s="82">
+        <v>4103</v>
+      </c>
+      <c r="F41" s="82">
+        <v>23182405</v>
+      </c>
+      <c r="G41" s="23">
+        <f t="shared" si="3"/>
+        <v>0.21015069024303129</v>
+      </c>
+      <c r="I41" s="82"/>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D42" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E42" s="82">
+        <v>4073</v>
+      </c>
+      <c r="F42" s="82">
+        <v>23012867</v>
+      </c>
+      <c r="G42" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20861381226499479</v>
+      </c>
+      <c r="I42" s="82"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D43" s="82" t="s">
+        <v>223</v>
+      </c>
+      <c r="E43" s="82">
+        <v>4073</v>
+      </c>
+      <c r="F43" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G43" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="I43" s="82"/>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D44" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="E44" s="82">
+        <v>4059</v>
+      </c>
+      <c r="F44" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G44" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="I44" s="82"/>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D45" s="82" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="82">
+        <v>4059</v>
+      </c>
+      <c r="F45" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G45" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="I45" s="82"/>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D46" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="E46" s="82">
+        <v>4059</v>
+      </c>
+      <c r="F46" s="82">
+        <v>22945346</v>
+      </c>
+      <c r="G46" s="23">
+        <f t="shared" si="3"/>
+        <v>0.20800172802455902</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="I46" s="82"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="I33:K33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8694,94 +8777,94 @@
   <sheetData>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C2" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="E2" s="91" t="s">
+        <v>341</v>
+      </c>
+      <c r="E2" s="92" t="s">
         <v>242</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="M2" s="91" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="M2" s="92" t="s">
         <v>241</v>
       </c>
-      <c r="N2" s="91"/>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
-      <c r="S2" s="91"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="I3" s="91" t="s">
         <v>325</v>
       </c>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="I3" s="90" t="s">
-        <v>326</v>
-      </c>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="M3" s="90" t="s">
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="M3" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="91" t="s">
         <v>325</v>
       </c>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="90" t="s">
-        <v>326</v>
-      </c>
-      <c r="R3" s="90"/>
-      <c r="S3" s="90"/>
+      <c r="R3" s="91"/>
+      <c r="S3" s="91"/>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E4" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="G4" s="31" t="s">
         <v>322</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>323</v>
       </c>
       <c r="H4" s="31"/>
       <c r="I4" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="J4" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="K4" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="M4" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="O4" s="44" t="s">
         <v>322</v>
-      </c>
-      <c r="K4" s="42" t="s">
-        <v>324</v>
-      </c>
-      <c r="M4" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="N4" s="44" t="s">
-        <v>322</v>
-      </c>
-      <c r="O4" s="44" t="s">
-        <v>323</v>
       </c>
       <c r="P4" s="44"/>
       <c r="Q4" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="R4" s="44" t="s">
         <v>321</v>
       </c>
-      <c r="R4" s="44" t="s">
-        <v>322</v>
-      </c>
       <c r="S4" s="42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E5" s="43">
         <v>0.82180149999999996</v>
@@ -8824,7 +8907,7 @@
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E6" s="43">
         <v>0.8236696</v>
@@ -8867,7 +8950,7 @@
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E7" s="43">
         <v>0.82320090000000001</v>
@@ -8914,104 +8997,104 @@
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="E10" s="43"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E11" s="91" t="s">
+      <c r="E11" s="92" t="s">
         <v>242</v>
       </c>
-      <c r="F11" s="91"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
       <c r="L11" s="49"/>
-      <c r="M11" s="91" t="s">
+      <c r="M11" s="92" t="s">
         <v>241</v>
       </c>
-      <c r="N11" s="91"/>
-      <c r="O11" s="91"/>
-      <c r="P11" s="91"/>
-      <c r="Q11" s="91"/>
-      <c r="R11" s="91"/>
-      <c r="S11" s="91"/>
+      <c r="N11" s="92"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="92"/>
+      <c r="Q11" s="92"/>
+      <c r="R11" s="92"/>
+      <c r="S11" s="92"/>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D12" s="49"/>
-      <c r="E12" s="90" t="s">
+      <c r="E12" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="F12" s="91"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="91" t="s">
         <v>325</v>
       </c>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="90" t="s">
-        <v>326</v>
-      </c>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="90" t="s">
+      <c r="M12" s="91" t="s">
+        <v>324</v>
+      </c>
+      <c r="N12" s="91"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="91" t="s">
         <v>325</v>
       </c>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="49"/>
-      <c r="Q12" s="90" t="s">
-        <v>326</v>
-      </c>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
+      <c r="R12" s="91"/>
+      <c r="S12" s="91"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D13" s="49"/>
       <c r="E13" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="F13" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="G13" s="48" t="s">
         <v>322</v>
-      </c>
-      <c r="G13" s="48" t="s">
-        <v>323</v>
       </c>
       <c r="H13" s="48"/>
       <c r="I13" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="J13" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="J13" s="48" t="s">
-        <v>322</v>
-      </c>
       <c r="K13" s="42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L13" s="49"/>
       <c r="M13" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="N13" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="N13" s="48" t="s">
+      <c r="O13" s="48" t="s">
         <v>322</v>
-      </c>
-      <c r="O13" s="48" t="s">
-        <v>323</v>
       </c>
       <c r="P13" s="48"/>
       <c r="Q13" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="R13" s="48" t="s">
         <v>321</v>
       </c>
-      <c r="R13" s="48" t="s">
-        <v>322</v>
-      </c>
       <c r="S13" s="42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D14" s="49" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E14" s="43">
         <v>0.84530419999999995</v>
@@ -9055,7 +9138,7 @@
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D15" s="49" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E15" s="53">
         <v>0.84761169999999997</v>
@@ -9099,7 +9182,7 @@
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D16" s="49" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E16" s="43">
         <v>0.84655320000000001</v>
@@ -9143,18 +9226,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="M2:S2"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="Q12:S12"/>
     <mergeCell ref="E11:K11"/>
     <mergeCell ref="M11:S11"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="M2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -9197,109 +9280,109 @@
       <c r="D6" s="57"/>
       <c r="E6" s="57"/>
       <c r="F6" s="57"/>
-      <c r="G6" s="90" t="s">
-        <v>350</v>
-      </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="90"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
+      <c r="G6" s="91" t="s">
+        <v>349</v>
+      </c>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="91"/>
+      <c r="U6" s="91"/>
+      <c r="V6" s="91"/>
+      <c r="W6" s="91"/>
       <c r="Y6" s="57"/>
       <c r="Z6" s="57"/>
       <c r="AA6" s="57"/>
-      <c r="AB6" s="90" t="s">
-        <v>353</v>
-      </c>
-      <c r="AC6" s="90"/>
-      <c r="AD6" s="90"/>
-      <c r="AE6" s="90"/>
-      <c r="AF6" s="90"/>
-      <c r="AG6" s="90"/>
-      <c r="AH6" s="90"/>
-      <c r="AI6" s="90"/>
-      <c r="AJ6" s="90"/>
-      <c r="AK6" s="90"/>
-      <c r="AL6" s="90"/>
-      <c r="AM6" s="90"/>
-      <c r="AN6" s="90"/>
-      <c r="AO6" s="90"/>
-      <c r="AP6" s="90"/>
-      <c r="AQ6" s="90"/>
-      <c r="AR6" s="90"/>
+      <c r="AB6" s="91" t="s">
+        <v>352</v>
+      </c>
+      <c r="AC6" s="91"/>
+      <c r="AD6" s="91"/>
+      <c r="AE6" s="91"/>
+      <c r="AF6" s="91"/>
+      <c r="AG6" s="91"/>
+      <c r="AH6" s="91"/>
+      <c r="AI6" s="91"/>
+      <c r="AJ6" s="91"/>
+      <c r="AK6" s="91"/>
+      <c r="AL6" s="91"/>
+      <c r="AM6" s="91"/>
+      <c r="AN6" s="91"/>
+      <c r="AO6" s="91"/>
+      <c r="AP6" s="91"/>
+      <c r="AQ6" s="91"/>
+      <c r="AR6" s="91"/>
       <c r="BA6" s="57"/>
       <c r="BB6" s="57"/>
       <c r="BC6" s="57"/>
-      <c r="BD6" s="90"/>
-      <c r="BE6" s="90"/>
-      <c r="BF6" s="90"/>
-      <c r="BG6" s="90"/>
-      <c r="BH6" s="90"/>
-      <c r="BI6" s="90"/>
-      <c r="BJ6" s="90"/>
-      <c r="BK6" s="90"/>
-      <c r="BL6" s="90"/>
-      <c r="BM6" s="90"/>
-      <c r="BN6" s="90"/>
+      <c r="BD6" s="91"/>
+      <c r="BE6" s="91"/>
+      <c r="BF6" s="91"/>
+      <c r="BG6" s="91"/>
+      <c r="BH6" s="91"/>
+      <c r="BI6" s="91"/>
+      <c r="BJ6" s="91"/>
+      <c r="BK6" s="91"/>
+      <c r="BL6" s="91"/>
+      <c r="BM6" s="91"/>
+      <c r="BN6" s="91"/>
     </row>
     <row r="7" spans="4:66" s="57" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G7" s="95" t="s">
-        <v>262</v>
-      </c>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
+      <c r="G7" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
       <c r="L7" s="35"/>
-      <c r="M7" s="95" t="s">
+      <c r="M7" s="93" t="s">
         <v>164</v>
       </c>
-      <c r="N7" s="95"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
+      <c r="N7" s="93"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
       <c r="R7" s="35"/>
-      <c r="S7" s="95" t="s">
+      <c r="S7" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="95"/>
-      <c r="U7" s="95"/>
-      <c r="V7" s="95"/>
-      <c r="W7" s="95"/>
-      <c r="AB7" s="95" t="s">
-        <v>262</v>
-      </c>
-      <c r="AC7" s="95"/>
-      <c r="AD7" s="95"/>
-      <c r="AE7" s="95"/>
-      <c r="AF7" s="95"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="93"/>
+      <c r="V7" s="93"/>
+      <c r="W7" s="93"/>
+      <c r="AB7" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC7" s="93"/>
+      <c r="AD7" s="93"/>
+      <c r="AE7" s="93"/>
+      <c r="AF7" s="93"/>
       <c r="AG7" s="35"/>
-      <c r="AH7" s="95" t="s">
+      <c r="AH7" s="93" t="s">
         <v>164</v>
       </c>
-      <c r="AI7" s="95"/>
-      <c r="AJ7" s="95"/>
-      <c r="AK7" s="95"/>
-      <c r="AL7" s="95"/>
+      <c r="AI7" s="93"/>
+      <c r="AJ7" s="93"/>
+      <c r="AK7" s="93"/>
+      <c r="AL7" s="93"/>
       <c r="AM7" s="35"/>
-      <c r="AN7" s="95" t="s">
+      <c r="AN7" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="AO7" s="95"/>
-      <c r="AP7" s="95"/>
-      <c r="AQ7" s="95"/>
-      <c r="AR7" s="95"/>
+      <c r="AO7" s="93"/>
+      <c r="AP7" s="93"/>
+      <c r="AQ7" s="93"/>
+      <c r="AR7" s="93"/>
       <c r="BD7" s="35"/>
       <c r="BE7" s="35"/>
       <c r="BF7" s="35"/>
@@ -9317,77 +9400,77 @@
       <c r="E8" s="57"/>
       <c r="F8" s="13"/>
       <c r="G8" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H8" s="57"/>
       <c r="I8" s="24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J8" s="57"/>
       <c r="K8" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="73" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N8" s="73"/>
       <c r="O8" s="73" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P8" s="73"/>
       <c r="Q8" s="73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="R8" s="24"/>
       <c r="S8" s="73" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="T8" s="28"/>
       <c r="U8" s="73" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="V8" s="28"/>
       <c r="W8" s="73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Y8" s="57"/>
       <c r="Z8" s="57"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC8" s="57"/>
       <c r="AD8" s="24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AE8" s="57"/>
       <c r="AF8" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AG8" s="32"/>
       <c r="AH8" s="73" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AI8" s="73"/>
       <c r="AJ8" s="73" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AK8" s="73"/>
       <c r="AL8" s="73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AM8" s="24"/>
       <c r="AN8" s="73" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AO8" s="28"/>
       <c r="AP8" s="73" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AQ8" s="28"/>
       <c r="AR8" s="73" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="BA8" s="57"/>
       <c r="BB8" s="57"/>
@@ -9409,77 +9492,77 @@
       <c r="E9" s="57"/>
       <c r="F9" s="24"/>
       <c r="G9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H9" s="55"/>
       <c r="I9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J9" s="55"/>
       <c r="K9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L9" s="55"/>
       <c r="M9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N9" s="33"/>
       <c r="O9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P9" s="33"/>
       <c r="Q9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R9" s="33"/>
       <c r="S9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T9" s="55"/>
       <c r="U9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="V9" s="55"/>
       <c r="W9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y9" s="57"/>
       <c r="Z9" s="57"/>
       <c r="AA9" s="24"/>
       <c r="AB9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AC9" s="55"/>
       <c r="AD9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AE9" s="55"/>
       <c r="AF9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AG9" s="55"/>
       <c r="AH9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AI9" s="33"/>
       <c r="AJ9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AK9" s="33"/>
       <c r="AL9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AM9" s="33"/>
       <c r="AN9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AO9" s="55"/>
       <c r="AP9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="AQ9" s="55"/>
       <c r="AR9" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BA9" s="57"/>
       <c r="BB9" s="57"/>
@@ -9497,10 +9580,10 @@
       <c r="BN9" s="55"/>
     </row>
     <row r="10" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D10" s="92" t="s">
-        <v>352</v>
-      </c>
-      <c r="E10" s="93"/>
+      <c r="D10" s="94" t="s">
+        <v>351</v>
+      </c>
+      <c r="E10" s="95"/>
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10" s="57"/>
@@ -9515,10 +9598,10 @@
       <c r="U10" s="57"/>
       <c r="V10" s="57"/>
       <c r="W10" s="57"/>
-      <c r="Y10" s="92" t="s">
-        <v>352</v>
-      </c>
-      <c r="Z10" s="93"/>
+      <c r="Y10" s="94" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z10" s="95"/>
       <c r="AA10" s="57"/>
       <c r="AB10" s="57"/>
       <c r="AC10" s="57"/>
@@ -9537,8 +9620,8 @@
       <c r="AP10" s="57"/>
       <c r="AQ10" s="57"/>
       <c r="AR10" s="57"/>
-      <c r="BA10" s="92"/>
-      <c r="BB10" s="92"/>
+      <c r="BA10" s="94"/>
+      <c r="BB10" s="94"/>
       <c r="BC10" s="57"/>
       <c r="BD10" s="57"/>
       <c r="BE10" s="57"/>
@@ -9553,10 +9636,10 @@
       <c r="BN10" s="57"/>
     </row>
     <row r="11" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D11" s="94" t="s">
-        <v>351</v>
-      </c>
-      <c r="E11" s="94"/>
+      <c r="D11" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="E11" s="96"/>
       <c r="F11" s="57"/>
       <c r="G11" s="11">
         <v>0.27</v>
@@ -9592,10 +9675,10 @@
       <c r="W11" s="11">
         <v>-0.63</v>
       </c>
-      <c r="Y11" s="94" t="s">
-        <v>351</v>
-      </c>
-      <c r="Z11" s="94"/>
+      <c r="Y11" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z11" s="96"/>
       <c r="AA11" s="57"/>
       <c r="AB11" s="11">
         <v>1.51</v>
@@ -9632,8 +9715,8 @@
       <c r="AR11" s="11">
         <v>-0.5</v>
       </c>
-      <c r="BA11" s="94"/>
-      <c r="BB11" s="94"/>
+      <c r="BA11" s="96"/>
+      <c r="BB11" s="96"/>
       <c r="BC11" s="57"/>
       <c r="BD11" s="11"/>
       <c r="BE11" s="65"/>
@@ -9693,7 +9776,7 @@
     </row>
     <row r="13" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D13" s="56" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E13" s="57"/>
       <c r="F13" s="57"/>
@@ -9714,7 +9797,7 @@
       <c r="V13" s="58"/>
       <c r="W13" s="58"/>
       <c r="Y13" s="56" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Z13" s="57"/>
       <c r="AA13" s="57"/>
@@ -9902,88 +9985,88 @@
       <c r="BN15" s="57"/>
     </row>
     <row r="16" spans="4:66" x14ac:dyDescent="0.25">
-      <c r="D16" s="92" t="s">
-        <v>346</v>
-      </c>
-      <c r="E16" s="92"/>
+      <c r="D16" s="94" t="s">
+        <v>345</v>
+      </c>
+      <c r="E16" s="94"/>
       <c r="F16" s="57"/>
       <c r="G16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H16" s="55"/>
       <c r="I16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J16" s="55"/>
       <c r="K16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L16" s="33"/>
       <c r="M16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N16" s="77"/>
       <c r="O16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="P16" s="77"/>
       <c r="Q16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R16" s="33"/>
       <c r="S16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="T16" s="55"/>
       <c r="U16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="V16" s="55"/>
       <c r="W16" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="Y16" s="92" t="s">
-        <v>346</v>
-      </c>
-      <c r="Z16" s="92"/>
+        <v>353</v>
+      </c>
+      <c r="Y16" s="94" t="s">
+        <v>345</v>
+      </c>
+      <c r="Z16" s="94"/>
       <c r="AA16" s="57"/>
       <c r="AB16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AC16" s="55"/>
       <c r="AD16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AE16" s="55"/>
       <c r="AF16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AG16" s="33"/>
       <c r="AH16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AI16" s="33"/>
       <c r="AJ16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AK16" s="33"/>
       <c r="AL16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AM16" s="33"/>
       <c r="AN16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AO16" s="55"/>
       <c r="AP16" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AQ16" s="55"/>
       <c r="AR16" s="33" t="s">
-        <v>354</v>
-      </c>
-      <c r="BA16" s="92"/>
-      <c r="BB16" s="92"/>
+        <v>353</v>
+      </c>
+      <c r="BA16" s="94"/>
+      <c r="BB16" s="94"/>
       <c r="BC16" s="57"/>
       <c r="BD16" s="33"/>
       <c r="BE16" s="33"/>
@@ -10002,7 +10085,7 @@
         <v>55</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F17" s="57"/>
       <c r="G17" s="78">
@@ -10044,7 +10127,7 @@
         <v>55</v>
       </c>
       <c r="Z17" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AA17" s="57"/>
       <c r="AB17" s="63">
@@ -10099,10 +10182,10 @@
     </row>
     <row r="18" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D18" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="24" t="s">
         <v>267</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>268</v>
       </c>
       <c r="F18" s="57"/>
       <c r="G18" s="78">
@@ -10150,10 +10233,10 @@
         <v>0.87201284177197025</v>
       </c>
       <c r="Y18" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z18" s="24" t="s">
         <v>267</v>
-      </c>
-      <c r="Z18" s="24" t="s">
-        <v>268</v>
       </c>
       <c r="AA18" s="57"/>
       <c r="AB18" s="63">
@@ -10218,7 +10301,7 @@
     <row r="19" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D19" s="56"/>
       <c r="E19" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F19" s="57"/>
       <c r="G19" s="78">
@@ -10267,7 +10350,7 @@
       </c>
       <c r="Y19" s="56"/>
       <c r="Z19" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA19" s="57"/>
       <c r="AB19" s="63">
@@ -10332,7 +10415,7 @@
     <row r="20" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D20" s="56"/>
       <c r="E20" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F20" s="57"/>
       <c r="G20" s="78">
@@ -10381,7 +10464,7 @@
       </c>
       <c r="Y20" s="56"/>
       <c r="Z20" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AA20" s="57"/>
       <c r="AB20" s="63">
@@ -10445,7 +10528,7 @@
     </row>
     <row r="21" spans="4:66" x14ac:dyDescent="0.25">
       <c r="D21" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E21" s="57">
         <v>1</v>
@@ -10487,7 +10570,7 @@
         <v>0.06</v>
       </c>
       <c r="Y21" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Z21" s="57">
         <v>1</v>
@@ -11409,11 +11492,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AN7:AR7"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D16:E16"/>
     <mergeCell ref="BD6:BN6"/>
     <mergeCell ref="BA10:BB10"/>
     <mergeCell ref="BA11:BB11"/>
@@ -11427,6 +11505,11 @@
     <mergeCell ref="AB6:AR6"/>
     <mergeCell ref="AB7:AF7"/>
     <mergeCell ref="AH7:AL7"/>
+    <mergeCell ref="AN7:AR7"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>